<commit_message>
Added all entry fields
</commit_message>
<xml_diff>
--- a/SO_Test.xlsx
+++ b/SO_Test.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="10">
   <si>
     <t>REF NUM</t>
   </si>
@@ -35,6 +35,12 @@
   </si>
   <si>
     <t>PRICE</t>
+  </si>
+  <si>
+    <t>VENDER</t>
+  </si>
+  <si>
+    <t>TYPE</t>
   </si>
   <si>
     <t>CLERK NAME</t>
@@ -384,7 +390,7 @@
   <sheetPr>
     <outlinePr summaryBelow="0"/>
   </sheetPr>
-  <dimension ref="A1:H1"/>
+  <dimension ref="A1:J1"/>
   <sheetViews>
     <sheetView workbookViewId="0" tabSelected="1"/>
   </sheetViews>
@@ -397,7 +403,9 @@
     <col min="5" max="5" style="2" width="13.576428571428572" customWidth="1" bestFit="1"/>
     <col min="6" max="6" style="2" width="13.576428571428572" customWidth="1" bestFit="1"/>
     <col min="7" max="7" style="2" width="13.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="8" max="8" style="2" width="19.433571428571426" customWidth="1" bestFit="1"/>
+    <col min="8" max="8" style="2" width="13.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="9" max="9" style="2" width="13.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="10" max="10" style="2" width="19.433571428571426" customWidth="1" bestFit="1"/>
   </cols>
   <sheetData>
     <row x14ac:dyDescent="0.25" r="1" customHeight="1" ht="18.75">
@@ -425,6 +433,12 @@
       <c r="H1" s="1" t="s">
         <v>7</v>
       </c>
+      <c r="I1" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="J1" s="1" t="s">
+        <v>9</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Modifications - SO_Test.xlsx     1. Added a column to store the current date - main.py     1. Added today's date to the data list - generators.py     1. Added a new function to count the number of     entries for the current day in order to generate     the reference value accordingly
</commit_message>
<xml_diff>
--- a/SO_Test.xlsx
+++ b/SO_Test.xlsx
@@ -14,7 +14,10 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="11">
+  <si>
+    <t>DATE</t>
+  </si>
   <si>
     <t>REF NUM</t>
   </si>
@@ -390,22 +393,23 @@
   <sheetPr>
     <outlinePr summaryBelow="0"/>
   </sheetPr>
-  <dimension ref="A1:J1"/>
+  <dimension ref="A1:K1"/>
   <sheetViews>
     <sheetView workbookViewId="0" tabSelected="1"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" style="2" width="16.290714285714284" customWidth="1" bestFit="1"/>
-    <col min="2" max="2" style="2" width="14.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="3" max="3" style="2" width="13.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="1" max="1" style="2" width="13.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="2" max="2" style="2" width="16.290714285714284" customWidth="1" bestFit="1"/>
+    <col min="3" max="3" style="2" width="14.576428571428572" customWidth="1" bestFit="1"/>
     <col min="4" max="4" style="2" width="13.576428571428572" customWidth="1" bestFit="1"/>
     <col min="5" max="5" style="2" width="13.576428571428572" customWidth="1" bestFit="1"/>
     <col min="6" max="6" style="2" width="13.576428571428572" customWidth="1" bestFit="1"/>
     <col min="7" max="7" style="2" width="13.576428571428572" customWidth="1" bestFit="1"/>
     <col min="8" max="8" style="2" width="13.576428571428572" customWidth="1" bestFit="1"/>
     <col min="9" max="9" style="2" width="13.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="10" max="10" style="2" width="19.433571428571426" customWidth="1" bestFit="1"/>
+    <col min="10" max="10" style="2" width="13.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="11" max="11" style="2" width="19.433571428571426" customWidth="1" bestFit="1"/>
   </cols>
   <sheetData>
     <row x14ac:dyDescent="0.25" r="1" customHeight="1" ht="18.75">
@@ -439,6 +443,9 @@
       <c r="J1" s="1" t="s">
         <v>9</v>
       </c>
+      <c r="K1" s="1" t="s">
+        <v>10</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Modifications - main.py     1. Modified the check_proper_info function to work     with space seperation of full name input - SO_Test.xlsx     1. Saving the testing data in order to test functionality     of the get_todays_entries_count() function in generators.py         ~ Will be doing further testing tomorrow
</commit_message>
<xml_diff>
--- a/SO_Test.xlsx
+++ b/SO_Test.xlsx
@@ -1,71 +1,33 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion rupBuild="9303" lowestEdited="5" lastEdited="5" appName="xl"/>
+<workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
   <bookViews>
-    <workbookView xWindow="480" yWindow="60" windowWidth="18195" windowHeight="8505" activeTab="0"/>
+    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" xWindow="480" yWindow="60" windowWidth="18195" windowHeight="8505" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
-    <sheet r:id="rId1" sheetId="1" name="Sheet1"/>
+    <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId1"/>
   </sheets>
-  <calcPr fullCalcOnLoad="1"/>
+  <definedNames/>
+  <calcPr calcId="124519" fullCalcOnLoad="1"/>
 </workbook>
 </file>
 
-<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="11">
-  <si>
-    <t>DATE</t>
-  </si>
-  <si>
-    <t>REF NUM</t>
-  </si>
-  <si>
-    <t>CX NAME</t>
-  </si>
-  <si>
-    <t>PHONE</t>
-  </si>
-  <si>
-    <t>ARTIST</t>
-  </si>
-  <si>
-    <t>TITLE</t>
-  </si>
-  <si>
-    <t>DEPOSIT</t>
-  </si>
-  <si>
-    <t>PRICE</t>
-  </si>
-  <si>
-    <t>VENDOR</t>
-  </si>
-  <si>
-    <t>TYPE</t>
-  </si>
-  <si>
-    <t>CLERK NAME</t>
-  </si>
-</sst>
-</file>
-
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="0"/>
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="1">
     <font>
-      <sz val="11"/>
-      <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
+      <color theme="1"/>
+      <sz val="11"/>
       <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="2">
     <fill>
-      <patternFill patternType="none"/>
+      <patternFill/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
@@ -84,24 +46,86 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
   <cellXfs count="3">
-    <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0"/>
-    <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="general"/>
     </xf>
-    <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="general"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle xfId="0" builtinId="0" name="Normal"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
-  <extLst>
-    <ext uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
-      <x14ac:slicerStyles xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" defaultSlicerStyle="SlicerStyleLight1"/>
-    </ext>
-  </extLst>
+  <colors>
+    <indexedColors>
+      <rgbColor rgb="00000000"/>
+      <rgbColor rgb="00FFFFFF"/>
+      <rgbColor rgb="00FF0000"/>
+      <rgbColor rgb="0000FF00"/>
+      <rgbColor rgb="000000FF"/>
+      <rgbColor rgb="00FFFF00"/>
+      <rgbColor rgb="00FF00FF"/>
+      <rgbColor rgb="0000FFFF"/>
+      <rgbColor rgb="00000000"/>
+      <rgbColor rgb="00FFFFFF"/>
+      <rgbColor rgb="00FF0000"/>
+      <rgbColor rgb="0000FF00"/>
+      <rgbColor rgb="000000FF"/>
+      <rgbColor rgb="00FFFF00"/>
+      <rgbColor rgb="00FF00FF"/>
+      <rgbColor rgb="0000FFFF"/>
+      <rgbColor rgb="00800000"/>
+      <rgbColor rgb="00008000"/>
+      <rgbColor rgb="00000080"/>
+      <rgbColor rgb="00808000"/>
+      <rgbColor rgb="00800080"/>
+      <rgbColor rgb="00008080"/>
+      <rgbColor rgb="00C0C0C0"/>
+      <rgbColor rgb="00808080"/>
+      <rgbColor rgb="009999FF"/>
+      <rgbColor rgb="00993366"/>
+      <rgbColor rgb="00FFFFCC"/>
+      <rgbColor rgb="00CCFFFF"/>
+      <rgbColor rgb="00660066"/>
+      <rgbColor rgb="00FF8080"/>
+      <rgbColor rgb="000066CC"/>
+      <rgbColor rgb="00CCCCFF"/>
+      <rgbColor rgb="00000080"/>
+      <rgbColor rgb="00FF00FF"/>
+      <rgbColor rgb="00FFFF00"/>
+      <rgbColor rgb="0000FFFF"/>
+      <rgbColor rgb="00800080"/>
+      <rgbColor rgb="00800000"/>
+      <rgbColor rgb="00008080"/>
+      <rgbColor rgb="000000FF"/>
+      <rgbColor rgb="0000CCFF"/>
+      <rgbColor rgb="00CCFFFF"/>
+      <rgbColor rgb="00CCFFCC"/>
+      <rgbColor rgb="00FFFF99"/>
+      <rgbColor rgb="0099CCFF"/>
+      <rgbColor rgb="00FF99CC"/>
+      <rgbColor rgb="00CC99FF"/>
+      <rgbColor rgb="00FFCC99"/>
+      <rgbColor rgb="003366FF"/>
+      <rgbColor rgb="0033CCCC"/>
+      <rgbColor rgb="0099CC00"/>
+      <rgbColor rgb="00FFCC00"/>
+      <rgbColor rgb="00FF9900"/>
+      <rgbColor rgb="00FF6600"/>
+      <rgbColor rgb="00666699"/>
+      <rgbColor rgb="00969696"/>
+      <rgbColor rgb="00003366"/>
+      <rgbColor rgb="00339966"/>
+      <rgbColor rgb="00003300"/>
+      <rgbColor rgb="00333300"/>
+      <rgbColor rgb="00993300"/>
+      <rgbColor rgb="00993366"/>
+      <rgbColor rgb="00333399"/>
+      <rgbColor rgb="00333333"/>
+    </indexedColors>
+  </colors>
 </styleSheet>
 </file>
 
@@ -389,62 +413,193 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <sheetPr>
     <outlinePr summaryBelow="0"/>
+    <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:K1"/>
+  <dimension ref="A1:K3"/>
   <sheetViews>
-    <sheetView workbookViewId="0" tabSelected="1"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" style="2" width="13.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="2" max="2" style="2" width="16.290714285714284" customWidth="1" bestFit="1"/>
-    <col min="3" max="3" style="2" width="14.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="4" max="4" style="2" width="13.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="5" max="5" style="2" width="13.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="6" max="6" style="2" width="13.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="7" max="7" style="2" width="13.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="8" max="8" style="2" width="13.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="9" max="9" style="2" width="13.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="10" max="10" style="2" width="13.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="11" max="11" style="2" width="19.433571428571426" customWidth="1" bestFit="1"/>
+    <col width="13.57642857142857" bestFit="1" customWidth="1" style="2" min="1" max="1"/>
+    <col width="16.29071428571428" bestFit="1" customWidth="1" style="2" min="2" max="2"/>
+    <col width="14.57642857142857" bestFit="1" customWidth="1" style="2" min="3" max="3"/>
+    <col width="13.57642857142857" bestFit="1" customWidth="1" style="2" min="4" max="4"/>
+    <col width="13.57642857142857" bestFit="1" customWidth="1" style="2" min="5" max="5"/>
+    <col width="13.57642857142857" bestFit="1" customWidth="1" style="2" min="6" max="6"/>
+    <col width="13.57642857142857" bestFit="1" customWidth="1" style="2" min="7" max="7"/>
+    <col width="13.57642857142857" bestFit="1" customWidth="1" style="2" min="8" max="8"/>
+    <col width="13.57642857142857" bestFit="1" customWidth="1" style="2" min="9" max="9"/>
+    <col width="13.57642857142857" bestFit="1" customWidth="1" style="2" min="10" max="10"/>
+    <col width="19.43357142857143" bestFit="1" customWidth="1" style="2" min="11" max="11"/>
   </cols>
   <sheetData>
-    <row x14ac:dyDescent="0.25" r="1" customHeight="1" ht="18.75">
-      <c r="A1" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="F1" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="G1" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="H1" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="I1" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="J1" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="K1" s="1" t="s">
-        <v>10</v>
+    <row r="1" ht="18.75" customHeight="1">
+      <c r="A1" s="2" t="inlineStr">
+        <is>
+          <t>DATE</t>
+        </is>
+      </c>
+      <c r="B1" s="2" t="inlineStr">
+        <is>
+          <t>REF NUM</t>
+        </is>
+      </c>
+      <c r="C1" s="2" t="inlineStr">
+        <is>
+          <t>CX NAME</t>
+        </is>
+      </c>
+      <c r="D1" s="2" t="inlineStr">
+        <is>
+          <t>PHONE</t>
+        </is>
+      </c>
+      <c r="E1" s="2" t="inlineStr">
+        <is>
+          <t>ARTIST</t>
+        </is>
+      </c>
+      <c r="F1" s="2" t="inlineStr">
+        <is>
+          <t>TITLE</t>
+        </is>
+      </c>
+      <c r="G1" s="2" t="inlineStr">
+        <is>
+          <t>DEPOSIT</t>
+        </is>
+      </c>
+      <c r="H1" s="2" t="inlineStr">
+        <is>
+          <t>PRICE</t>
+        </is>
+      </c>
+      <c r="I1" s="2" t="inlineStr">
+        <is>
+          <t>VENDOR</t>
+        </is>
+      </c>
+      <c r="J1" s="2" t="inlineStr">
+        <is>
+          <t>TYPE</t>
+        </is>
+      </c>
+      <c r="K1" s="2" t="inlineStr">
+        <is>
+          <t>CLERK NAME</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="inlineStr">
+        <is>
+          <t>01/10/2024</t>
+        </is>
+      </c>
+      <c r="B2" t="inlineStr">
+        <is>
+          <t>SO240110001</t>
+        </is>
+      </c>
+      <c r="C2" t="inlineStr">
+        <is>
+          <t>AshleyBaker</t>
+        </is>
+      </c>
+      <c r="D2" t="inlineStr">
+        <is>
+          <t>9157994875</t>
+        </is>
+      </c>
+      <c r="E2" t="inlineStr">
+        <is>
+          <t>Tool</t>
+        </is>
+      </c>
+      <c r="F2" t="inlineStr">
+        <is>
+          <t>Aenima</t>
+        </is>
+      </c>
+      <c r="G2" t="n">
+        <v>50</v>
+      </c>
+      <c r="H2" t="n">
+        <v>90.98999999999999</v>
+      </c>
+      <c r="I2" t="inlineStr">
+        <is>
+          <t>AEC</t>
+        </is>
+      </c>
+      <c r="J2" t="inlineStr">
+        <is>
+          <t>DVD</t>
+        </is>
+      </c>
+      <c r="K2" t="inlineStr">
+        <is>
+          <t>Ashley</t>
+        </is>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="inlineStr">
+        <is>
+          <t>01/10/2024</t>
+        </is>
+      </c>
+      <c r="B3" t="inlineStr">
+        <is>
+          <t>SO240110002</t>
+        </is>
+      </c>
+      <c r="C3" t="inlineStr">
+        <is>
+          <t>Ashley Baker</t>
+        </is>
+      </c>
+      <c r="D3" t="inlineStr">
+        <is>
+          <t>9157994875</t>
+        </is>
+      </c>
+      <c r="E3" t="inlineStr">
+        <is>
+          <t>SOAD</t>
+        </is>
+      </c>
+      <c r="F3" t="inlineStr">
+        <is>
+          <t>Hypnotize</t>
+        </is>
+      </c>
+      <c r="G3" t="n">
+        <v>50</v>
+      </c>
+      <c r="H3" t="n">
+        <v>125</v>
+      </c>
+      <c r="I3" t="inlineStr">
+        <is>
+          <t>AMS</t>
+        </is>
+      </c>
+      <c r="J3" t="inlineStr">
+        <is>
+          <t>LP</t>
+        </is>
+      </c>
+      <c r="K3" t="inlineStr">
+        <is>
+          <t>Ashley</t>
+        </is>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Modification to generators.py now there will be an empty row insertted to the excel file to seperate the orders done the previous day from the orders that will be appended to the excel file on the current day.
</commit_message>
<xml_diff>
--- a/SO_Test.xlsx
+++ b/SO_Test.xlsx
@@ -418,13 +418,13 @@
     <outlinePr summaryBelow="0"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:K3"/>
+  <dimension ref="A1:K5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15" outlineLevelCol="0"/>
   <cols>
     <col width="13.57642857142857" bestFit="1" customWidth="1" style="2" min="1" max="1"/>
     <col width="16.29071428571428" bestFit="1" customWidth="1" style="2" min="2" max="2"/>
@@ -602,6 +602,59 @@
         </is>
       </c>
     </row>
+    <row r="5">
+      <c r="A5" t="inlineStr">
+        <is>
+          <t>01/11/2024</t>
+        </is>
+      </c>
+      <c r="B5" t="inlineStr">
+        <is>
+          <t>SO240111001</t>
+        </is>
+      </c>
+      <c r="C5" t="inlineStr">
+        <is>
+          <t>Ashley Baker</t>
+        </is>
+      </c>
+      <c r="D5" t="inlineStr">
+        <is>
+          <t>9157994875</t>
+        </is>
+      </c>
+      <c r="E5" t="inlineStr">
+        <is>
+          <t>Smashing Pumpkins</t>
+        </is>
+      </c>
+      <c r="F5" t="inlineStr">
+        <is>
+          <t>Siamese Dream</t>
+        </is>
+      </c>
+      <c r="G5" t="n">
+        <v>55</v>
+      </c>
+      <c r="H5" t="n">
+        <v>120.99</v>
+      </c>
+      <c r="I5" t="inlineStr">
+        <is>
+          <t>AEC</t>
+        </is>
+      </c>
+      <c r="J5" t="inlineStr">
+        <is>
+          <t>DVD</t>
+        </is>
+      </c>
+      <c r="K5" t="inlineStr">
+        <is>
+          <t>Ashley</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Working on 2 things 1. The 'PHONE' feild is showing the phone number as a float when it should be displayed as a string 2. When creating/saving a new SO, the frame to show the previous SO's is not updating.
</commit_message>
<xml_diff>
--- a/SO_Test.xlsx
+++ b/SO_Test.xlsx
@@ -418,13 +418,13 @@
     <outlinePr summaryBelow="0"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:K5"/>
+  <dimension ref="A1:K7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15" outlineLevelCol="0"/>
   <cols>
     <col width="13.57642857142857" bestFit="1" customWidth="1" style="2" min="1" max="1"/>
     <col width="16.29071428571428" bestFit="1" customWidth="1" style="2" min="2" max="2"/>
@@ -656,6 +656,59 @@
         </is>
       </c>
     </row>
+    <row r="7">
+      <c r="A7" t="inlineStr">
+        <is>
+          <t>01/12/2024</t>
+        </is>
+      </c>
+      <c r="B7" t="inlineStr">
+        <is>
+          <t>SO240112001</t>
+        </is>
+      </c>
+      <c r="C7" t="inlineStr">
+        <is>
+          <t>Ashley Baker</t>
+        </is>
+      </c>
+      <c r="D7" t="inlineStr">
+        <is>
+          <t>9157994875</t>
+        </is>
+      </c>
+      <c r="E7" t="inlineStr">
+        <is>
+          <t>Korn</t>
+        </is>
+      </c>
+      <c r="F7" t="inlineStr">
+        <is>
+          <t>Whatever</t>
+        </is>
+      </c>
+      <c r="G7" t="n">
+        <v>50</v>
+      </c>
+      <c r="H7" t="n">
+        <v>95</v>
+      </c>
+      <c r="I7" t="inlineStr">
+        <is>
+          <t>AMS</t>
+        </is>
+      </c>
+      <c r="J7" t="inlineStr">
+        <is>
+          <t>DVD</t>
+        </is>
+      </c>
+      <c r="K7" t="inlineStr">
+        <is>
+          <t>Ashley</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Still figuring out how to resolve previous issues
</commit_message>
<xml_diff>
--- a/SO_Test.xlsx
+++ b/SO_Test.xlsx
@@ -16,13 +16,19 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="0"/>
-  <fonts count="1">
+  <fonts count="2">
     <font>
       <name val="Calibri"/>
       <family val="2"/>
       <color theme="1"/>
       <sz val="11"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <color theme="1"/>
+      <sz val="11"/>
     </font>
   </fonts>
   <fills count="2">
@@ -33,7 +39,14 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
     <border>
       <left/>
       <right/>
@@ -43,15 +56,27 @@
     </border>
   </borders>
   <cellStyleXfs count="1">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="general"/>
     </xf>
+    <xf numFmtId="3" fontId="0" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="3" fontId="1" fillId="0" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="4" fontId="1" fillId="0" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="right"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="general"/>
+    </xf>
+    <xf numFmtId="3" fontId="0" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="right"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -418,294 +443,531 @@
     <outlinePr summaryBelow="0"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:K7"/>
+  <dimension ref="A1:K11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15" outlineLevelCol="0"/>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <cols>
-    <col width="13.57642857142857" bestFit="1" customWidth="1" style="2" min="1" max="1"/>
-    <col width="16.29071428571428" bestFit="1" customWidth="1" style="2" min="2" max="2"/>
-    <col width="14.57642857142857" bestFit="1" customWidth="1" style="2" min="3" max="3"/>
-    <col width="13.57642857142857" bestFit="1" customWidth="1" style="2" min="4" max="4"/>
-    <col width="13.57642857142857" bestFit="1" customWidth="1" style="2" min="5" max="5"/>
-    <col width="13.57642857142857" bestFit="1" customWidth="1" style="2" min="6" max="6"/>
-    <col width="13.57642857142857" bestFit="1" customWidth="1" style="2" min="7" max="7"/>
-    <col width="13.57642857142857" bestFit="1" customWidth="1" style="2" min="8" max="8"/>
-    <col width="13.57642857142857" bestFit="1" customWidth="1" style="2" min="9" max="9"/>
-    <col width="13.57642857142857" bestFit="1" customWidth="1" style="2" min="10" max="10"/>
-    <col width="19.43357142857143" bestFit="1" customWidth="1" style="2" min="11" max="11"/>
+    <col width="13.57642857142857" bestFit="1" customWidth="1" style="5" min="1" max="1"/>
+    <col width="16.29071428571428" bestFit="1" customWidth="1" style="5" min="2" max="2"/>
+    <col width="14.57642857142857" bestFit="1" customWidth="1" style="5" min="3" max="3"/>
+    <col width="13.57642857142857" bestFit="1" customWidth="1" style="5" min="4" max="4"/>
+    <col width="13.57642857142857" bestFit="1" customWidth="1" style="5" min="5" max="5"/>
+    <col width="13.57642857142857" bestFit="1" customWidth="1" style="5" min="6" max="6"/>
+    <col width="13.57642857142857" bestFit="1" customWidth="1" style="6" min="7" max="7"/>
+    <col width="13.57642857142857" bestFit="1" customWidth="1" style="6" min="8" max="8"/>
+    <col width="13.57642857142857" bestFit="1" customWidth="1" style="5" min="9" max="9"/>
+    <col width="13.57642857142857" bestFit="1" customWidth="1" style="5" min="10" max="10"/>
+    <col width="19.43357142857143" bestFit="1" customWidth="1" style="5" min="11" max="11"/>
   </cols>
   <sheetData>
     <row r="1" ht="18.75" customHeight="1">
-      <c r="A1" s="2" t="inlineStr">
+      <c r="A1" s="5" t="inlineStr">
         <is>
           <t>DATE</t>
         </is>
       </c>
-      <c r="B1" s="2" t="inlineStr">
+      <c r="B1" s="5" t="inlineStr">
         <is>
           <t>REF NUM</t>
         </is>
       </c>
-      <c r="C1" s="2" t="inlineStr">
+      <c r="C1" s="5" t="inlineStr">
         <is>
           <t>CX NAME</t>
         </is>
       </c>
-      <c r="D1" s="2" t="inlineStr">
+      <c r="D1" s="5" t="inlineStr">
         <is>
           <t>PHONE</t>
         </is>
       </c>
-      <c r="E1" s="2" t="inlineStr">
+      <c r="E1" s="5" t="inlineStr">
         <is>
           <t>ARTIST</t>
         </is>
       </c>
-      <c r="F1" s="2" t="inlineStr">
+      <c r="F1" s="5" t="inlineStr">
         <is>
           <t>TITLE</t>
         </is>
       </c>
-      <c r="G1" s="2" t="inlineStr">
+      <c r="G1" s="6" t="inlineStr">
         <is>
           <t>DEPOSIT</t>
         </is>
       </c>
-      <c r="H1" s="2" t="inlineStr">
+      <c r="H1" s="6" t="inlineStr">
         <is>
           <t>PRICE</t>
         </is>
       </c>
-      <c r="I1" s="2" t="inlineStr">
+      <c r="I1" s="5" t="inlineStr">
         <is>
           <t>VENDOR</t>
         </is>
       </c>
-      <c r="J1" s="2" t="inlineStr">
+      <c r="J1" s="5" t="inlineStr">
         <is>
           <t>TYPE</t>
         </is>
       </c>
-      <c r="K1" s="2" t="inlineStr">
+      <c r="K1" s="5" t="inlineStr">
         <is>
           <t>CLERK NAME</t>
         </is>
       </c>
     </row>
-    <row r="2">
-      <c r="A2" t="inlineStr">
+    <row r="2" ht="18.75" customHeight="1">
+      <c r="A2" s="5" t="inlineStr">
         <is>
           <t>01/10/2024</t>
         </is>
       </c>
-      <c r="B2" t="inlineStr">
+      <c r="B2" s="5" t="inlineStr">
         <is>
           <t>SO240110001</t>
         </is>
       </c>
-      <c r="C2" t="inlineStr">
+      <c r="C2" s="5" t="inlineStr">
         <is>
           <t>AshleyBaker</t>
         </is>
       </c>
-      <c r="D2" t="inlineStr">
+      <c r="D2" s="5" t="inlineStr">
         <is>
           <t>9157994875</t>
         </is>
       </c>
-      <c r="E2" t="inlineStr">
+      <c r="E2" s="5" t="inlineStr">
         <is>
           <t>Tool</t>
         </is>
       </c>
-      <c r="F2" t="inlineStr">
+      <c r="F2" s="5" t="inlineStr">
         <is>
           <t>Aenima</t>
         </is>
       </c>
-      <c r="G2" t="n">
+      <c r="G2" s="3" t="n">
         <v>50</v>
       </c>
-      <c r="H2" t="n">
+      <c r="H2" s="4" t="n">
         <v>90.98999999999999</v>
       </c>
-      <c r="I2" t="inlineStr">
+      <c r="I2" s="5" t="inlineStr">
         <is>
           <t>AEC</t>
         </is>
       </c>
-      <c r="J2" t="inlineStr">
+      <c r="J2" s="5" t="inlineStr">
         <is>
           <t>DVD</t>
         </is>
       </c>
-      <c r="K2" t="inlineStr">
+      <c r="K2" s="5" t="inlineStr">
         <is>
           <t>Ashley</t>
         </is>
       </c>
     </row>
-    <row r="3">
-      <c r="A3" t="inlineStr">
+    <row r="3" ht="18.75" customHeight="1">
+      <c r="A3" s="5" t="inlineStr">
         <is>
           <t>01/10/2024</t>
         </is>
       </c>
-      <c r="B3" t="inlineStr">
+      <c r="B3" s="5" t="inlineStr">
         <is>
           <t>SO240110002</t>
         </is>
       </c>
-      <c r="C3" t="inlineStr">
+      <c r="C3" s="5" t="inlineStr">
         <is>
           <t>Ashley Baker</t>
         </is>
       </c>
-      <c r="D3" t="inlineStr">
+      <c r="D3" s="5" t="inlineStr">
         <is>
           <t>9157994875</t>
         </is>
       </c>
-      <c r="E3" t="inlineStr">
+      <c r="E3" s="5" t="inlineStr">
         <is>
           <t>SOAD</t>
         </is>
       </c>
-      <c r="F3" t="inlineStr">
+      <c r="F3" s="5" t="inlineStr">
         <is>
           <t>Hypnotize</t>
         </is>
       </c>
-      <c r="G3" t="n">
+      <c r="G3" s="3" t="n">
         <v>50</v>
       </c>
-      <c r="H3" t="n">
+      <c r="H3" s="3" t="n">
         <v>125</v>
       </c>
-      <c r="I3" t="inlineStr">
+      <c r="I3" s="5" t="inlineStr">
         <is>
           <t>AMS</t>
         </is>
       </c>
-      <c r="J3" t="inlineStr">
+      <c r="J3" s="5" t="inlineStr">
         <is>
           <t>LP</t>
         </is>
       </c>
-      <c r="K3" t="inlineStr">
+      <c r="K3" s="5" t="inlineStr">
         <is>
           <t>Ashley</t>
         </is>
       </c>
     </row>
-    <row r="4"/>
-    <row r="5">
-      <c r="A5" t="inlineStr">
+    <row r="4" ht="18.75" customHeight="1">
+      <c r="A4" s="5" t="n"/>
+      <c r="B4" s="5" t="n"/>
+      <c r="C4" s="5" t="n"/>
+      <c r="D4" s="5" t="n"/>
+      <c r="E4" s="5" t="n"/>
+      <c r="F4" s="5" t="n"/>
+      <c r="G4" s="6" t="n"/>
+      <c r="H4" s="6" t="n"/>
+      <c r="I4" s="5" t="n"/>
+      <c r="J4" s="5" t="n"/>
+      <c r="K4" s="5" t="n"/>
+    </row>
+    <row r="5" ht="18.75" customHeight="1">
+      <c r="A5" s="5" t="inlineStr">
         <is>
           <t>01/11/2024</t>
         </is>
       </c>
-      <c r="B5" t="inlineStr">
+      <c r="B5" s="5" t="inlineStr">
         <is>
           <t>SO240111001</t>
         </is>
       </c>
-      <c r="C5" t="inlineStr">
+      <c r="C5" s="5" t="inlineStr">
         <is>
           <t>Ashley Baker</t>
         </is>
       </c>
-      <c r="D5" t="inlineStr">
+      <c r="D5" s="5" t="inlineStr">
         <is>
           <t>9157994875</t>
         </is>
       </c>
-      <c r="E5" t="inlineStr">
+      <c r="E5" s="5" t="inlineStr">
         <is>
           <t>Smashing Pumpkins</t>
         </is>
       </c>
-      <c r="F5" t="inlineStr">
+      <c r="F5" s="5" t="inlineStr">
         <is>
           <t>Siamese Dream</t>
         </is>
       </c>
-      <c r="G5" t="n">
+      <c r="G5" s="3" t="n">
         <v>55</v>
       </c>
-      <c r="H5" t="n">
+      <c r="H5" s="4" t="n">
         <v>120.99</v>
       </c>
-      <c r="I5" t="inlineStr">
+      <c r="I5" s="5" t="inlineStr">
         <is>
           <t>AEC</t>
         </is>
       </c>
-      <c r="J5" t="inlineStr">
+      <c r="J5" s="5" t="inlineStr">
         <is>
           <t>DVD</t>
         </is>
       </c>
-      <c r="K5" t="inlineStr">
+      <c r="K5" s="5" t="inlineStr">
         <is>
           <t>Ashley</t>
         </is>
       </c>
     </row>
-    <row r="7">
-      <c r="A7" t="inlineStr">
+    <row r="6" ht="18.75" customHeight="1">
+      <c r="A6" s="5" t="n"/>
+      <c r="B6" s="5" t="n"/>
+      <c r="C6" s="5" t="n"/>
+      <c r="D6" s="5" t="n"/>
+      <c r="E6" s="5" t="n"/>
+      <c r="F6" s="5" t="n"/>
+      <c r="G6" s="6" t="n"/>
+      <c r="H6" s="6" t="n"/>
+      <c r="I6" s="5" t="n"/>
+      <c r="J6" s="5" t="n"/>
+      <c r="K6" s="5" t="n"/>
+    </row>
+    <row r="7" ht="18.75" customHeight="1">
+      <c r="A7" s="5" t="inlineStr">
         <is>
           <t>01/12/2024</t>
         </is>
       </c>
-      <c r="B7" t="inlineStr">
+      <c r="B7" s="5" t="inlineStr">
         <is>
           <t>SO240112001</t>
         </is>
       </c>
-      <c r="C7" t="inlineStr">
+      <c r="C7" s="5" t="inlineStr">
         <is>
           <t>Ashley Baker</t>
         </is>
       </c>
-      <c r="D7" t="inlineStr">
+      <c r="D7" s="5" t="inlineStr">
         <is>
           <t>9157994875</t>
         </is>
       </c>
-      <c r="E7" t="inlineStr">
+      <c r="E7" s="5" t="inlineStr">
         <is>
           <t>Korn</t>
         </is>
       </c>
-      <c r="F7" t="inlineStr">
+      <c r="F7" s="5" t="inlineStr">
         <is>
           <t>Whatever</t>
         </is>
       </c>
-      <c r="G7" t="n">
+      <c r="G7" s="3" t="n">
         <v>50</v>
       </c>
-      <c r="H7" t="n">
+      <c r="H7" s="3" t="n">
         <v>95</v>
       </c>
-      <c r="I7" t="inlineStr">
+      <c r="I7" s="5" t="inlineStr">
         <is>
           <t>AMS</t>
         </is>
       </c>
-      <c r="J7" t="inlineStr">
+      <c r="J7" s="5" t="inlineStr">
         <is>
           <t>DVD</t>
         </is>
       </c>
-      <c r="K7" t="inlineStr">
+      <c r="K7" s="5" t="inlineStr">
         <is>
           <t>Ashley</t>
+        </is>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="inlineStr">
+        <is>
+          <t>01/12/2024</t>
+        </is>
+      </c>
+      <c r="B8" t="inlineStr">
+        <is>
+          <t>SO240112002</t>
+        </is>
+      </c>
+      <c r="C8" t="inlineStr">
+        <is>
+          <t>Ashley</t>
+        </is>
+      </c>
+      <c r="D8" t="inlineStr">
+        <is>
+          <t>9157994875</t>
+        </is>
+      </c>
+      <c r="E8" t="inlineStr">
+        <is>
+          <t>ATTILA</t>
+        </is>
+      </c>
+      <c r="F8" t="inlineStr">
+        <is>
+          <t>ABOUT THAT LIFE</t>
+        </is>
+      </c>
+      <c r="G8" t="n">
+        <v>25</v>
+      </c>
+      <c r="H8" t="n">
+        <v>65</v>
+      </c>
+      <c r="I8" t="inlineStr">
+        <is>
+          <t>AMS</t>
+        </is>
+      </c>
+      <c r="J8" t="inlineStr">
+        <is>
+          <t>CD</t>
+        </is>
+      </c>
+      <c r="K8" t="inlineStr">
+        <is>
+          <t>Ashley</t>
+        </is>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="inlineStr">
+        <is>
+          <t>01/12/2024</t>
+        </is>
+      </c>
+      <c r="B9" t="inlineStr">
+        <is>
+          <t>SO240112003</t>
+        </is>
+      </c>
+      <c r="C9" t="inlineStr">
+        <is>
+          <t>Ashley</t>
+        </is>
+      </c>
+      <c r="D9" t="inlineStr">
+        <is>
+          <t>9157994875</t>
+        </is>
+      </c>
+      <c r="E9" t="inlineStr">
+        <is>
+          <t>Chicago</t>
+        </is>
+      </c>
+      <c r="F9" t="inlineStr">
+        <is>
+          <t>EH</t>
+        </is>
+      </c>
+      <c r="G9" t="n">
+        <v>15</v>
+      </c>
+      <c r="H9" t="n">
+        <v>74</v>
+      </c>
+      <c r="I9" t="inlineStr">
+        <is>
+          <t>AMA</t>
+        </is>
+      </c>
+      <c r="J9" t="inlineStr">
+        <is>
+          <t>DVD</t>
+        </is>
+      </c>
+      <c r="K9" t="inlineStr">
+        <is>
+          <t>Ashley</t>
+        </is>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="inlineStr">
+        <is>
+          <t>01/12/2024</t>
+        </is>
+      </c>
+      <c r="B10" t="inlineStr">
+        <is>
+          <t>SO240112004</t>
+        </is>
+      </c>
+      <c r="C10" t="inlineStr">
+        <is>
+          <t>A</t>
+        </is>
+      </c>
+      <c r="D10" t="inlineStr">
+        <is>
+          <t>9157994875</t>
+        </is>
+      </c>
+      <c r="E10" t="inlineStr">
+        <is>
+          <t>666</t>
+        </is>
+      </c>
+      <c r="F10" t="inlineStr">
+        <is>
+          <t>999</t>
+        </is>
+      </c>
+      <c r="G10" t="n">
+        <v>12</v>
+      </c>
+      <c r="H10" t="n">
+        <v>999</v>
+      </c>
+      <c r="I10" t="inlineStr">
+        <is>
+          <t>AMS</t>
+        </is>
+      </c>
+      <c r="J10" t="inlineStr">
+        <is>
+          <t>LP</t>
+        </is>
+      </c>
+      <c r="K10" t="inlineStr">
+        <is>
+          <t>A</t>
+        </is>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" t="inlineStr">
+        <is>
+          <t>01/12/2024</t>
+        </is>
+      </c>
+      <c r="B11" t="inlineStr">
+        <is>
+          <t>SO240112005</t>
+        </is>
+      </c>
+      <c r="C11" t="inlineStr">
+        <is>
+          <t>ASHLEY</t>
+        </is>
+      </c>
+      <c r="D11" t="inlineStr">
+        <is>
+          <t>9157994875</t>
+        </is>
+      </c>
+      <c r="E11" t="inlineStr">
+        <is>
+          <t>ASAASASASAS</t>
+        </is>
+      </c>
+      <c r="F11" t="inlineStr">
+        <is>
+          <t>OSDFGJKH</t>
+        </is>
+      </c>
+      <c r="G11" t="n">
+        <v>25</v>
+      </c>
+      <c r="H11" t="n">
+        <v>3333</v>
+      </c>
+      <c r="I11" t="inlineStr">
+        <is>
+          <t>AMS</t>
+        </is>
+      </c>
+      <c r="J11" t="inlineStr">
+        <is>
+          <t>BLU-RAY</t>
+        </is>
+      </c>
+      <c r="K11" t="inlineStr">
+        <is>
+          <t>A</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
Still dealing with issues
</commit_message>
<xml_diff>
--- a/SO_Test.xlsx
+++ b/SO_Test.xlsx
@@ -443,7 +443,7 @@
     <outlinePr summaryBelow="0"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:K11"/>
+  <dimension ref="A1:K12"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -971,6 +971,59 @@
         </is>
       </c>
     </row>
+    <row r="12">
+      <c r="A12" t="inlineStr">
+        <is>
+          <t>01/12/2024</t>
+        </is>
+      </c>
+      <c r="B12" t="inlineStr">
+        <is>
+          <t>SO240112006</t>
+        </is>
+      </c>
+      <c r="C12" t="inlineStr">
+        <is>
+          <t>a</t>
+        </is>
+      </c>
+      <c r="D12" t="inlineStr">
+        <is>
+          <t>9157994875</t>
+        </is>
+      </c>
+      <c r="E12" t="inlineStr">
+        <is>
+          <t>a</t>
+        </is>
+      </c>
+      <c r="F12" t="inlineStr">
+        <is>
+          <t>a</t>
+        </is>
+      </c>
+      <c r="G12" t="n">
+        <v>2</v>
+      </c>
+      <c r="H12" t="n">
+        <v>42</v>
+      </c>
+      <c r="I12" t="inlineStr">
+        <is>
+          <t>AEC</t>
+        </is>
+      </c>
+      <c r="J12" t="inlineStr">
+        <is>
+          <t>OTHER</t>
+        </is>
+      </c>
+      <c r="K12" t="inlineStr">
+        <is>
+          <t>a</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Changed format of the phone coumn in xlsx file
</commit_message>
<xml_diff>
--- a/SO_Test.xlsx
+++ b/SO_Test.xlsx
@@ -1,15 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion rupBuild="9303" lowestEdited="5" lastEdited="5" appName="xl"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="27126"/>
   <workbookPr/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/c9838447ef4aa4dc/Documents/AllThatMusic_SpecialOrdersForm/"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="1" documentId="11_1558BCD8F2A574A071554D09FF14FFCE80F41B3A" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{EFFC56CB-1E58-47E8-841E-7C3EE04A6A49}"/>
   <bookViews>
-    <workbookView xWindow="480" yWindow="60" windowWidth="18195" windowHeight="8505" activeTab="0"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21120" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet r:id="rId1" sheetId="1" name="Sheet1"/>
+    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr fullCalcOnLoad="1"/>
+  <calcPr calcId="0"/>
 </workbook>
 </file>
 
@@ -181,8 +187,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" mc:Ignorable="x14ac">
-  <numFmts count="0"/>
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -231,35 +236,33 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
-    <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0"/>
-    <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0" applyAlignment="1">
-      <alignment horizontal="general"/>
-    </xf>
-    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="1" applyBorder="1" fontId="1" applyFont="1" fillId="0" applyAlignment="1">
+  <cellXfs count="6">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="3" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="1" applyBorder="1" fontId="2" applyFont="1" fillId="0" applyAlignment="1">
+    <xf numFmtId="3" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf xfId="0" numFmtId="4" applyNumberFormat="1" borderId="1" applyBorder="1" fontId="2" applyFont="1" fillId="0" applyAlignment="1">
+    <xf numFmtId="4" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0" applyAlignment="1">
-      <alignment horizontal="general"/>
-    </xf>
-    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="0" fontId="0" fillId="0" applyAlignment="1">
+    <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle xfId="0" builtinId="0" name="Normal"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
-    <ext uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
-      <x14ac:slicerStyles xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" defaultSlicerStyle="SlicerStyleLight1"/>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
     </ext>
   </extLst>
 </styleSheet>
@@ -270,10 +273,10 @@
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
-        <a:sysClr lastClr="000000" val="windowText"/>
+        <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
       <a:lt1>
-        <a:sysClr lastClr="FFFFFF" val="window"/>
+        <a:sysClr val="window" lastClr="FFFFFF"/>
       </a:lt1>
       <a:dk2>
         <a:srgbClr val="44546A"/>
@@ -311,71 +314,71 @@
         <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
-        <a:font typeface="ＭＳ Ｐゴシック" script="Jpan"/>
-        <a:font typeface="맑은 고딕" script="Hang"/>
-        <a:font typeface="宋体" script="Hans"/>
-        <a:font typeface="新細明體" script="Hant"/>
-        <a:font typeface="Times New Roman" script="Arab"/>
-        <a:font typeface="Times New Roman" script="Hebr"/>
-        <a:font typeface="Tahoma" script="Thai"/>
-        <a:font typeface="Nyala" script="Ethi"/>
-        <a:font typeface="Vrinda" script="Beng"/>
-        <a:font typeface="Shruti" script="Gujr"/>
-        <a:font typeface="MoolBoran" script="Khmr"/>
-        <a:font typeface="Tunga" script="Knda"/>
-        <a:font typeface="Raavi" script="Guru"/>
-        <a:font typeface="Euphemia" script="Cans"/>
-        <a:font typeface="Plantagenet Cherokee" script="Cher"/>
-        <a:font typeface="Microsoft Yi Baiti" script="Yiii"/>
-        <a:font typeface="Microsoft Himalaya" script="Tibt"/>
-        <a:font typeface="MV Boli" script="Thaa"/>
-        <a:font typeface="Mangal" script="Deva"/>
-        <a:font typeface="Gautami" script="Telu"/>
-        <a:font typeface="Latha" script="Taml"/>
-        <a:font typeface="Estrangelo Edessa" script="Syrc"/>
-        <a:font typeface="Kalinga" script="Orya"/>
-        <a:font typeface="Kartika" script="Mlym"/>
-        <a:font typeface="DokChampa" script="Laoo"/>
-        <a:font typeface="Iskoola Pota" script="Sinh"/>
-        <a:font typeface="Mongolian Baiti" script="Mong"/>
-        <a:font typeface="Times New Roman" script="Viet"/>
-        <a:font typeface="Microsoft Uighur" script="Uigh"/>
-        <a:font typeface="Sylfaen" script="Geor"/>
+        <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
+        <a:font script="Hang" typeface="맑은 고딕"/>
+        <a:font script="Hans" typeface="宋体"/>
+        <a:font script="Hant" typeface="新細明體"/>
+        <a:font script="Arab" typeface="Times New Roman"/>
+        <a:font script="Hebr" typeface="Times New Roman"/>
+        <a:font script="Thai" typeface="Tahoma"/>
+        <a:font script="Ethi" typeface="Nyala"/>
+        <a:font script="Beng" typeface="Vrinda"/>
+        <a:font script="Gujr" typeface="Shruti"/>
+        <a:font script="Khmr" typeface="MoolBoran"/>
+        <a:font script="Knda" typeface="Tunga"/>
+        <a:font script="Guru" typeface="Raavi"/>
+        <a:font script="Cans" typeface="Euphemia"/>
+        <a:font script="Cher" typeface="Plantagenet Cherokee"/>
+        <a:font script="Yiii" typeface="Microsoft Yi Baiti"/>
+        <a:font script="Tibt" typeface="Microsoft Himalaya"/>
+        <a:font script="Thaa" typeface="MV Boli"/>
+        <a:font script="Deva" typeface="Mangal"/>
+        <a:font script="Telu" typeface="Gautami"/>
+        <a:font script="Taml" typeface="Latha"/>
+        <a:font script="Syrc" typeface="Estrangelo Edessa"/>
+        <a:font script="Orya" typeface="Kalinga"/>
+        <a:font script="Mlym" typeface="Kartika"/>
+        <a:font script="Laoo" typeface="DokChampa"/>
+        <a:font script="Sinh" typeface="Iskoola Pota"/>
+        <a:font script="Mong" typeface="Mongolian Baiti"/>
+        <a:font script="Viet" typeface="Times New Roman"/>
+        <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
-        <a:font typeface="ＭＳ Ｐゴシック" script="Jpan"/>
-        <a:font typeface="맑은 고딕" script="Hang"/>
-        <a:font typeface="宋体" script="Hans"/>
-        <a:font typeface="新細明體" script="Hant"/>
-        <a:font typeface="Arial" script="Arab"/>
-        <a:font typeface="Arial" script="Hebr"/>
-        <a:font typeface="Tahoma" script="Thai"/>
-        <a:font typeface="Nyala" script="Ethi"/>
-        <a:font typeface="Vrinda" script="Beng"/>
-        <a:font typeface="Shruti" script="Gujr"/>
-        <a:font typeface="DaunPenh" script="Khmr"/>
-        <a:font typeface="Tunga" script="Knda"/>
-        <a:font typeface="Raavi" script="Guru"/>
-        <a:font typeface="Euphemia" script="Cans"/>
-        <a:font typeface="Plantagenet Cherokee" script="Cher"/>
-        <a:font typeface="Microsoft Yi Baiti" script="Yiii"/>
-        <a:font typeface="Microsoft Himalaya" script="Tibt"/>
-        <a:font typeface="MV Boli" script="Thaa"/>
-        <a:font typeface="Mangal" script="Deva"/>
-        <a:font typeface="Gautami" script="Telu"/>
-        <a:font typeface="Latha" script="Taml"/>
-        <a:font typeface="Estrangelo Edessa" script="Syrc"/>
-        <a:font typeface="Kalinga" script="Orya"/>
-        <a:font typeface="Kartika" script="Mlym"/>
-        <a:font typeface="DokChampa" script="Laoo"/>
-        <a:font typeface="Iskoola Pota" script="Sinh"/>
-        <a:font typeface="Mongolian Baiti" script="Mong"/>
-        <a:font typeface="Arial" script="Viet"/>
-        <a:font typeface="Microsoft Uighur" script="Uigh"/>
-        <a:font typeface="Sylfaen" script="Geor"/>
+        <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
+        <a:font script="Hang" typeface="맑은 고딕"/>
+        <a:font script="Hans" typeface="宋体"/>
+        <a:font script="Hant" typeface="新細明體"/>
+        <a:font script="Arab" typeface="Arial"/>
+        <a:font script="Hebr" typeface="Arial"/>
+        <a:font script="Thai" typeface="Tahoma"/>
+        <a:font script="Ethi" typeface="Nyala"/>
+        <a:font script="Beng" typeface="Vrinda"/>
+        <a:font script="Gujr" typeface="Shruti"/>
+        <a:font script="Khmr" typeface="DaunPenh"/>
+        <a:font script="Knda" typeface="Tunga"/>
+        <a:font script="Guru" typeface="Raavi"/>
+        <a:font script="Cans" typeface="Euphemia"/>
+        <a:font script="Cher" typeface="Plantagenet Cherokee"/>
+        <a:font script="Yiii" typeface="Microsoft Yi Baiti"/>
+        <a:font script="Tibt" typeface="Microsoft Himalaya"/>
+        <a:font script="Thaa" typeface="MV Boli"/>
+        <a:font script="Deva" typeface="Mangal"/>
+        <a:font script="Telu" typeface="Gautami"/>
+        <a:font script="Taml" typeface="Latha"/>
+        <a:font script="Syrc" typeface="Estrangelo Edessa"/>
+        <a:font script="Orya" typeface="Kalinga"/>
+        <a:font script="Mlym" typeface="Kartika"/>
+        <a:font script="Laoo" typeface="DokChampa"/>
+        <a:font script="Sinh" typeface="Iskoola Pota"/>
+        <a:font script="Mong" typeface="Mongolian Baiti"/>
+        <a:font script="Viet" typeface="Arial"/>
+        <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -403,7 +406,7 @@
               </a:schemeClr>
             </a:gs>
           </a:gsLst>
-          <a:lin scaled="1" ang="16200000"/>
+          <a:lin ang="16200000" scaled="1"/>
         </a:gradFill>
         <a:gradFill rotWithShape="1">
           <a:gsLst>
@@ -426,11 +429,11 @@
               </a:schemeClr>
             </a:gs>
           </a:gsLst>
-          <a:lin scaled="1" ang="16200000"/>
+          <a:lin ang="16200000" scaled="1"/>
         </a:gradFill>
       </a:fillStyleLst>
       <a:lnStyleLst>
-        <a:ln algn="ctr" cmpd="sng" cap="flat" w="9525">
+        <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
           <a:solidFill>
             <a:schemeClr val="phClr">
               <a:shade val="9500"/>
@@ -439,13 +442,13 @@
           </a:solidFill>
           <a:prstDash val="solid"/>
         </a:ln>
-        <a:ln algn="ctr" cmpd="sng" cap="flat" w="25400">
+        <a:ln w="25400" cap="flat" cmpd="sng" algn="ctr">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
           <a:prstDash val="solid"/>
         </a:ln>
-        <a:ln algn="ctr" cmpd="sng" cap="flat" w="38100">
+        <a:ln w="38100" cap="flat" cmpd="sng" algn="ctr">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
@@ -455,7 +458,7 @@
       <a:effectStyleLst>
         <a:effectStyle>
           <a:effectLst>
-            <a:outerShdw dir="5400000" rotWithShape="0" dist="23000" blurRad="40000">
+            <a:outerShdw blurRad="40000" dist="23000" dir="5400000" rotWithShape="0">
               <a:srgbClr val="000000">
                 <a:alpha val="38000"/>
               </a:srgbClr>
@@ -464,7 +467,7 @@
         </a:effectStyle>
         <a:effectStyle>
           <a:effectLst>
-            <a:outerShdw dir="5400000" rotWithShape="0" dist="23000" blurRad="40000">
+            <a:outerShdw blurRad="40000" dist="23000" dir="5400000" rotWithShape="0">
               <a:srgbClr val="000000">
                 <a:alpha val="35000"/>
               </a:srgbClr>
@@ -473,7 +476,7 @@
         </a:effectStyle>
         <a:effectStyle>
           <a:effectLst>
-            <a:outerShdw dir="5400000" rotWithShape="0" dist="23000" blurRad="40000">
+            <a:outerShdw blurRad="40000" dist="23000" dir="5400000" rotWithShape="0">
               <a:srgbClr val="000000">
                 <a:alpha val="35000"/>
               </a:srgbClr>
@@ -481,10 +484,10 @@
           </a:effectLst>
           <a:scene3d>
             <a:camera prst="orthographicFront">
-              <a:rot rev="0" lon="0" lat="0"/>
+              <a:rot lat="0" lon="0" rev="0"/>
             </a:camera>
-            <a:lightRig dir="t" rig="threePt">
-              <a:rot rev="1200000" lon="0" lat="0"/>
+            <a:lightRig rig="threePt" dir="t">
+              <a:rot lat="0" lon="0" rev="1200000"/>
             </a:lightRig>
           </a:scene3d>
           <a:sp3d>
@@ -549,402 +552,383 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <sheetPr>
     <outlinePr summaryBelow="0"/>
   </sheetPr>
   <dimension ref="A1:K12"/>
   <sheetViews>
-    <sheetView workbookViewId="0" tabSelected="1"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F22" sqref="F22"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" style="5" width="13.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="2" max="2" style="5" width="16.290714285714284" customWidth="1" bestFit="1"/>
-    <col min="3" max="3" style="5" width="14.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="4" max="4" style="5" width="13.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="5" max="5" style="5" width="13.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="6" max="6" style="5" width="13.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="7" max="7" style="6" width="13.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="8" max="8" style="6" width="13.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="9" max="9" style="5" width="13.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="10" max="10" style="5" width="13.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="11" max="11" style="5" width="19.433571428571426" customWidth="1" bestFit="1"/>
+    <col min="1" max="1" width="13.5703125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="16.28515625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="14.5703125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="13.5703125" style="5" bestFit="1" customWidth="1"/>
+    <col min="5" max="6" width="13.5703125" bestFit="1" customWidth="1"/>
+    <col min="7" max="8" width="13.5703125" style="4" bestFit="1" customWidth="1"/>
+    <col min="9" max="10" width="13.5703125" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="19.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row x14ac:dyDescent="0.25" r="1" customHeight="1" ht="18.75">
-      <c r="A1" s="1" t="s">
+    <row r="1" spans="1:11" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="B1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="C1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="D1" s="5" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="E1" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="F1" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="2" t="s">
+      <c r="G1" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="H1" s="2" t="s">
+      <c r="H1" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="I1" s="1" t="s">
+      <c r="I1" t="s">
         <v>8</v>
       </c>
-      <c r="J1" s="1" t="s">
+      <c r="J1" t="s">
         <v>9</v>
       </c>
-      <c r="K1" s="1" t="s">
+      <c r="K1" t="s">
         <v>10</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="2" customHeight="1" ht="19.5">
-      <c r="A2" s="1" t="s">
+    <row r="2" spans="1:11" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
         <v>11</v>
       </c>
-      <c r="B2" s="1" t="s">
+      <c r="B2" t="s">
         <v>12</v>
       </c>
-      <c r="C2" s="1" t="s">
+      <c r="C2" t="s">
         <v>13</v>
       </c>
-      <c r="D2" s="1" t="s">
+      <c r="D2" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="E2" s="1" t="s">
+      <c r="E2" t="s">
         <v>15</v>
       </c>
-      <c r="F2" s="1" t="s">
+      <c r="F2" t="s">
         <v>16</v>
       </c>
-      <c r="G2" s="3">
+      <c r="G2" s="2">
         <v>50</v>
       </c>
-      <c r="H2" s="4">
+      <c r="H2" s="3">
         <v>90.99</v>
       </c>
-      <c r="I2" s="1" t="s">
+      <c r="I2" t="s">
         <v>17</v>
       </c>
-      <c r="J2" s="1" t="s">
+      <c r="J2" t="s">
         <v>18</v>
       </c>
-      <c r="K2" s="1" t="s">
+      <c r="K2" t="s">
         <v>19</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="3" customHeight="1" ht="19.5">
-      <c r="A3" s="1" t="s">
+    <row r="3" spans="1:11" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
         <v>11</v>
       </c>
-      <c r="B3" s="1" t="s">
+      <c r="B3" t="s">
         <v>20</v>
       </c>
-      <c r="C3" s="1" t="s">
+      <c r="C3" t="s">
         <v>21</v>
       </c>
-      <c r="D3" s="1" t="s">
+      <c r="D3" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="E3" s="1" t="s">
+      <c r="E3" t="s">
         <v>22</v>
       </c>
-      <c r="F3" s="1" t="s">
+      <c r="F3" t="s">
         <v>23</v>
       </c>
-      <c r="G3" s="3">
+      <c r="G3" s="2">
         <v>50</v>
       </c>
-      <c r="H3" s="3">
+      <c r="H3" s="2">
         <v>125</v>
       </c>
-      <c r="I3" s="1" t="s">
+      <c r="I3" t="s">
         <v>24</v>
       </c>
-      <c r="J3" s="1" t="s">
+      <c r="J3" t="s">
         <v>25</v>
       </c>
-      <c r="K3" s="1" t="s">
+      <c r="K3" t="s">
         <v>19</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="4" customHeight="1" ht="18.75">
-      <c r="A4" s="1"/>
-      <c r="B4" s="1"/>
-      <c r="C4" s="1"/>
-      <c r="D4" s="1"/>
-      <c r="E4" s="1"/>
-      <c r="F4" s="1"/>
-      <c r="G4" s="2"/>
-      <c r="H4" s="2"/>
-      <c r="I4" s="1"/>
-      <c r="J4" s="1"/>
-      <c r="K4" s="1"/>
-    </row>
-    <row x14ac:dyDescent="0.25" r="5" customHeight="1" ht="19.5">
-      <c r="A5" s="1" t="s">
+    <row r="4" spans="1:11" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="G4" s="1"/>
+      <c r="H4" s="1"/>
+    </row>
+    <row r="5" spans="1:11" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
         <v>26</v>
       </c>
-      <c r="B5" s="1" t="s">
+      <c r="B5" t="s">
         <v>27</v>
       </c>
-      <c r="C5" s="1" t="s">
+      <c r="C5" t="s">
         <v>21</v>
       </c>
-      <c r="D5" s="1" t="s">
+      <c r="D5" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="E5" s="1" t="s">
+      <c r="E5" t="s">
         <v>28</v>
       </c>
-      <c r="F5" s="1" t="s">
+      <c r="F5" t="s">
         <v>29</v>
       </c>
-      <c r="G5" s="3">
+      <c r="G5" s="2">
         <v>55</v>
       </c>
-      <c r="H5" s="4">
+      <c r="H5" s="3">
         <v>120.99</v>
       </c>
-      <c r="I5" s="1" t="s">
+      <c r="I5" t="s">
         <v>17</v>
       </c>
-      <c r="J5" s="1" t="s">
+      <c r="J5" t="s">
         <v>18</v>
       </c>
-      <c r="K5" s="1" t="s">
+      <c r="K5" t="s">
         <v>19</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="6" customHeight="1" ht="18.75">
-      <c r="A6" s="1"/>
-      <c r="B6" s="1"/>
-      <c r="C6" s="1"/>
-      <c r="D6" s="1"/>
-      <c r="E6" s="1"/>
-      <c r="F6" s="1"/>
-      <c r="G6" s="2"/>
-      <c r="H6" s="2"/>
-      <c r="I6" s="1"/>
-      <c r="J6" s="1"/>
-      <c r="K6" s="1"/>
-    </row>
-    <row x14ac:dyDescent="0.25" r="7" customHeight="1" ht="19.5">
-      <c r="A7" s="1" t="s">
+    <row r="6" spans="1:11" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="G6" s="1"/>
+      <c r="H6" s="1"/>
+    </row>
+    <row r="7" spans="1:11" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
         <v>30</v>
       </c>
-      <c r="B7" s="1" t="s">
+      <c r="B7" t="s">
         <v>31</v>
       </c>
-      <c r="C7" s="1" t="s">
+      <c r="C7" t="s">
         <v>21</v>
       </c>
-      <c r="D7" s="1" t="s">
+      <c r="D7" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="E7" s="1" t="s">
+      <c r="E7" t="s">
         <v>32</v>
       </c>
-      <c r="F7" s="1" t="s">
+      <c r="F7" t="s">
         <v>33</v>
       </c>
-      <c r="G7" s="3">
+      <c r="G7" s="2">
         <v>50</v>
       </c>
-      <c r="H7" s="3">
+      <c r="H7" s="2">
         <v>95</v>
       </c>
-      <c r="I7" s="1" t="s">
+      <c r="I7" t="s">
         <v>24</v>
       </c>
-      <c r="J7" s="1" t="s">
+      <c r="J7" t="s">
         <v>18</v>
       </c>
-      <c r="K7" s="1" t="s">
+      <c r="K7" t="s">
         <v>19</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="8" customHeight="1" ht="18.75">
-      <c r="A8" s="1" t="s">
+    <row r="8" spans="1:11" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
         <v>30</v>
       </c>
-      <c r="B8" s="1" t="s">
+      <c r="B8" t="s">
         <v>34</v>
       </c>
-      <c r="C8" s="1" t="s">
+      <c r="C8" t="s">
         <v>19</v>
       </c>
-      <c r="D8" s="1" t="s">
+      <c r="D8" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="E8" s="1" t="s">
+      <c r="E8" t="s">
         <v>35</v>
       </c>
-      <c r="F8" s="1" t="s">
+      <c r="F8" t="s">
         <v>36</v>
       </c>
-      <c r="G8" s="2">
+      <c r="G8" s="1">
         <v>25</v>
       </c>
-      <c r="H8" s="2">
+      <c r="H8" s="1">
         <v>65</v>
       </c>
-      <c r="I8" s="1" t="s">
+      <c r="I8" t="s">
         <v>24</v>
       </c>
-      <c r="J8" s="1" t="s">
+      <c r="J8" t="s">
         <v>37</v>
       </c>
-      <c r="K8" s="1" t="s">
+      <c r="K8" t="s">
         <v>19</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="9" customHeight="1" ht="18.75">
-      <c r="A9" s="1" t="s">
+    <row r="9" spans="1:11" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
         <v>30</v>
       </c>
-      <c r="B9" s="1" t="s">
+      <c r="B9" t="s">
         <v>38</v>
       </c>
-      <c r="C9" s="1" t="s">
+      <c r="C9" t="s">
         <v>19</v>
       </c>
-      <c r="D9" s="1" t="s">
+      <c r="D9" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="E9" s="1" t="s">
+      <c r="E9" t="s">
         <v>39</v>
       </c>
-      <c r="F9" s="1" t="s">
+      <c r="F9" t="s">
         <v>40</v>
       </c>
-      <c r="G9" s="2">
+      <c r="G9" s="1">
         <v>15</v>
       </c>
-      <c r="H9" s="2">
+      <c r="H9" s="1">
         <v>74</v>
       </c>
-      <c r="I9" s="1" t="s">
+      <c r="I9" t="s">
         <v>41</v>
       </c>
-      <c r="J9" s="1" t="s">
+      <c r="J9" t="s">
         <v>18</v>
       </c>
-      <c r="K9" s="1" t="s">
+      <c r="K9" t="s">
         <v>19</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="10" customHeight="1" ht="18.75">
-      <c r="A10" s="1" t="s">
+    <row r="10" spans="1:11" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
         <v>30</v>
       </c>
-      <c r="B10" s="1" t="s">
+      <c r="B10" t="s">
         <v>42</v>
       </c>
-      <c r="C10" s="1" t="s">
+      <c r="C10" t="s">
         <v>43</v>
       </c>
-      <c r="D10" s="1" t="s">
+      <c r="D10" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="E10" s="1" t="s">
+      <c r="E10" t="s">
         <v>44</v>
       </c>
-      <c r="F10" s="1" t="s">
+      <c r="F10" t="s">
         <v>45</v>
       </c>
-      <c r="G10" s="2">
+      <c r="G10" s="1">
         <v>12</v>
       </c>
-      <c r="H10" s="2">
+      <c r="H10" s="1">
         <v>999</v>
       </c>
-      <c r="I10" s="1" t="s">
+      <c r="I10" t="s">
         <v>24</v>
       </c>
-      <c r="J10" s="1" t="s">
+      <c r="J10" t="s">
         <v>25</v>
       </c>
-      <c r="K10" s="1" t="s">
+      <c r="K10" t="s">
         <v>43</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="11" customHeight="1" ht="18.75">
-      <c r="A11" s="1" t="s">
+    <row r="11" spans="1:11" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
         <v>30</v>
       </c>
-      <c r="B11" s="1" t="s">
+      <c r="B11" t="s">
         <v>46</v>
       </c>
-      <c r="C11" s="1" t="s">
+      <c r="C11" t="s">
         <v>47</v>
       </c>
-      <c r="D11" s="1" t="s">
+      <c r="D11" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="E11" s="1" t="s">
+      <c r="E11" t="s">
         <v>48</v>
       </c>
-      <c r="F11" s="1" t="s">
+      <c r="F11" t="s">
         <v>49</v>
       </c>
-      <c r="G11" s="2">
+      <c r="G11" s="1">
         <v>25</v>
       </c>
-      <c r="H11" s="2">
+      <c r="H11" s="1">
         <v>3333</v>
       </c>
-      <c r="I11" s="1" t="s">
+      <c r="I11" t="s">
         <v>24</v>
       </c>
-      <c r="J11" s="1" t="s">
+      <c r="J11" t="s">
         <v>50</v>
       </c>
-      <c r="K11" s="1" t="s">
+      <c r="K11" t="s">
         <v>43</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="12" customHeight="1" ht="18.75">
-      <c r="A12" s="1" t="s">
+    <row r="12" spans="1:11" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
         <v>30</v>
       </c>
-      <c r="B12" s="1" t="s">
+      <c r="B12" t="s">
         <v>51</v>
       </c>
-      <c r="C12" s="1" t="s">
+      <c r="C12" t="s">
         <v>52</v>
       </c>
-      <c r="D12" s="1" t="s">
+      <c r="D12" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="E12" s="1" t="s">
+      <c r="E12" t="s">
         <v>52</v>
       </c>
-      <c r="F12" s="1" t="s">
+      <c r="F12" t="s">
         <v>52</v>
       </c>
-      <c r="G12" s="2">
+      <c r="G12" s="1">
         <v>2</v>
       </c>
-      <c r="H12" s="2">
+      <c r="H12" s="1">
         <v>42</v>
       </c>
-      <c r="I12" s="1" t="s">
+      <c r="I12" t="s">
         <v>17</v>
       </c>
-      <c r="J12" s="1" t="s">
+      <c r="J12" t="s">
         <v>53</v>
       </c>
-      <c r="K12" s="1" t="s">
+      <c r="K12" t="s">
         <v>52</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Fixed the dialog window in PrevSO() - added uneditable fields
</commit_message>
<xml_diff>
--- a/SO_Test.xlsx
+++ b/SO_Test.xlsx
@@ -450,7 +450,7 @@
       <selection activeCell="F22" sqref="F22"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15" outlineLevelCol="0"/>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <cols>
     <col width="13.5703125" bestFit="1" customWidth="1" min="1" max="1"/>
     <col width="16.28515625" bestFit="1" customWidth="1" min="2" max="2"/>
@@ -642,7 +642,7 @@
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t>Ashley Baker</t>
+          <t>Ashley Bake</t>
         </is>
       </c>
       <c r="D5" s="5" t="inlineStr">
@@ -660,11 +660,15 @@
           <t>Siamese Dream</t>
         </is>
       </c>
-      <c r="G5" s="2" t="n">
-        <v>55</v>
-      </c>
-      <c r="H5" s="3" t="n">
-        <v>120.99</v>
+      <c r="G5" s="2" t="inlineStr">
+        <is>
+          <t>55.0</t>
+        </is>
+      </c>
+      <c r="H5" s="3" t="inlineStr">
+        <is>
+          <t>120.99</t>
+        </is>
       </c>
       <c r="I5" t="inlineStr">
         <is>
@@ -805,7 +809,7 @@
       </c>
       <c r="C9" t="inlineStr">
         <is>
-          <t>Ashley</t>
+          <t>AshleyB</t>
         </is>
       </c>
       <c r="D9" s="5" t="inlineStr">
@@ -823,11 +827,15 @@
           <t>EH</t>
         </is>
       </c>
-      <c r="G9" s="1" t="n">
-        <v>15</v>
-      </c>
-      <c r="H9" s="1" t="n">
-        <v>74</v>
+      <c r="G9" s="1" t="inlineStr">
+        <is>
+          <t>15.0</t>
+        </is>
+      </c>
+      <c r="H9" s="1" t="inlineStr">
+        <is>
+          <t>74.0</t>
+        </is>
       </c>
       <c r="I9" t="inlineStr">
         <is>

</xml_diff>

<commit_message>
main.py modified but still not working
</commit_message>
<xml_diff>
--- a/SO_Test.xlsx
+++ b/SO_Test.xlsx
@@ -464,13 +464,13 @@
     <outlinePr summaryBelow="0"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:AR16"/>
+  <dimension ref="A1:AR18"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15" outlineLevelCol="0"/>
   <cols>
     <col width="13.57642857142857" bestFit="1" customWidth="1" style="9" min="1" max="1"/>
     <col width="16.29071428571428" bestFit="1" customWidth="1" style="9" min="2" max="2"/>
@@ -1784,6 +1784,64 @@
       <c r="AQ16" s="9" t="n"/>
       <c r="AR16" s="9" t="n"/>
     </row>
+    <row r="18">
+      <c r="A18" t="inlineStr">
+        <is>
+          <t>02/14/2024</t>
+        </is>
+      </c>
+      <c r="B18" t="inlineStr">
+        <is>
+          <t>SO240214001</t>
+        </is>
+      </c>
+      <c r="C18" t="inlineStr">
+        <is>
+          <t>AB</t>
+        </is>
+      </c>
+      <c r="D18" t="inlineStr">
+        <is>
+          <t>9999999999</t>
+        </is>
+      </c>
+      <c r="E18" t="inlineStr">
+        <is>
+          <t>ARTIST</t>
+        </is>
+      </c>
+      <c r="F18" t="inlineStr">
+        <is>
+          <t>TITLE</t>
+        </is>
+      </c>
+      <c r="G18" t="n">
+        <v>5</v>
+      </c>
+      <c r="H18" t="n">
+        <v>50</v>
+      </c>
+      <c r="I18" t="inlineStr">
+        <is>
+          <t>AEC</t>
+        </is>
+      </c>
+      <c r="J18" t="inlineStr">
+        <is>
+          <t>LP</t>
+        </is>
+      </c>
+      <c r="K18" t="inlineStr">
+        <is>
+          <t>Ashley</t>
+        </is>
+      </c>
+      <c r="L18" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
main.py -> Prev_SO fixing shipping info entries and the horizontal scrollbar
</commit_message>
<xml_diff>
--- a/SO_Test.xlsx
+++ b/SO_Test.xlsx
@@ -1417,39 +1417,43 @@
     <row r="12" ht="19.5" customHeight="1">
       <c r="A12" s="9" t="inlineStr">
         <is>
-          <t>01/12/2024</t>
+          <t>02/14/2024</t>
         </is>
       </c>
       <c r="B12" s="9" t="inlineStr">
         <is>
-          <t>SO240112006</t>
+          <t>SO240214001</t>
         </is>
       </c>
       <c r="C12" s="9" t="inlineStr">
         <is>
-          <t>a</t>
+          <t>AB</t>
         </is>
       </c>
       <c r="D12" s="2" t="inlineStr">
         <is>
-          <t>9157994875</t>
+          <t>9999999999</t>
         </is>
       </c>
       <c r="E12" s="9" t="inlineStr">
         <is>
-          <t>a</t>
+          <t>ARTIST</t>
         </is>
       </c>
       <c r="F12" s="9" t="inlineStr">
         <is>
-          <t>a</t>
-        </is>
-      </c>
-      <c r="G12" s="3" t="n">
-        <v>2</v>
-      </c>
-      <c r="H12" s="3" t="n">
-        <v>42</v>
+          <t>TITLE</t>
+        </is>
+      </c>
+      <c r="G12" s="3" t="inlineStr">
+        <is>
+          <t>5.0</t>
+        </is>
+      </c>
+      <c r="H12" s="3" t="inlineStr">
+        <is>
+          <t>50.0</t>
+        </is>
       </c>
       <c r="I12" s="9" t="inlineStr">
         <is>
@@ -1458,19 +1462,39 @@
       </c>
       <c r="J12" s="9" t="inlineStr">
         <is>
-          <t>OTHER</t>
+          <t>LP</t>
         </is>
       </c>
       <c r="K12" s="9" t="inlineStr">
         <is>
-          <t>a</t>
-        </is>
-      </c>
-      <c r="L12" s="9" t="n"/>
-      <c r="M12" s="9" t="n"/>
-      <c r="N12" s="9" t="n"/>
-      <c r="O12" s="9" t="n"/>
-      <c r="P12" s="9" t="n"/>
+          <t>Ashley</t>
+        </is>
+      </c>
+      <c r="L12" s="9" t="inlineStr">
+        <is>
+          <t>YES</t>
+        </is>
+      </c>
+      <c r="M12" s="9" t="inlineStr">
+        <is>
+          <t>test</t>
+        </is>
+      </c>
+      <c r="N12" s="9" t="inlineStr">
+        <is>
+          <t>test</t>
+        </is>
+      </c>
+      <c r="O12" s="9" t="inlineStr">
+        <is>
+          <t>te</t>
+        </is>
+      </c>
+      <c r="P12" s="9" t="inlineStr">
+        <is>
+          <t>79935</t>
+        </is>
+      </c>
       <c r="Q12" s="9" t="n"/>
       <c r="R12" s="9" t="n"/>
       <c r="S12" s="9" t="n"/>

</xml_diff>

<commit_message>
main.py > Prev_SO save() issue is now fixed I might change the SHIPPING? switch to a checkbox
</commit_message>
<xml_diff>
--- a/SO_Test.xlsx
+++ b/SO_Test.xlsx
@@ -1553,22 +1553,86 @@
       <c r="AR13" s="10" t="n"/>
     </row>
     <row r="14" ht="18.75" customHeight="1">
-      <c r="A14" s="10" t="n"/>
-      <c r="B14" s="10" t="n"/>
-      <c r="C14" s="10" t="n"/>
-      <c r="D14" s="4" t="n"/>
-      <c r="E14" s="10" t="n"/>
-      <c r="F14" s="10" t="n"/>
-      <c r="G14" s="4" t="n"/>
-      <c r="H14" s="4" t="n"/>
-      <c r="I14" s="10" t="n"/>
-      <c r="J14" s="10" t="n"/>
-      <c r="K14" s="10" t="n"/>
-      <c r="L14" s="10" t="n"/>
-      <c r="M14" s="10" t="n"/>
-      <c r="N14" s="10" t="n"/>
-      <c r="O14" s="10" t="n"/>
-      <c r="P14" s="10" t="n"/>
+      <c r="A14" s="10" t="inlineStr">
+        <is>
+          <t>02/05/2024</t>
+        </is>
+      </c>
+      <c r="B14" s="10" t="inlineStr">
+        <is>
+          <t>SO240205001</t>
+        </is>
+      </c>
+      <c r="C14" s="10" t="inlineStr">
+        <is>
+          <t>a</t>
+        </is>
+      </c>
+      <c r="D14" s="4" t="inlineStr">
+        <is>
+          <t>7539514563</t>
+        </is>
+      </c>
+      <c r="E14" s="10" t="inlineStr">
+        <is>
+          <t>a</t>
+        </is>
+      </c>
+      <c r="F14" s="10" t="inlineStr">
+        <is>
+          <t>a</t>
+        </is>
+      </c>
+      <c r="G14" s="4" t="inlineStr">
+        <is>
+          <t>20.0</t>
+        </is>
+      </c>
+      <c r="H14" s="4" t="inlineStr">
+        <is>
+          <t>50.0</t>
+        </is>
+      </c>
+      <c r="I14" s="10" t="inlineStr">
+        <is>
+          <t>AMS</t>
+        </is>
+      </c>
+      <c r="J14" s="10" t="inlineStr">
+        <is>
+          <t>DVD</t>
+        </is>
+      </c>
+      <c r="K14" s="10" t="inlineStr">
+        <is>
+          <t>Ashley</t>
+        </is>
+      </c>
+      <c r="L14" s="10" t="inlineStr">
+        <is>
+          <t>YES</t>
+        </is>
+      </c>
+      <c r="M14" s="10" t="inlineStr">
+        <is>
+          <t>1234 Address</t>
+        </is>
+      </c>
+      <c r="N14" s="10" t="inlineStr">
+        <is>
+          <t>CITY</t>
+        </is>
+      </c>
+      <c r="O14" s="10" t="inlineStr">
+        <is>
+          <t>TX</t>
+        </is>
+      </c>
+      <c r="P14" s="10" t="inlineStr">
+        <is>
+          <t>79935</t>
+        </is>
+      </c>
       <c r="Q14" s="10" t="n"/>
       <c r="R14" s="10" t="n"/>
       <c r="S14" s="10" t="n"/>
@@ -1705,22 +1769,82 @@
       <c r="AR15" s="10" t="n"/>
     </row>
     <row r="16" ht="18.75" customHeight="1">
-      <c r="A16" s="10" t="n"/>
-      <c r="B16" s="10" t="n"/>
-      <c r="C16" s="10" t="n"/>
-      <c r="D16" s="11" t="n"/>
-      <c r="E16" s="10" t="n"/>
-      <c r="F16" s="10" t="n"/>
-      <c r="G16" s="12" t="n"/>
-      <c r="H16" s="12" t="n"/>
-      <c r="I16" s="10" t="n"/>
-      <c r="J16" s="10" t="n"/>
-      <c r="K16" s="10" t="n"/>
-      <c r="L16" s="10" t="n"/>
-      <c r="M16" s="10" t="n"/>
-      <c r="N16" s="10" t="n"/>
-      <c r="O16" s="10" t="n"/>
-      <c r="P16" s="10" t="n"/>
+      <c r="A16" s="10" t="inlineStr">
+        <is>
+          <t>02/14/2024</t>
+        </is>
+      </c>
+      <c r="B16" s="10" t="inlineStr">
+        <is>
+          <t>SO240214001</t>
+        </is>
+      </c>
+      <c r="C16" s="10" t="inlineStr">
+        <is>
+          <t>AB</t>
+        </is>
+      </c>
+      <c r="D16" s="11" t="inlineStr">
+        <is>
+          <t>9999999999</t>
+        </is>
+      </c>
+      <c r="E16" s="10" t="inlineStr">
+        <is>
+          <t>ARTIST</t>
+        </is>
+      </c>
+      <c r="F16" s="10" t="inlineStr">
+        <is>
+          <t>TITLE</t>
+        </is>
+      </c>
+      <c r="G16" s="12" t="n">
+        <v>0</v>
+      </c>
+      <c r="H16" s="12" t="n">
+        <v>0</v>
+      </c>
+      <c r="I16" s="10" t="inlineStr">
+        <is>
+          <t>AEC</t>
+        </is>
+      </c>
+      <c r="J16" s="10" t="inlineStr">
+        <is>
+          <t>LP</t>
+        </is>
+      </c>
+      <c r="K16" s="10" t="inlineStr">
+        <is>
+          <t>Ashley</t>
+        </is>
+      </c>
+      <c r="L16" s="10" t="inlineStr">
+        <is>
+          <t>YES</t>
+        </is>
+      </c>
+      <c r="M16" s="10" t="inlineStr">
+        <is>
+          <t>1234 test address</t>
+        </is>
+      </c>
+      <c r="N16" s="10" t="inlineStr">
+        <is>
+          <t>city</t>
+        </is>
+      </c>
+      <c r="O16" s="10" t="inlineStr">
+        <is>
+          <t>tx</t>
+        </is>
+      </c>
+      <c r="P16" s="10" t="inlineStr">
+        <is>
+          <t>79935</t>
+        </is>
+      </c>
       <c r="Q16" s="10" t="n"/>
       <c r="R16" s="10" t="n"/>
       <c r="S16" s="10" t="n"/>

</xml_diff>

<commit_message>
Modified main.py > Prev_SO and SO_App
Now newly submitted SO forms will be displayed in the Previous Special Orders frame right after they are created
</commit_message>
<xml_diff>
--- a/SO_Test.xlsx
+++ b/SO_Test.xlsx
@@ -443,13 +443,13 @@
     <outlinePr summaryBelow="0"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:P2"/>
+  <dimension ref="A1:P4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15" outlineLevelCol="0"/>
   <cols>
     <col width="13.57642857142857" bestFit="1" customWidth="1" style="4" min="1" max="1"/>
     <col width="16.29071428571428" bestFit="1" customWidth="1" style="4" min="2" max="2"/>
@@ -608,7 +608,83 @@
           <t>NO</t>
         </is>
       </c>
-      <c r="M2" t="inlineStr"/>
+    </row>
+    <row r="3">
+      <c r="A3" t="inlineStr"/>
+      <c r="B3" t="inlineStr"/>
+      <c r="C3" t="inlineStr"/>
+      <c r="D3" t="inlineStr"/>
+      <c r="E3" t="inlineStr"/>
+      <c r="F3" t="inlineStr"/>
+      <c r="G3" t="inlineStr"/>
+      <c r="H3" t="inlineStr"/>
+      <c r="I3" t="inlineStr"/>
+      <c r="J3" t="inlineStr"/>
+      <c r="K3" t="inlineStr"/>
+      <c r="L3" t="inlineStr"/>
+      <c r="M3" t="inlineStr"/>
+      <c r="N3" t="inlineStr"/>
+      <c r="O3" t="inlineStr"/>
+      <c r="P3" t="inlineStr"/>
+    </row>
+    <row r="4">
+      <c r="A4" t="inlineStr">
+        <is>
+          <t>02/19/2024</t>
+        </is>
+      </c>
+      <c r="B4" t="inlineStr">
+        <is>
+          <t>SO240219001</t>
+        </is>
+      </c>
+      <c r="C4" t="inlineStr">
+        <is>
+          <t>ab</t>
+        </is>
+      </c>
+      <c r="D4" t="inlineStr">
+        <is>
+          <t>7894561230</t>
+        </is>
+      </c>
+      <c r="E4" t="inlineStr">
+        <is>
+          <t>a</t>
+        </is>
+      </c>
+      <c r="F4" t="inlineStr">
+        <is>
+          <t>a</t>
+        </is>
+      </c>
+      <c r="G4" t="n">
+        <v>12</v>
+      </c>
+      <c r="H4" t="n">
+        <v>34</v>
+      </c>
+      <c r="I4" t="inlineStr">
+        <is>
+          <t>AMA</t>
+        </is>
+      </c>
+      <c r="J4" t="inlineStr">
+        <is>
+          <t>OTHER</t>
+        </is>
+      </c>
+      <c r="K4" t="inlineStr">
+        <is>
+          <t>ab</t>
+        </is>
+      </c>
+      <c r="L4" t="inlineStr">
+        <is>
+          <t>NO</t>
+        </is>
+      </c>
+      <c r="M4" t="inlineStr"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
position modified in main and ai_project_frame_test
</commit_message>
<xml_diff>
--- a/SO_Test.xlsx
+++ b/SO_Test.xlsx
@@ -443,13 +443,13 @@
     <outlinePr summaryBelow="0"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:P4"/>
+  <dimension ref="A1:P5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15" outlineLevelCol="0"/>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <cols>
     <col width="13.57642857142857" bestFit="1" customWidth="1" style="4" min="1" max="1"/>
     <col width="16.29071428571428" bestFit="1" customWidth="1" style="4" min="2" max="2"/>
@@ -609,24 +609,7 @@
         </is>
       </c>
     </row>
-    <row r="3">
-      <c r="A3" t="inlineStr"/>
-      <c r="B3" t="inlineStr"/>
-      <c r="C3" t="inlineStr"/>
-      <c r="D3" t="inlineStr"/>
-      <c r="E3" t="inlineStr"/>
-      <c r="F3" t="inlineStr"/>
-      <c r="G3" t="inlineStr"/>
-      <c r="H3" t="inlineStr"/>
-      <c r="I3" t="inlineStr"/>
-      <c r="J3" t="inlineStr"/>
-      <c r="K3" t="inlineStr"/>
-      <c r="L3" t="inlineStr"/>
-      <c r="M3" t="inlineStr"/>
-      <c r="N3" t="inlineStr"/>
-      <c r="O3" t="inlineStr"/>
-      <c r="P3" t="inlineStr"/>
-    </row>
+    <row r="3"/>
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
@@ -684,7 +667,84 @@
           <t>NO</t>
         </is>
       </c>
-      <c r="M4" t="inlineStr"/>
+    </row>
+    <row r="5">
+      <c r="A5" t="inlineStr">
+        <is>
+          <t>02/19/2024</t>
+        </is>
+      </c>
+      <c r="B5" t="inlineStr">
+        <is>
+          <t>SO240219002</t>
+        </is>
+      </c>
+      <c r="C5" t="inlineStr">
+        <is>
+          <t>Me</t>
+        </is>
+      </c>
+      <c r="D5" t="inlineStr">
+        <is>
+          <t>5555555555</t>
+        </is>
+      </c>
+      <c r="E5" t="inlineStr">
+        <is>
+          <t>Type O Negative</t>
+        </is>
+      </c>
+      <c r="F5" t="inlineStr">
+        <is>
+          <t>Bloody Kisses</t>
+        </is>
+      </c>
+      <c r="G5" t="n">
+        <v>5</v>
+      </c>
+      <c r="H5" t="n">
+        <v>49.99</v>
+      </c>
+      <c r="I5" t="inlineStr">
+        <is>
+          <t>AMS</t>
+        </is>
+      </c>
+      <c r="J5" t="inlineStr">
+        <is>
+          <t>DVD</t>
+        </is>
+      </c>
+      <c r="K5" t="inlineStr">
+        <is>
+          <t>MTP</t>
+        </is>
+      </c>
+      <c r="L5" t="inlineStr">
+        <is>
+          <t>YES</t>
+        </is>
+      </c>
+      <c r="M5" t="inlineStr">
+        <is>
+          <t>59848</t>
+        </is>
+      </c>
+      <c r="N5" t="inlineStr">
+        <is>
+          <t>gh</t>
+        </is>
+      </c>
+      <c r="O5" t="inlineStr">
+        <is>
+          <t>hg</t>
+        </is>
+      </c>
+      <c r="P5" t="inlineStr">
+        <is>
+          <t>77777</t>
+        </is>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
modified CTK's json file to have red color
</commit_message>
<xml_diff>
--- a/SO_Test.xlsx
+++ b/SO_Test.xlsx
@@ -449,7 +449,7 @@
       <selection activeCell="A1" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15" outlineLevelCol="0"/>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <cols>
     <col width="13.57642857142857" bestFit="1" customWidth="1" style="4" min="1" max="1"/>
     <col width="16.29071428571428" bestFit="1" customWidth="1" style="4" min="2" max="2"/>
@@ -609,7 +609,6 @@
         </is>
       </c>
     </row>
-    <row r="3"/>
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
@@ -722,12 +721,12 @@
       </c>
       <c r="L5" t="inlineStr">
         <is>
-          <t>YES</t>
+          <t>NO</t>
         </is>
       </c>
       <c r="M5" t="inlineStr">
         <is>
-          <t>59848</t>
+          <t>59848.0</t>
         </is>
       </c>
       <c r="N5" t="inlineStr">
@@ -746,24 +745,7 @@
         </is>
       </c>
     </row>
-    <row r="6">
-      <c r="A6" t="inlineStr"/>
-      <c r="B6" t="inlineStr"/>
-      <c r="C6" t="inlineStr"/>
-      <c r="D6" t="inlineStr"/>
-      <c r="E6" t="inlineStr"/>
-      <c r="F6" t="inlineStr"/>
-      <c r="G6" t="inlineStr"/>
-      <c r="H6" t="inlineStr"/>
-      <c r="I6" t="inlineStr"/>
-      <c r="J6" t="inlineStr"/>
-      <c r="K6" t="inlineStr"/>
-      <c r="L6" t="inlineStr"/>
-      <c r="M6" t="inlineStr"/>
-      <c r="N6" t="inlineStr"/>
-      <c r="O6" t="inlineStr"/>
-      <c r="P6" t="inlineStr"/>
-    </row>
+    <row r="6"/>
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
@@ -821,7 +803,6 @@
           <t>NO</t>
         </is>
       </c>
-      <c r="M7" t="inlineStr"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Minor midifications to reconciliation form
</commit_message>
<xml_diff>
--- a/SO_Test.xlsx
+++ b/SO_Test.xlsx
@@ -443,13 +443,13 @@
     <outlinePr summaryBelow="0"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:P7"/>
+  <dimension ref="A1:P9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15" outlineLevelCol="0"/>
   <cols>
     <col width="13.57642857142857" bestFit="1" customWidth="1" style="4" min="1" max="1"/>
     <col width="16.29071428571428" bestFit="1" customWidth="1" style="4" min="2" max="2"/>
@@ -609,6 +609,7 @@
         </is>
       </c>
     </row>
+    <row r="3"/>
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
@@ -803,6 +804,79 @@
           <t>NO</t>
         </is>
       </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="inlineStr"/>
+      <c r="B8" t="inlineStr"/>
+      <c r="C8" t="inlineStr"/>
+      <c r="D8" t="inlineStr"/>
+      <c r="E8" t="inlineStr"/>
+      <c r="F8" t="inlineStr"/>
+      <c r="G8" t="inlineStr"/>
+      <c r="H8" t="inlineStr"/>
+      <c r="I8" t="inlineStr"/>
+      <c r="J8" t="inlineStr"/>
+      <c r="K8" t="inlineStr"/>
+      <c r="L8" t="inlineStr"/>
+      <c r="M8" t="inlineStr"/>
+      <c r="N8" t="inlineStr"/>
+      <c r="O8" t="inlineStr"/>
+      <c r="P8" t="inlineStr"/>
+    </row>
+    <row r="9">
+      <c r="A9" t="inlineStr">
+        <is>
+          <t>03/05/2024</t>
+        </is>
+      </c>
+      <c r="B9" t="inlineStr">
+        <is>
+          <t>SO240305001</t>
+        </is>
+      </c>
+      <c r="C9" t="inlineStr">
+        <is>
+          <t>asshley</t>
+        </is>
+      </c>
+      <c r="D9" t="inlineStr">
+        <is>
+          <t>5642858215</t>
+        </is>
+      </c>
+      <c r="E9" t="inlineStr">
+        <is>
+          <t>artist</t>
+        </is>
+      </c>
+      <c r="F9" t="inlineStr">
+        <is>
+          <t>title</t>
+        </is>
+      </c>
+      <c r="G9" t="n">
+        <v>50</v>
+      </c>
+      <c r="H9" t="n">
+        <v>58.63</v>
+      </c>
+      <c r="I9" t="inlineStr">
+        <is>
+          <t>AMS</t>
+        </is>
+      </c>
+      <c r="J9" t="inlineStr">
+        <is>
+          <t>LP</t>
+        </is>
+      </c>
+      <c r="K9" t="inlineStr"/>
+      <c r="L9" t="inlineStr">
+        <is>
+          <t>NO</t>
+        </is>
+      </c>
+      <c r="M9" t="inlineStr"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Modified main.py changed the phone number formatting so the phone number formats automatically in the SO_FORM after inputting 10 digits Also added new columns for text/call confirmations and added their corresponding widgets in the SO_FORM as well as in the Prev_SO's edit window
</commit_message>
<xml_diff>
--- a/SO_Test.xlsx
+++ b/SO_Test.xlsx
@@ -16,7 +16,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="0"/>
-  <fonts count="2">
+  <fonts count="3">
     <font>
       <name val="Calibri"/>
       <family val="2"/>
@@ -28,6 +28,12 @@
       <name val="Calibri"/>
       <family val="2"/>
       <color rgb="FF000000"/>
+      <sz val="11"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <color theme="1"/>
       <sz val="11"/>
     </font>
   </fonts>
@@ -58,21 +64,27 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="general"/>
     </xf>
-    <xf numFmtId="49" fontId="1" fillId="0" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="3" fontId="1" fillId="0" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="right"/>
     </xf>
+    <xf numFmtId="3" fontId="2" fillId="0" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="3" fontId="0" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="4" fontId="2" fillId="0" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="right"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="general"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="general"/>
     </xf>
     <xf numFmtId="3" fontId="0" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
@@ -443,44 +455,47 @@
     <outlinePr summaryBelow="0"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:P9"/>
+  <dimension ref="A1:S12"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15" outlineLevelCol="0"/>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <cols>
-    <col width="13.57642857142857" bestFit="1" customWidth="1" style="4" min="1" max="1"/>
-    <col width="16.29071428571428" bestFit="1" customWidth="1" style="4" min="2" max="2"/>
-    <col width="14.57642857142857" bestFit="1" customWidth="1" style="4" min="3" max="3"/>
-    <col width="13.57642857142857" bestFit="1" customWidth="1" style="5" min="4" max="4"/>
-    <col width="13.57642857142857" bestFit="1" customWidth="1" style="4" min="5" max="5"/>
-    <col width="13.57642857142857" bestFit="1" customWidth="1" style="4" min="6" max="6"/>
-    <col width="13.57642857142857" bestFit="1" customWidth="1" style="6" min="7" max="7"/>
-    <col width="13.57642857142857" bestFit="1" customWidth="1" style="6" min="8" max="8"/>
-    <col width="13.57642857142857" bestFit="1" customWidth="1" style="4" min="9" max="9"/>
-    <col width="13.57642857142857" bestFit="1" customWidth="1" style="4" min="10" max="10"/>
-    <col width="13.57642857142857" bestFit="1" customWidth="1" style="4" min="11" max="11"/>
-    <col width="13.57642857142857" bestFit="1" customWidth="1" style="4" min="12" max="12"/>
-    <col width="13.57642857142857" bestFit="1" customWidth="1" style="4" min="13" max="13"/>
-    <col width="13.57642857142857" bestFit="1" customWidth="1" style="4" min="14" max="14"/>
-    <col width="13.57642857142857" bestFit="1" customWidth="1" style="4" min="15" max="15"/>
-    <col width="19.43357142857143" bestFit="1" customWidth="1" style="4" min="16" max="16"/>
+    <col width="13.57642857142857" bestFit="1" customWidth="1" style="7" min="1" max="1"/>
+    <col width="16.29071428571428" bestFit="1" customWidth="1" style="7" min="2" max="2"/>
+    <col width="14.57642857142857" bestFit="1" customWidth="1" style="7" min="3" max="3"/>
+    <col width="13.57642857142857" bestFit="1" customWidth="1" style="7" min="4" max="4"/>
+    <col width="13.57642857142857" bestFit="1" customWidth="1" style="7" min="5" max="5"/>
+    <col width="13.57642857142857" bestFit="1" customWidth="1" style="7" min="6" max="6"/>
+    <col width="13.57642857142857" bestFit="1" customWidth="1" style="7" min="7" max="7"/>
+    <col width="13.57642857142857" bestFit="1" customWidth="1" style="7" min="8" max="8"/>
+    <col width="13.57642857142857" bestFit="1" customWidth="1" style="8" min="9" max="9"/>
+    <col width="13.57642857142857" bestFit="1" customWidth="1" style="8" min="10" max="10"/>
+    <col width="13.57642857142857" bestFit="1" customWidth="1" style="7" min="11" max="11"/>
+    <col width="13.57642857142857" bestFit="1" customWidth="1" style="7" min="12" max="12"/>
+    <col width="13.57642857142857" bestFit="1" customWidth="1" style="7" min="13" max="13"/>
+    <col width="13.57642857142857" bestFit="1" customWidth="1" style="7" min="14" max="14"/>
+    <col width="13.57642857142857" bestFit="1" customWidth="1" style="7" min="15" max="15"/>
+    <col width="13.57642857142857" bestFit="1" customWidth="1" style="7" min="16" max="16"/>
+    <col width="13.57642857142857" bestFit="1" customWidth="1" style="7" min="17" max="17"/>
+    <col width="13.57642857142857" bestFit="1" customWidth="1" style="7" min="18" max="18"/>
+    <col width="19.43357142857143" bestFit="1" customWidth="1" style="7" min="19" max="19"/>
   </cols>
   <sheetData>
     <row r="1" ht="19.5" customHeight="1">
-      <c r="A1" s="4" t="inlineStr">
+      <c r="A1" s="7" t="inlineStr">
         <is>
           <t>DATE</t>
         </is>
       </c>
-      <c r="B1" s="4" t="inlineStr">
+      <c r="B1" s="7" t="inlineStr">
         <is>
           <t>REF NUM</t>
         </is>
       </c>
-      <c r="C1" s="4" t="inlineStr">
+      <c r="C1" s="7" t="inlineStr">
         <is>
           <t>CX NAME</t>
         </is>
@@ -490,393 +505,644 @@
           <t>PHONE</t>
         </is>
       </c>
-      <c r="E1" s="4" t="inlineStr">
+      <c r="E1" s="7" t="inlineStr">
+        <is>
+          <t>TEXT?</t>
+        </is>
+      </c>
+      <c r="F1" s="7" t="inlineStr">
+        <is>
+          <t>CALL?</t>
+        </is>
+      </c>
+      <c r="G1" s="7" t="inlineStr">
         <is>
           <t>ARTIST</t>
         </is>
       </c>
-      <c r="F1" s="4" t="inlineStr">
+      <c r="H1" s="7" t="inlineStr">
         <is>
           <t>TITLE</t>
         </is>
       </c>
-      <c r="G1" s="3" t="inlineStr">
+      <c r="I1" s="3" t="inlineStr">
         <is>
           <t>DEPOSIT</t>
         </is>
       </c>
-      <c r="H1" s="3" t="inlineStr">
-        <is>
-          <t>PRICE</t>
-        </is>
-      </c>
-      <c r="I1" s="4" t="inlineStr">
+      <c r="J1" s="3" t="inlineStr">
+        <is>
+          <t>RETAIL</t>
+        </is>
+      </c>
+      <c r="K1" s="7" t="inlineStr">
+        <is>
+          <t>COG</t>
+        </is>
+      </c>
+      <c r="L1" s="7" t="inlineStr">
         <is>
           <t>VENDOR</t>
         </is>
       </c>
-      <c r="J1" s="4" t="inlineStr">
+      <c r="M1" s="7" t="inlineStr">
         <is>
           <t>TYPE</t>
         </is>
       </c>
-      <c r="K1" s="4" t="inlineStr">
+      <c r="N1" s="7" t="inlineStr">
         <is>
           <t>CLERK NAME</t>
         </is>
       </c>
-      <c r="L1" s="4" t="inlineStr">
+      <c r="O1" s="7" t="inlineStr">
         <is>
           <t>SHIPPING?</t>
         </is>
       </c>
-      <c r="M1" s="4" t="inlineStr">
+      <c r="P1" s="7" t="inlineStr">
         <is>
           <t>ADDRESS</t>
         </is>
       </c>
-      <c r="N1" s="4" t="inlineStr">
+      <c r="Q1" s="7" t="inlineStr">
         <is>
           <t>CITY</t>
         </is>
       </c>
-      <c r="O1" s="4" t="inlineStr">
+      <c r="R1" s="7" t="inlineStr">
         <is>
           <t>STATE</t>
         </is>
       </c>
-      <c r="P1" s="4" t="inlineStr">
+      <c r="S1" s="7" t="inlineStr">
         <is>
           <t>ZIPCODE</t>
         </is>
       </c>
     </row>
-    <row r="2">
-      <c r="A2" t="inlineStr">
+    <row r="2" ht="18.75" customHeight="1">
+      <c r="A2" s="7" t="inlineStr">
         <is>
           <t>02/18/2024</t>
         </is>
       </c>
-      <c r="B2" t="inlineStr">
+      <c r="B2" s="7" t="inlineStr">
         <is>
           <t>SO240218001</t>
         </is>
       </c>
-      <c r="C2" t="inlineStr">
+      <c r="C2" s="7" t="inlineStr">
         <is>
           <t>ab</t>
         </is>
       </c>
-      <c r="D2" t="inlineStr">
+      <c r="D2" s="7" t="inlineStr">
         <is>
           <t>7894561230</t>
         </is>
       </c>
-      <c r="E2" t="inlineStr">
+      <c r="E2" s="7" t="n"/>
+      <c r="F2" s="7" t="n"/>
+      <c r="G2" s="7" t="inlineStr">
         <is>
           <t>ab</t>
         </is>
       </c>
-      <c r="F2" t="inlineStr">
+      <c r="H2" s="7" t="inlineStr">
         <is>
           <t>ab</t>
         </is>
       </c>
-      <c r="G2" t="n">
+      <c r="I2" s="4" t="n">
         <v>12</v>
       </c>
-      <c r="H2" t="n">
+      <c r="J2" s="4" t="n">
         <v>24</v>
       </c>
-      <c r="I2" t="inlineStr">
+      <c r="K2" s="7" t="n"/>
+      <c r="L2" s="7" t="inlineStr">
         <is>
           <t>Vendors</t>
         </is>
       </c>
-      <c r="J2" t="inlineStr">
+      <c r="M2" s="7" t="inlineStr">
         <is>
           <t>DVD</t>
         </is>
       </c>
-      <c r="K2" t="inlineStr">
+      <c r="N2" s="7" t="inlineStr">
         <is>
           <t>ab</t>
         </is>
       </c>
-      <c r="L2" t="inlineStr">
+      <c r="O2" s="7" t="inlineStr">
         <is>
           <t>NO</t>
         </is>
       </c>
+      <c r="P2" s="7" t="n"/>
+      <c r="Q2" s="7" t="n"/>
+      <c r="R2" s="7" t="n"/>
+      <c r="S2" s="7" t="n"/>
     </row>
-    <row r="3"/>
-    <row r="4">
-      <c r="A4" t="inlineStr">
+    <row r="3" ht="18.75" customHeight="1">
+      <c r="A3" s="7" t="n"/>
+      <c r="B3" s="7" t="n"/>
+      <c r="C3" s="7" t="n"/>
+      <c r="D3" s="7" t="n"/>
+      <c r="E3" s="7" t="n"/>
+      <c r="F3" s="7" t="n"/>
+      <c r="G3" s="7" t="n"/>
+      <c r="H3" s="7" t="n"/>
+      <c r="I3" s="8" t="n"/>
+      <c r="J3" s="8" t="n"/>
+      <c r="K3" s="7" t="n"/>
+      <c r="L3" s="7" t="n"/>
+      <c r="M3" s="7" t="n"/>
+      <c r="N3" s="7" t="n"/>
+      <c r="O3" s="7" t="n"/>
+      <c r="P3" s="7" t="n"/>
+      <c r="Q3" s="7" t="n"/>
+      <c r="R3" s="7" t="n"/>
+      <c r="S3" s="7" t="n"/>
+    </row>
+    <row r="4" ht="18.75" customHeight="1">
+      <c r="A4" s="7" t="inlineStr">
         <is>
           <t>02/19/2024</t>
         </is>
       </c>
-      <c r="B4" t="inlineStr">
+      <c r="B4" s="7" t="inlineStr">
         <is>
           <t>SO240219001</t>
         </is>
       </c>
-      <c r="C4" t="inlineStr">
+      <c r="C4" s="7" t="inlineStr">
         <is>
           <t>ab</t>
         </is>
       </c>
-      <c r="D4" t="inlineStr">
+      <c r="D4" s="7" t="inlineStr">
         <is>
           <t>7894561230</t>
         </is>
       </c>
-      <c r="E4" t="inlineStr">
+      <c r="E4" s="7" t="n"/>
+      <c r="F4" s="7" t="n"/>
+      <c r="G4" s="7" t="inlineStr">
         <is>
           <t>a</t>
         </is>
       </c>
-      <c r="F4" t="inlineStr">
+      <c r="H4" s="7" t="inlineStr">
         <is>
           <t>a</t>
         </is>
       </c>
-      <c r="G4" t="n">
+      <c r="I4" s="4" t="n">
         <v>12</v>
       </c>
-      <c r="H4" t="n">
+      <c r="J4" s="4" t="n">
         <v>34</v>
       </c>
-      <c r="I4" t="inlineStr">
+      <c r="K4" s="7" t="n"/>
+      <c r="L4" s="7" t="inlineStr">
         <is>
           <t>AMA</t>
         </is>
       </c>
-      <c r="J4" t="inlineStr">
+      <c r="M4" s="7" t="inlineStr">
         <is>
           <t>OTHER</t>
         </is>
       </c>
-      <c r="K4" t="inlineStr">
+      <c r="N4" s="7" t="inlineStr">
         <is>
           <t>ab</t>
         </is>
       </c>
-      <c r="L4" t="inlineStr">
+      <c r="O4" s="7" t="inlineStr">
         <is>
           <t>NO</t>
         </is>
       </c>
+      <c r="P4" s="7" t="n"/>
+      <c r="Q4" s="7" t="n"/>
+      <c r="R4" s="7" t="n"/>
+      <c r="S4" s="7" t="n"/>
     </row>
-    <row r="5">
-      <c r="A5" t="inlineStr">
+    <row r="5" ht="18.75" customHeight="1">
+      <c r="A5" s="7" t="inlineStr">
         <is>
           <t>02/19/2024</t>
         </is>
       </c>
-      <c r="B5" t="inlineStr">
+      <c r="B5" s="7" t="inlineStr">
         <is>
           <t>SO240219002</t>
         </is>
       </c>
-      <c r="C5" t="inlineStr">
+      <c r="C5" s="7" t="inlineStr">
         <is>
           <t>Me</t>
         </is>
       </c>
-      <c r="D5" t="inlineStr">
+      <c r="D5" s="7" t="inlineStr">
         <is>
           <t>5555555555</t>
         </is>
       </c>
-      <c r="E5" t="inlineStr">
+      <c r="E5" s="7" t="n"/>
+      <c r="F5" s="7" t="n"/>
+      <c r="G5" s="7" t="inlineStr">
         <is>
           <t>Type O Negative</t>
         </is>
       </c>
-      <c r="F5" t="inlineStr">
+      <c r="H5" s="7" t="inlineStr">
         <is>
           <t>Bloody Kisses</t>
         </is>
       </c>
-      <c r="G5" t="n">
+      <c r="I5" s="4" t="n">
         <v>5</v>
       </c>
-      <c r="H5" t="n">
+      <c r="J5" s="6" t="n">
         <v>49.99</v>
       </c>
-      <c r="I5" t="inlineStr">
+      <c r="K5" s="7" t="n"/>
+      <c r="L5" s="7" t="inlineStr">
         <is>
           <t>AMS</t>
         </is>
       </c>
-      <c r="J5" t="inlineStr">
+      <c r="M5" s="7" t="inlineStr">
         <is>
           <t>DVD</t>
         </is>
       </c>
-      <c r="K5" t="inlineStr">
+      <c r="N5" s="7" t="inlineStr">
         <is>
           <t>MTP</t>
         </is>
       </c>
-      <c r="L5" t="inlineStr">
+      <c r="O5" s="7" t="inlineStr">
         <is>
           <t>NO</t>
         </is>
       </c>
-      <c r="M5" t="inlineStr">
+      <c r="P5" s="7" t="inlineStr">
         <is>
           <t>59848.0</t>
         </is>
       </c>
-      <c r="N5" t="inlineStr">
+      <c r="Q5" s="7" t="inlineStr">
         <is>
           <t>gh</t>
         </is>
       </c>
-      <c r="O5" t="inlineStr">
+      <c r="R5" s="7" t="inlineStr">
         <is>
           <t>hg</t>
         </is>
       </c>
-      <c r="P5" t="inlineStr">
+      <c r="S5" s="7" t="inlineStr">
         <is>
           <t>77777</t>
         </is>
       </c>
     </row>
-    <row r="6"/>
-    <row r="7">
-      <c r="A7" t="inlineStr">
+    <row r="6" ht="18.75" customHeight="1">
+      <c r="A6" s="7" t="n"/>
+      <c r="B6" s="7" t="n"/>
+      <c r="C6" s="7" t="n"/>
+      <c r="D6" s="7" t="n"/>
+      <c r="E6" s="7" t="n"/>
+      <c r="F6" s="7" t="n"/>
+      <c r="G6" s="7" t="n"/>
+      <c r="H6" s="7" t="n"/>
+      <c r="I6" s="8" t="n"/>
+      <c r="J6" s="8" t="n"/>
+      <c r="K6" s="7" t="n"/>
+      <c r="L6" s="7" t="n"/>
+      <c r="M6" s="7" t="n"/>
+      <c r="N6" s="7" t="n"/>
+      <c r="O6" s="7" t="n"/>
+      <c r="P6" s="7" t="n"/>
+      <c r="Q6" s="7" t="n"/>
+      <c r="R6" s="7" t="n"/>
+      <c r="S6" s="7" t="n"/>
+    </row>
+    <row r="7" ht="18.75" customHeight="1">
+      <c r="A7" s="7" t="inlineStr">
         <is>
           <t>02/20/2024</t>
         </is>
       </c>
-      <c r="B7" t="inlineStr">
+      <c r="B7" s="7" t="inlineStr">
         <is>
           <t>SO240220001</t>
         </is>
       </c>
-      <c r="C7" t="inlineStr">
+      <c r="C7" s="7" t="inlineStr">
         <is>
           <t>ab</t>
         </is>
       </c>
-      <c r="D7" t="inlineStr">
+      <c r="D7" s="7" t="inlineStr">
         <is>
           <t>9887456123</t>
         </is>
       </c>
-      <c r="E7" t="inlineStr">
+      <c r="E7" s="7" t="n"/>
+      <c r="F7" s="7" t="n"/>
+      <c r="G7" s="7" t="inlineStr">
         <is>
           <t>as</t>
         </is>
       </c>
-      <c r="F7" t="inlineStr">
+      <c r="H7" s="7" t="inlineStr">
         <is>
           <t>as</t>
         </is>
       </c>
-      <c r="G7" t="n">
+      <c r="I7" s="4" t="n">
         <v>50</v>
       </c>
-      <c r="H7" t="n">
+      <c r="J7" s="6" t="n">
         <v>50.2</v>
       </c>
-      <c r="I7" t="inlineStr">
+      <c r="K7" s="7" t="n"/>
+      <c r="L7" s="7" t="inlineStr">
         <is>
           <t>AMS</t>
         </is>
       </c>
-      <c r="J7" t="inlineStr">
+      <c r="M7" s="7" t="inlineStr">
         <is>
           <t>DVD</t>
         </is>
       </c>
-      <c r="K7" t="inlineStr">
+      <c r="N7" s="7" t="inlineStr">
         <is>
           <t>ab</t>
         </is>
       </c>
-      <c r="L7" t="inlineStr">
+      <c r="O7" s="7" t="inlineStr">
         <is>
           <t>NO</t>
         </is>
       </c>
+      <c r="P7" s="7" t="n"/>
+      <c r="Q7" s="7" t="n"/>
+      <c r="R7" s="7" t="n"/>
+      <c r="S7" s="7" t="n"/>
     </row>
-    <row r="8">
-      <c r="A8" t="inlineStr"/>
-      <c r="B8" t="inlineStr"/>
-      <c r="C8" t="inlineStr"/>
-      <c r="D8" t="inlineStr"/>
-      <c r="E8" t="inlineStr"/>
-      <c r="F8" t="inlineStr"/>
-      <c r="G8" t="inlineStr"/>
-      <c r="H8" t="inlineStr"/>
-      <c r="I8" t="inlineStr"/>
-      <c r="J8" t="inlineStr"/>
-      <c r="K8" t="inlineStr"/>
-      <c r="L8" t="inlineStr"/>
-      <c r="M8" t="inlineStr"/>
-      <c r="N8" t="inlineStr"/>
-      <c r="O8" t="inlineStr"/>
-      <c r="P8" t="inlineStr"/>
+    <row r="8" ht="18.75" customHeight="1">
+      <c r="A8" s="7" t="n"/>
+      <c r="B8" s="7" t="n"/>
+      <c r="C8" s="7" t="n"/>
+      <c r="D8" s="7" t="n"/>
+      <c r="E8" s="7" t="n"/>
+      <c r="F8" s="7" t="n"/>
+      <c r="G8" s="7" t="n"/>
+      <c r="H8" s="7" t="n"/>
+      <c r="I8" s="8" t="n"/>
+      <c r="J8" s="8" t="n"/>
+      <c r="K8" s="7" t="n"/>
+      <c r="L8" s="7" t="n"/>
+      <c r="M8" s="7" t="n"/>
+      <c r="N8" s="7" t="n"/>
+      <c r="O8" s="7" t="n"/>
+      <c r="P8" s="7" t="n"/>
+      <c r="Q8" s="7" t="n"/>
+      <c r="R8" s="7" t="n"/>
+      <c r="S8" s="7" t="n"/>
     </row>
-    <row r="9">
-      <c r="A9" t="inlineStr">
+    <row r="9" ht="18.75" customHeight="1">
+      <c r="A9" s="7" t="inlineStr">
         <is>
           <t>03/05/2024</t>
         </is>
       </c>
-      <c r="B9" t="inlineStr">
+      <c r="B9" s="7" t="inlineStr">
         <is>
           <t>SO240305001</t>
         </is>
       </c>
-      <c r="C9" t="inlineStr">
+      <c r="C9" s="7" t="inlineStr">
         <is>
           <t>asshley</t>
         </is>
       </c>
-      <c r="D9" t="inlineStr">
+      <c r="D9" s="7" t="inlineStr">
         <is>
           <t>5642858215</t>
         </is>
       </c>
-      <c r="E9" t="inlineStr">
+      <c r="E9" s="7" t="n"/>
+      <c r="F9" s="7" t="n"/>
+      <c r="G9" s="7" t="inlineStr">
         <is>
           <t>artist</t>
         </is>
       </c>
-      <c r="F9" t="inlineStr">
+      <c r="H9" s="7" t="inlineStr">
         <is>
           <t>title</t>
         </is>
       </c>
-      <c r="G9" t="n">
+      <c r="I9" s="4" t="n">
         <v>50</v>
       </c>
-      <c r="H9" t="n">
+      <c r="J9" s="6" t="n">
         <v>58.63</v>
       </c>
-      <c r="I9" t="inlineStr">
+      <c r="K9" s="7" t="n"/>
+      <c r="L9" s="7" t="inlineStr">
         <is>
           <t>AMS</t>
         </is>
       </c>
-      <c r="J9" t="inlineStr">
+      <c r="M9" s="7" t="inlineStr">
         <is>
           <t>LP</t>
         </is>
       </c>
-      <c r="K9" t="inlineStr"/>
-      <c r="L9" t="inlineStr">
+      <c r="N9" s="7" t="n"/>
+      <c r="O9" s="7" t="inlineStr">
         <is>
           <t>NO</t>
         </is>
       </c>
-      <c r="M9" t="inlineStr"/>
+      <c r="P9" s="7" t="n"/>
+      <c r="Q9" s="7" t="n"/>
+      <c r="R9" s="7" t="n"/>
+      <c r="S9" s="7" t="n"/>
+    </row>
+    <row r="10" ht="18.75" customHeight="1">
+      <c r="A10" s="7" t="n"/>
+      <c r="B10" s="7" t="n"/>
+      <c r="C10" s="7" t="n"/>
+      <c r="D10" s="7" t="n"/>
+      <c r="E10" s="7" t="n"/>
+      <c r="F10" s="7" t="n"/>
+      <c r="G10" s="7" t="n"/>
+      <c r="H10" s="7" t="n"/>
+      <c r="I10" s="8" t="n"/>
+      <c r="J10" s="8" t="n"/>
+      <c r="K10" s="7" t="n"/>
+      <c r="L10" s="7" t="n"/>
+      <c r="M10" s="7" t="n"/>
+      <c r="N10" s="7" t="n"/>
+      <c r="O10" s="7" t="n"/>
+      <c r="P10" s="7" t="n"/>
+      <c r="Q10" s="7" t="n"/>
+      <c r="R10" s="7" t="n"/>
+      <c r="S10" s="7" t="n"/>
+    </row>
+    <row r="11" ht="18.75" customHeight="1">
+      <c r="A11" s="7" t="inlineStr">
+        <is>
+          <t>03/06/2024</t>
+        </is>
+      </c>
+      <c r="B11" s="7" t="inlineStr">
+        <is>
+          <t>SO240306001</t>
+        </is>
+      </c>
+      <c r="C11" s="7" t="inlineStr">
+        <is>
+          <t>Ashley Baker</t>
+        </is>
+      </c>
+      <c r="D11" s="7" t="inlineStr">
+        <is>
+          <t>(272)727-2000</t>
+        </is>
+      </c>
+      <c r="E11" s="7" t="n"/>
+      <c r="F11" s="7" t="n"/>
+      <c r="G11" s="7" t="inlineStr">
+        <is>
+          <t>Artist</t>
+        </is>
+      </c>
+      <c r="H11" s="7" t="inlineStr">
+        <is>
+          <t>Title</t>
+        </is>
+      </c>
+      <c r="I11" s="4" t="n">
+        <v>34</v>
+      </c>
+      <c r="J11" s="4" t="n">
+        <v>199</v>
+      </c>
+      <c r="K11" s="7" t="n"/>
+      <c r="L11" s="7" t="inlineStr">
+        <is>
+          <t>AMA</t>
+        </is>
+      </c>
+      <c r="M11" s="7" t="inlineStr">
+        <is>
+          <t>LP</t>
+        </is>
+      </c>
+      <c r="N11" s="7" t="inlineStr">
+        <is>
+          <t>Ashley</t>
+        </is>
+      </c>
+      <c r="O11" s="7" t="inlineStr">
+        <is>
+          <t>NO</t>
+        </is>
+      </c>
+      <c r="P11" s="7" t="n"/>
+      <c r="Q11" s="7" t="n"/>
+      <c r="R11" s="7" t="n"/>
+      <c r="S11" s="7" t="n"/>
+    </row>
+    <row r="12">
+      <c r="A12" t="inlineStr">
+        <is>
+          <t>03/06/2024</t>
+        </is>
+      </c>
+      <c r="B12" t="inlineStr">
+        <is>
+          <t>SO240306002</t>
+        </is>
+      </c>
+      <c r="C12" t="inlineStr">
+        <is>
+          <t>Ashley</t>
+        </is>
+      </c>
+      <c r="D12" t="inlineStr">
+        <is>
+          <t>(987)456-3210</t>
+        </is>
+      </c>
+      <c r="E12" t="inlineStr">
+        <is>
+          <t>YES</t>
+        </is>
+      </c>
+      <c r="F12" t="inlineStr">
+        <is>
+          <t>YES</t>
+        </is>
+      </c>
+      <c r="G12" t="inlineStr">
+        <is>
+          <t>artist</t>
+        </is>
+      </c>
+      <c r="H12" t="inlineStr">
+        <is>
+          <t>title</t>
+        </is>
+      </c>
+      <c r="I12" t="n">
+        <v>5</v>
+      </c>
+      <c r="J12" t="n">
+        <v>15</v>
+      </c>
+      <c r="K12" t="inlineStr">
+        <is>
+          <t> </t>
+        </is>
+      </c>
+      <c r="L12" t="inlineStr">
+        <is>
+          <t>AMA</t>
+        </is>
+      </c>
+      <c r="M12" t="inlineStr">
+        <is>
+          <t>CD</t>
+        </is>
+      </c>
+      <c r="N12" t="inlineStr">
+        <is>
+          <t>Ashley</t>
+        </is>
+      </c>
+      <c r="O12" t="inlineStr">
+        <is>
+          <t>NO</t>
+        </is>
+      </c>
+      <c r="P12" t="inlineStr"/>
+      <c r="Q12" t="inlineStr"/>
+      <c r="R12" t="inlineStr"/>
+      <c r="S12" t="inlineStr"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
modifying Prev_SO's treeview widget
</commit_message>
<xml_diff>
--- a/SO_Test.xlsx
+++ b/SO_Test.xlsx
@@ -449,13 +449,13 @@
     <outlinePr summaryBelow="0"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:W14"/>
+  <dimension ref="A1:W15"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15" outlineLevelCol="0"/>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <cols>
     <col width="13.57642857142857" bestFit="1" customWidth="1" style="6" min="1" max="1"/>
     <col width="16.29071428571428" bestFit="1" customWidth="1" style="6" min="2" max="2"/>
@@ -1234,31 +1234,7 @@
       <c r="V12" s="6" t="n"/>
       <c r="W12" s="6" t="n"/>
     </row>
-    <row r="13">
-      <c r="A13" t="inlineStr"/>
-      <c r="B13" t="inlineStr"/>
-      <c r="C13" t="inlineStr"/>
-      <c r="D13" t="inlineStr"/>
-      <c r="E13" t="inlineStr"/>
-      <c r="F13" t="inlineStr"/>
-      <c r="G13" t="inlineStr"/>
-      <c r="H13" t="inlineStr"/>
-      <c r="I13" t="inlineStr"/>
-      <c r="J13" t="inlineStr"/>
-      <c r="K13" t="inlineStr"/>
-      <c r="L13" t="inlineStr"/>
-      <c r="M13" t="inlineStr"/>
-      <c r="N13" t="inlineStr"/>
-      <c r="O13" t="inlineStr"/>
-      <c r="P13" t="inlineStr"/>
-      <c r="Q13" t="inlineStr"/>
-      <c r="R13" t="inlineStr"/>
-      <c r="S13" t="inlineStr"/>
-      <c r="T13" t="inlineStr"/>
-      <c r="U13" t="inlineStr"/>
-      <c r="V13" t="inlineStr"/>
-      <c r="W13" t="inlineStr"/>
-    </row>
+    <row r="13"/>
     <row r="14">
       <c r="A14" t="inlineStr">
         <is>
@@ -1332,6 +1308,84 @@
         </is>
       </c>
       <c r="P14" t="inlineStr">
+        <is>
+          <t>PICKUP</t>
+        </is>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" t="inlineStr">
+        <is>
+          <t>03/07/2024</t>
+        </is>
+      </c>
+      <c r="B15" t="inlineStr">
+        <is>
+          <t>SO240307002</t>
+        </is>
+      </c>
+      <c r="C15" t="inlineStr">
+        <is>
+          <t>NO</t>
+        </is>
+      </c>
+      <c r="D15" t="inlineStr">
+        <is>
+          <t>ab</t>
+        </is>
+      </c>
+      <c r="E15" t="inlineStr">
+        <is>
+          <t>(787)978-9777</t>
+        </is>
+      </c>
+      <c r="F15" t="inlineStr">
+        <is>
+          <t>NO</t>
+        </is>
+      </c>
+      <c r="G15" t="inlineStr">
+        <is>
+          <t>NO</t>
+        </is>
+      </c>
+      <c r="H15" t="inlineStr">
+        <is>
+          <t>artist</t>
+        </is>
+      </c>
+      <c r="I15" t="inlineStr">
+        <is>
+          <t>title</t>
+        </is>
+      </c>
+      <c r="J15" t="n">
+        <v>5</v>
+      </c>
+      <c r="K15" t="n">
+        <v>87</v>
+      </c>
+      <c r="L15" t="inlineStr">
+        <is>
+          <t> </t>
+        </is>
+      </c>
+      <c r="M15" t="inlineStr">
+        <is>
+          <t>AMA</t>
+        </is>
+      </c>
+      <c r="N15" t="inlineStr">
+        <is>
+          <t>CD</t>
+        </is>
+      </c>
+      <c r="O15" t="inlineStr">
+        <is>
+          <t>abake</t>
+        </is>
+      </c>
+      <c r="P15" t="inlineStr">
         <is>
           <t>PICKUP</t>
         </is>

</xml_diff>

<commit_message>
fixed the vertical scroll in Prev_SO need to fix the reset function in SO_Form because widgets shift to the right and the SO label is not as expected
</commit_message>
<xml_diff>
--- a/SO_Test.xlsx
+++ b/SO_Test.xlsx
@@ -16,7 +16,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="0"/>
-  <fonts count="2">
+  <fonts count="3">
     <font>
       <name val="Calibri"/>
       <family val="2"/>
@@ -28,6 +28,12 @@
       <name val="Calibri"/>
       <family val="2"/>
       <color rgb="FF000000"/>
+      <sz val="11"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <color theme="1"/>
       <sz val="11"/>
     </font>
   </fonts>
@@ -58,7 +64,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="general"/>
@@ -66,13 +72,19 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="3" fontId="0" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="3" fontId="1" fillId="0" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="right"/>
     </xf>
+    <xf numFmtId="3" fontId="2" fillId="0" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="right"/>
+    </xf>
     <xf numFmtId="4" fontId="1" fillId="0" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="3" fontId="0" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
@@ -80,9 +92,6 @@
     </xf>
     <xf numFmtId="3" fontId="0" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="3" fontId="0" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="general"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -449,7 +458,7 @@
     <outlinePr summaryBelow="0"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:W15"/>
+  <dimension ref="A1:W17"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -457,48 +466,48 @@
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <cols>
-    <col width="13.57642857142857" bestFit="1" customWidth="1" style="6" min="1" max="1"/>
-    <col width="16.29071428571428" bestFit="1" customWidth="1" style="6" min="2" max="2"/>
-    <col width="13.57642857142857" bestFit="1" customWidth="1" style="6" min="3" max="3"/>
-    <col width="14.57642857142857" bestFit="1" customWidth="1" style="6" min="4" max="4"/>
-    <col width="13.57642857142857" bestFit="1" customWidth="1" style="6" min="5" max="5"/>
-    <col width="6.147857142857143" bestFit="1" customWidth="1" style="6" min="6" max="6"/>
-    <col width="6.433571428571429" bestFit="1" customWidth="1" style="6" min="7" max="7"/>
-    <col width="13.57642857142857" bestFit="1" customWidth="1" style="6" min="8" max="8"/>
-    <col width="13.57642857142857" bestFit="1" customWidth="1" style="7" min="9" max="9"/>
-    <col width="13.57642857142857" bestFit="1" customWidth="1" style="7" min="10" max="10"/>
-    <col width="13.57642857142857" bestFit="1" customWidth="1" style="8" min="11" max="11"/>
-    <col width="13.57642857142857" bestFit="1" customWidth="1" style="6" min="12" max="12"/>
-    <col width="10.005" bestFit="1" customWidth="1" style="6" min="13" max="13"/>
-    <col width="8.576428571428572" bestFit="1" customWidth="1" style="6" min="14" max="14"/>
-    <col width="13.57642857142857" bestFit="1" customWidth="1" style="6" min="15" max="15"/>
-    <col width="10.43357142857143" bestFit="1" customWidth="1" style="6" min="16" max="16"/>
-    <col width="33.71928571428572" bestFit="1" customWidth="1" style="6" min="17" max="17"/>
-    <col width="14.71928571428571" bestFit="1" customWidth="1" style="6" min="18" max="18"/>
-    <col width="7.719285714285714" bestFit="1" customWidth="1" style="6" min="19" max="19"/>
-    <col width="10.005" bestFit="1" customWidth="1" style="6" min="20" max="20"/>
-    <col width="13.57642857142857" bestFit="1" customWidth="1" style="6" min="21" max="21"/>
-    <col width="13.57642857142857" bestFit="1" customWidth="1" style="6" min="22" max="22"/>
-    <col width="19.43357142857143" bestFit="1" customWidth="1" style="6" min="23" max="23"/>
+    <col width="13.57642857142857" bestFit="1" customWidth="1" style="8" min="1" max="1"/>
+    <col width="16.29071428571428" bestFit="1" customWidth="1" style="8" min="2" max="2"/>
+    <col width="13.57642857142857" bestFit="1" customWidth="1" style="8" min="3" max="3"/>
+    <col width="14.57642857142857" bestFit="1" customWidth="1" style="8" min="4" max="4"/>
+    <col width="13.57642857142857" bestFit="1" customWidth="1" style="8" min="5" max="5"/>
+    <col width="6.147857142857143" bestFit="1" customWidth="1" style="8" min="6" max="6"/>
+    <col width="6.433571428571429" bestFit="1" customWidth="1" style="8" min="7" max="7"/>
+    <col width="13.57642857142857" bestFit="1" customWidth="1" style="8" min="8" max="8"/>
+    <col width="13.57642857142857" bestFit="1" customWidth="1" style="8" min="9" max="9"/>
+    <col width="13.57642857142857" bestFit="1" customWidth="1" style="9" min="10" max="10"/>
+    <col width="13.57642857142857" bestFit="1" customWidth="1" style="9" min="11" max="11"/>
+    <col width="13.57642857142857" bestFit="1" customWidth="1" style="8" min="12" max="12"/>
+    <col width="10.005" bestFit="1" customWidth="1" style="8" min="13" max="13"/>
+    <col width="8.576428571428572" bestFit="1" customWidth="1" style="8" min="14" max="14"/>
+    <col width="13.57642857142857" bestFit="1" customWidth="1" style="8" min="15" max="15"/>
+    <col width="10.43357142857143" bestFit="1" customWidth="1" style="8" min="16" max="16"/>
+    <col width="33.71928571428572" bestFit="1" customWidth="1" style="8" min="17" max="17"/>
+    <col width="14.71928571428571" bestFit="1" customWidth="1" style="8" min="18" max="18"/>
+    <col width="7.719285714285714" bestFit="1" customWidth="1" style="8" min="19" max="19"/>
+    <col width="10.005" bestFit="1" customWidth="1" style="8" min="20" max="20"/>
+    <col width="13.57642857142857" bestFit="1" customWidth="1" style="8" min="21" max="21"/>
+    <col width="13.57642857142857" bestFit="1" customWidth="1" style="8" min="22" max="22"/>
+    <col width="19.43357142857143" bestFit="1" customWidth="1" style="8" min="23" max="23"/>
   </cols>
   <sheetData>
     <row r="1" ht="19.5" customHeight="1">
-      <c r="A1" s="6" t="inlineStr">
+      <c r="A1" s="8" t="inlineStr">
         <is>
           <t>DATE</t>
         </is>
       </c>
-      <c r="B1" s="6" t="inlineStr">
+      <c r="B1" s="8" t="inlineStr">
         <is>
           <t>REF NUM</t>
         </is>
       </c>
-      <c r="C1" s="6" t="inlineStr">
+      <c r="C1" s="8" t="inlineStr">
         <is>
           <t>COMPLETED</t>
         </is>
       </c>
-      <c r="D1" s="6" t="inlineStr">
+      <c r="D1" s="8" t="inlineStr">
         <is>
           <t>CX NAME</t>
         </is>
@@ -508,22 +517,22 @@
           <t>PHONE</t>
         </is>
       </c>
-      <c r="F1" s="6" t="inlineStr">
+      <c r="F1" s="8" t="inlineStr">
         <is>
           <t>TEXT?</t>
         </is>
       </c>
-      <c r="G1" s="6" t="inlineStr">
+      <c r="G1" s="8" t="inlineStr">
         <is>
           <t>CALL?</t>
         </is>
       </c>
-      <c r="H1" s="6" t="inlineStr">
+      <c r="H1" s="8" t="inlineStr">
         <is>
           <t>ARTIST</t>
         </is>
       </c>
-      <c r="I1" s="7" t="inlineStr">
+      <c r="I1" s="3" t="inlineStr">
         <is>
           <t>TITLE</t>
         </is>
@@ -538,101 +547,101 @@
           <t>RETAIL</t>
         </is>
       </c>
-      <c r="L1" s="6" t="inlineStr">
+      <c r="L1" s="8" t="inlineStr">
         <is>
           <t>COG</t>
         </is>
       </c>
-      <c r="M1" s="6" t="inlineStr">
+      <c r="M1" s="8" t="inlineStr">
         <is>
           <t>VENDOR</t>
         </is>
       </c>
-      <c r="N1" s="6" t="inlineStr">
+      <c r="N1" s="8" t="inlineStr">
         <is>
           <t>TYPE</t>
         </is>
       </c>
-      <c r="O1" s="6" t="inlineStr">
+      <c r="O1" s="8" t="inlineStr">
         <is>
           <t>CLERK NAME</t>
         </is>
       </c>
-      <c r="P1" s="6" t="inlineStr">
+      <c r="P1" s="8" t="inlineStr">
         <is>
           <t>SHIPPING?</t>
         </is>
       </c>
-      <c r="Q1" s="6" t="inlineStr">
+      <c r="Q1" s="8" t="inlineStr">
         <is>
           <t>ADDRESS</t>
         </is>
       </c>
-      <c r="R1" s="6" t="inlineStr">
+      <c r="R1" s="8" t="inlineStr">
         <is>
           <t>CITY</t>
         </is>
       </c>
-      <c r="S1" s="6" t="inlineStr">
+      <c r="S1" s="8" t="inlineStr">
         <is>
           <t>STATE</t>
         </is>
       </c>
-      <c r="T1" s="6" t="inlineStr">
+      <c r="T1" s="8" t="inlineStr">
         <is>
           <t>ZIPCODE</t>
         </is>
       </c>
-      <c r="U1" s="6" t="inlineStr">
-        <is>
-          <t>CALLED PICKUP</t>
-        </is>
-      </c>
-      <c r="V1" s="6" t="inlineStr">
-        <is>
-          <t>DATE</t>
-        </is>
-      </c>
-      <c r="W1" s="6" t="inlineStr">
-        <is>
-          <t>CLERK</t>
+      <c r="U1" s="8" t="inlineStr">
+        <is>
+          <t>PICKUP CALL</t>
+        </is>
+      </c>
+      <c r="V1" s="8" t="inlineStr">
+        <is>
+          <t>CALL DATE</t>
+        </is>
+      </c>
+      <c r="W1" s="8" t="inlineStr">
+        <is>
+          <t>ASSISTING CLERK</t>
         </is>
       </c>
     </row>
     <row r="2" ht="19.5" customHeight="1">
-      <c r="A2" s="6" t="inlineStr">
+      <c r="A2" s="8" t="inlineStr">
         <is>
           <t>02/18/2024</t>
         </is>
       </c>
-      <c r="B2" s="6" t="inlineStr">
+      <c r="B2" s="8" t="inlineStr">
         <is>
           <t>SO240218001</t>
         </is>
       </c>
-      <c r="C2" s="6" t="inlineStr">
-        <is>
-          <t>NO</t>
-        </is>
-      </c>
-      <c r="D2" s="6" t="inlineStr">
+      <c r="C2" s="8" t="inlineStr">
+        <is>
+          <t>NO</t>
+        </is>
+      </c>
+      <c r="D2" s="8" t="inlineStr">
         <is>
           <t>ab</t>
         </is>
       </c>
-      <c r="E2" s="6" t="inlineStr">
+      <c r="E2" s="8" t="inlineStr">
         <is>
           <t>7894561230</t>
         </is>
       </c>
-      <c r="F2" s="6" t="n"/>
-      <c r="G2" s="6" t="n"/>
-      <c r="H2" s="6" t="inlineStr">
+      <c r="F2" s="8" t="n"/>
+      <c r="G2" s="8" t="n"/>
+      <c r="H2" s="8" t="inlineStr">
         <is>
           <t>ab</t>
         </is>
       </c>
-      <c r="I2" s="7" t="inlineStr">
+      <c r="I2" s="3" t="inlineStr">
         <is>
           <t>ab</t>
         </is>
@@ -643,94 +652,94 @@
       <c r="K2" s="4" t="n">
         <v>24</v>
       </c>
-      <c r="L2" s="6" t="n"/>
-      <c r="M2" s="6" t="inlineStr">
+      <c r="L2" s="8" t="n"/>
+      <c r="M2" s="8" t="inlineStr">
         <is>
           <t>Vendors</t>
         </is>
       </c>
-      <c r="N2" s="6" t="inlineStr">
+      <c r="N2" s="8" t="inlineStr">
         <is>
           <t>DVD</t>
         </is>
       </c>
-      <c r="O2" s="6" t="inlineStr">
+      <c r="O2" s="8" t="inlineStr">
         <is>
           <t>ab</t>
         </is>
       </c>
-      <c r="P2" s="6" t="inlineStr">
-        <is>
-          <t>NO</t>
-        </is>
-      </c>
-      <c r="Q2" s="6" t="n"/>
-      <c r="R2" s="6" t="n"/>
-      <c r="S2" s="6" t="n"/>
-      <c r="T2" s="6" t="n"/>
-      <c r="U2" s="6" t="n"/>
-      <c r="V2" s="6" t="n"/>
-      <c r="W2" s="6" t="n"/>
+      <c r="P2" s="8" t="inlineStr">
+        <is>
+          <t>NO</t>
+        </is>
+      </c>
+      <c r="Q2" s="8" t="n"/>
+      <c r="R2" s="8" t="n"/>
+      <c r="S2" s="8" t="n"/>
+      <c r="T2" s="8" t="n"/>
+      <c r="U2" s="8" t="n"/>
+      <c r="V2" s="8" t="n"/>
+      <c r="W2" s="8" t="n"/>
     </row>
     <row r="3" ht="19.5" customHeight="1">
-      <c r="A3" s="6" t="n"/>
-      <c r="B3" s="6" t="n"/>
-      <c r="C3" s="6" t="n"/>
-      <c r="D3" s="6" t="n"/>
-      <c r="E3" s="6" t="n"/>
-      <c r="F3" s="6" t="n"/>
-      <c r="G3" s="6" t="n"/>
-      <c r="H3" s="6" t="n"/>
-      <c r="I3" s="7" t="n"/>
+      <c r="A3" s="8" t="n"/>
+      <c r="B3" s="8" t="n"/>
+      <c r="C3" s="8" t="n"/>
+      <c r="D3" s="8" t="n"/>
+      <c r="E3" s="8" t="n"/>
+      <c r="F3" s="8" t="n"/>
+      <c r="G3" s="8" t="n"/>
+      <c r="H3" s="8" t="n"/>
+      <c r="I3" s="5" t="n"/>
       <c r="J3" s="4" t="n"/>
       <c r="K3" s="4" t="n"/>
-      <c r="L3" s="6" t="n"/>
-      <c r="M3" s="6" t="n"/>
-      <c r="N3" s="6" t="n"/>
-      <c r="O3" s="6" t="n"/>
-      <c r="P3" s="6" t="n"/>
-      <c r="Q3" s="6" t="n"/>
-      <c r="R3" s="6" t="n"/>
-      <c r="S3" s="6" t="n"/>
-      <c r="T3" s="6" t="n"/>
-      <c r="U3" s="6" t="n"/>
-      <c r="V3" s="6" t="n"/>
-      <c r="W3" s="6" t="n"/>
+      <c r="L3" s="8" t="n"/>
+      <c r="M3" s="8" t="n"/>
+      <c r="N3" s="8" t="n"/>
+      <c r="O3" s="8" t="n"/>
+      <c r="P3" s="8" t="n"/>
+      <c r="Q3" s="8" t="n"/>
+      <c r="R3" s="8" t="n"/>
+      <c r="S3" s="8" t="n"/>
+      <c r="T3" s="8" t="n"/>
+      <c r="U3" s="8" t="n"/>
+      <c r="V3" s="8" t="n"/>
+      <c r="W3" s="8" t="n"/>
     </row>
     <row r="4" ht="19.5" customHeight="1">
-      <c r="A4" s="6" t="inlineStr">
+      <c r="A4" s="8" t="inlineStr">
         <is>
           <t>02/19/2024</t>
         </is>
       </c>
-      <c r="B4" s="6" t="inlineStr">
+      <c r="B4" s="8" t="inlineStr">
         <is>
           <t>SO240219001</t>
         </is>
       </c>
-      <c r="C4" s="6" t="inlineStr">
+      <c r="C4" s="8" t="inlineStr">
         <is>
           <t>YES</t>
         </is>
       </c>
-      <c r="D4" s="6" t="inlineStr">
+      <c r="D4" s="8" t="inlineStr">
         <is>
           <t>ab</t>
         </is>
       </c>
-      <c r="E4" s="6" t="inlineStr">
+      <c r="E4" s="8" t="inlineStr">
         <is>
           <t>7894561230</t>
         </is>
       </c>
-      <c r="F4" s="6" t="n"/>
-      <c r="G4" s="6" t="n"/>
-      <c r="H4" s="6" t="inlineStr">
+      <c r="F4" s="8" t="n"/>
+      <c r="G4" s="8" t="n"/>
+      <c r="H4" s="8" t="inlineStr">
         <is>
           <t>a</t>
         </is>
       </c>
-      <c r="I4" s="7" t="inlineStr">
+      <c r="I4" s="3" t="inlineStr">
         <is>
           <t>a</t>
         </is>
@@ -741,69 +750,69 @@
       <c r="K4" s="4" t="n">
         <v>34</v>
       </c>
-      <c r="L4" s="6" t="n"/>
-      <c r="M4" s="6" t="inlineStr">
+      <c r="L4" s="8" t="n"/>
+      <c r="M4" s="8" t="inlineStr">
         <is>
           <t>AMA</t>
         </is>
       </c>
-      <c r="N4" s="6" t="inlineStr">
+      <c r="N4" s="8" t="inlineStr">
         <is>
           <t>OTHER</t>
         </is>
       </c>
-      <c r="O4" s="6" t="inlineStr">
+      <c r="O4" s="8" t="inlineStr">
         <is>
           <t>ab</t>
         </is>
       </c>
-      <c r="P4" s="6" t="inlineStr">
-        <is>
-          <t>NO</t>
-        </is>
-      </c>
-      <c r="Q4" s="6" t="n"/>
-      <c r="R4" s="6" t="n"/>
-      <c r="S4" s="6" t="n"/>
-      <c r="T4" s="6" t="n"/>
-      <c r="U4" s="6" t="n"/>
-      <c r="V4" s="6" t="n"/>
-      <c r="W4" s="6" t="n"/>
+      <c r="P4" s="8" t="inlineStr">
+        <is>
+          <t>NO</t>
+        </is>
+      </c>
+      <c r="Q4" s="8" t="n"/>
+      <c r="R4" s="8" t="n"/>
+      <c r="S4" s="8" t="n"/>
+      <c r="T4" s="8" t="n"/>
+      <c r="U4" s="8" t="n"/>
+      <c r="V4" s="8" t="n"/>
+      <c r="W4" s="8" t="n"/>
     </row>
     <row r="5" ht="19.5" customHeight="1">
-      <c r="A5" s="6" t="inlineStr">
+      <c r="A5" s="8" t="inlineStr">
         <is>
           <t>02/19/2024</t>
         </is>
       </c>
-      <c r="B5" s="6" t="inlineStr">
+      <c r="B5" s="8" t="inlineStr">
         <is>
           <t>SO240219002</t>
         </is>
       </c>
-      <c r="C5" s="6" t="inlineStr">
-        <is>
-          <t>NO</t>
-        </is>
-      </c>
-      <c r="D5" s="6" t="inlineStr">
+      <c r="C5" s="8" t="inlineStr">
+        <is>
+          <t>NO</t>
+        </is>
+      </c>
+      <c r="D5" s="8" t="inlineStr">
         <is>
           <t>Me</t>
         </is>
       </c>
-      <c r="E5" s="6" t="inlineStr">
+      <c r="E5" s="8" t="inlineStr">
         <is>
           <t>5555555555</t>
         </is>
       </c>
-      <c r="F5" s="6" t="n"/>
-      <c r="G5" s="6" t="n"/>
-      <c r="H5" s="6" t="inlineStr">
+      <c r="F5" s="8" t="n"/>
+      <c r="G5" s="8" t="n"/>
+      <c r="H5" s="8" t="inlineStr">
         <is>
           <t>Type O Negative</t>
         </is>
       </c>
-      <c r="I5" s="7" t="inlineStr">
+      <c r="I5" s="3" t="inlineStr">
         <is>
           <t>Bloody Kisses</t>
         </is>
@@ -811,113 +820,113 @@
       <c r="J5" s="4" t="n">
         <v>5</v>
       </c>
-      <c r="K5" s="5" t="n">
+      <c r="K5" s="6" t="n">
         <v>49.99</v>
       </c>
-      <c r="L5" s="6" t="n"/>
-      <c r="M5" s="6" t="inlineStr">
+      <c r="L5" s="8" t="n"/>
+      <c r="M5" s="8" t="inlineStr">
         <is>
           <t>AMS</t>
         </is>
       </c>
-      <c r="N5" s="6" t="inlineStr">
+      <c r="N5" s="8" t="inlineStr">
         <is>
           <t>DVD</t>
         </is>
       </c>
-      <c r="O5" s="6" t="inlineStr">
+      <c r="O5" s="8" t="inlineStr">
         <is>
           <t>MTP</t>
         </is>
       </c>
-      <c r="P5" s="6" t="inlineStr">
-        <is>
-          <t>NO</t>
-        </is>
-      </c>
-      <c r="Q5" s="6" t="inlineStr">
+      <c r="P5" s="8" t="inlineStr">
+        <is>
+          <t>NO</t>
+        </is>
+      </c>
+      <c r="Q5" s="8" t="inlineStr">
         <is>
           <t>59848.0</t>
         </is>
       </c>
-      <c r="R5" s="6" t="inlineStr">
+      <c r="R5" s="8" t="inlineStr">
         <is>
           <t>gh</t>
         </is>
       </c>
-      <c r="S5" s="6" t="inlineStr">
+      <c r="S5" s="8" t="inlineStr">
         <is>
           <t>hg</t>
         </is>
       </c>
-      <c r="T5" s="6" t="inlineStr">
+      <c r="T5" s="8" t="inlineStr">
         <is>
           <t>77777</t>
         </is>
       </c>
-      <c r="U5" s="6" t="n"/>
-      <c r="V5" s="6" t="n"/>
-      <c r="W5" s="6" t="n"/>
+      <c r="U5" s="8" t="n"/>
+      <c r="V5" s="8" t="n"/>
+      <c r="W5" s="8" t="n"/>
     </row>
     <row r="6" ht="19.5" customHeight="1">
-      <c r="A6" s="6" t="n"/>
-      <c r="B6" s="6" t="n"/>
-      <c r="C6" s="6" t="n"/>
-      <c r="D6" s="6" t="n"/>
-      <c r="E6" s="6" t="n"/>
-      <c r="F6" s="6" t="n"/>
-      <c r="G6" s="6" t="n"/>
-      <c r="H6" s="6" t="n"/>
-      <c r="I6" s="7" t="n"/>
+      <c r="A6" s="8" t="n"/>
+      <c r="B6" s="8" t="n"/>
+      <c r="C6" s="8" t="n"/>
+      <c r="D6" s="8" t="n"/>
+      <c r="E6" s="8" t="n"/>
+      <c r="F6" s="8" t="n"/>
+      <c r="G6" s="8" t="n"/>
+      <c r="H6" s="8" t="n"/>
+      <c r="I6" s="5" t="n"/>
       <c r="J6" s="4" t="n"/>
       <c r="K6" s="4" t="n"/>
-      <c r="L6" s="6" t="n"/>
-      <c r="M6" s="6" t="n"/>
-      <c r="N6" s="6" t="n"/>
-      <c r="O6" s="6" t="n"/>
-      <c r="P6" s="6" t="n"/>
-      <c r="Q6" s="6" t="n"/>
-      <c r="R6" s="6" t="n"/>
-      <c r="S6" s="6" t="n"/>
-      <c r="T6" s="6" t="n"/>
-      <c r="U6" s="6" t="n"/>
-      <c r="V6" s="6" t="n"/>
-      <c r="W6" s="6" t="n"/>
+      <c r="L6" s="8" t="n"/>
+      <c r="M6" s="8" t="n"/>
+      <c r="N6" s="8" t="n"/>
+      <c r="O6" s="8" t="n"/>
+      <c r="P6" s="8" t="n"/>
+      <c r="Q6" s="8" t="n"/>
+      <c r="R6" s="8" t="n"/>
+      <c r="S6" s="8" t="n"/>
+      <c r="T6" s="8" t="n"/>
+      <c r="U6" s="8" t="n"/>
+      <c r="V6" s="8" t="n"/>
+      <c r="W6" s="8" t="n"/>
     </row>
     <row r="7" ht="19.5" customHeight="1">
-      <c r="A7" s="6" t="inlineStr">
+      <c r="A7" s="8" t="inlineStr">
         <is>
           <t>02/20/2024</t>
         </is>
       </c>
-      <c r="B7" s="6" t="inlineStr">
+      <c r="B7" s="8" t="inlineStr">
         <is>
           <t>SO240220001</t>
         </is>
       </c>
-      <c r="C7" s="6" t="inlineStr">
-        <is>
-          <t>NO</t>
-        </is>
-      </c>
-      <c r="D7" s="6" t="inlineStr">
+      <c r="C7" s="8" t="inlineStr">
+        <is>
+          <t>NO</t>
+        </is>
+      </c>
+      <c r="D7" s="8" t="inlineStr">
         <is>
           <t>ab</t>
         </is>
       </c>
-      <c r="E7" s="6" t="inlineStr">
+      <c r="E7" s="8" t="inlineStr">
         <is>
           <t>9887456123</t>
         </is>
       </c>
-      <c r="F7" s="6" t="n"/>
-      <c r="G7" s="6" t="n"/>
-      <c r="H7" s="6" t="inlineStr">
+      <c r="F7" s="8" t="n"/>
+      <c r="G7" s="8" t="n"/>
+      <c r="H7" s="8" t="inlineStr">
         <is>
           <t>as</t>
         </is>
       </c>
-      <c r="I7" s="7" t="inlineStr">
+      <c r="I7" s="3" t="inlineStr">
         <is>
           <t>as</t>
         </is>
@@ -925,97 +934,97 @@
       <c r="J7" s="4" t="n">
         <v>50</v>
       </c>
-      <c r="K7" s="5" t="n">
+      <c r="K7" s="6" t="n">
         <v>50.2</v>
       </c>
-      <c r="L7" s="6" t="n"/>
-      <c r="M7" s="6" t="inlineStr">
+      <c r="L7" s="8" t="n"/>
+      <c r="M7" s="8" t="inlineStr">
         <is>
           <t>AMS</t>
         </is>
       </c>
-      <c r="N7" s="6" t="inlineStr">
+      <c r="N7" s="8" t="inlineStr">
         <is>
           <t>DVD</t>
         </is>
       </c>
-      <c r="O7" s="6" t="inlineStr">
+      <c r="O7" s="8" t="inlineStr">
         <is>
           <t>ab</t>
         </is>
       </c>
-      <c r="P7" s="6" t="inlineStr">
-        <is>
-          <t>NO</t>
-        </is>
-      </c>
-      <c r="Q7" s="6" t="n"/>
-      <c r="R7" s="6" t="n"/>
-      <c r="S7" s="6" t="n"/>
-      <c r="T7" s="6" t="n"/>
-      <c r="U7" s="6" t="n"/>
-      <c r="V7" s="6" t="n"/>
-      <c r="W7" s="6" t="n"/>
+      <c r="P7" s="8" t="inlineStr">
+        <is>
+          <t>NO</t>
+        </is>
+      </c>
+      <c r="Q7" s="8" t="n"/>
+      <c r="R7" s="8" t="n"/>
+      <c r="S7" s="8" t="n"/>
+      <c r="T7" s="8" t="n"/>
+      <c r="U7" s="8" t="n"/>
+      <c r="V7" s="8" t="n"/>
+      <c r="W7" s="8" t="n"/>
     </row>
     <row r="8" ht="19.5" customHeight="1">
-      <c r="A8" s="6" t="n"/>
-      <c r="B8" s="6" t="n"/>
-      <c r="C8" s="6" t="n"/>
-      <c r="D8" s="6" t="n"/>
-      <c r="E8" s="6" t="n"/>
-      <c r="F8" s="6" t="n"/>
-      <c r="G8" s="6" t="n"/>
-      <c r="H8" s="6" t="n"/>
-      <c r="I8" s="7" t="n"/>
+      <c r="A8" s="8" t="n"/>
+      <c r="B8" s="8" t="n"/>
+      <c r="C8" s="8" t="n"/>
+      <c r="D8" s="8" t="n"/>
+      <c r="E8" s="8" t="n"/>
+      <c r="F8" s="8" t="n"/>
+      <c r="G8" s="8" t="n"/>
+      <c r="H8" s="8" t="n"/>
+      <c r="I8" s="5" t="n"/>
       <c r="J8" s="4" t="n"/>
       <c r="K8" s="4" t="n"/>
-      <c r="L8" s="6" t="n"/>
-      <c r="M8" s="6" t="n"/>
-      <c r="N8" s="6" t="n"/>
-      <c r="O8" s="6" t="n"/>
-      <c r="P8" s="6" t="n"/>
-      <c r="Q8" s="6" t="n"/>
-      <c r="R8" s="6" t="n"/>
-      <c r="S8" s="6" t="n"/>
-      <c r="T8" s="6" t="n"/>
-      <c r="U8" s="6" t="n"/>
-      <c r="V8" s="6" t="n"/>
-      <c r="W8" s="6" t="n"/>
+      <c r="L8" s="8" t="n"/>
+      <c r="M8" s="8" t="n"/>
+      <c r="N8" s="8" t="n"/>
+      <c r="O8" s="8" t="n"/>
+      <c r="P8" s="8" t="n"/>
+      <c r="Q8" s="8" t="n"/>
+      <c r="R8" s="8" t="n"/>
+      <c r="S8" s="8" t="n"/>
+      <c r="T8" s="8" t="n"/>
+      <c r="U8" s="8" t="n"/>
+      <c r="V8" s="8" t="n"/>
+      <c r="W8" s="8" t="n"/>
     </row>
     <row r="9" ht="19.5" customHeight="1">
-      <c r="A9" s="6" t="inlineStr">
+      <c r="A9" s="8" t="inlineStr">
         <is>
           <t>03/05/2024</t>
         </is>
       </c>
-      <c r="B9" s="6" t="inlineStr">
+      <c r="B9" s="8" t="inlineStr">
         <is>
           <t>SO240305001</t>
         </is>
       </c>
-      <c r="C9" s="6" t="inlineStr">
-        <is>
-          <t>NO</t>
-        </is>
-      </c>
-      <c r="D9" s="6" t="inlineStr">
+      <c r="C9" s="8" t="inlineStr">
+        <is>
+          <t>NO</t>
+        </is>
+      </c>
+      <c r="D9" s="8" t="inlineStr">
         <is>
           <t>asshley</t>
         </is>
       </c>
-      <c r="E9" s="6" t="inlineStr">
+      <c r="E9" s="8" t="inlineStr">
         <is>
           <t>5642858215</t>
         </is>
       </c>
-      <c r="F9" s="6" t="n"/>
-      <c r="G9" s="6" t="n"/>
-      <c r="H9" s="6" t="inlineStr">
+      <c r="F9" s="8" t="n"/>
+      <c r="G9" s="8" t="n"/>
+      <c r="H9" s="8" t="inlineStr">
         <is>
           <t>artist</t>
         </is>
       </c>
-      <c r="I9" s="7" t="inlineStr">
+      <c r="I9" s="3" t="inlineStr">
         <is>
           <t>title</t>
         </is>
@@ -1023,93 +1032,93 @@
       <c r="J9" s="4" t="n">
         <v>50</v>
       </c>
-      <c r="K9" s="5" t="n">
+      <c r="K9" s="6" t="n">
         <v>58.63</v>
       </c>
-      <c r="L9" s="6" t="n"/>
-      <c r="M9" s="6" t="inlineStr">
+      <c r="L9" s="8" t="n"/>
+      <c r="M9" s="8" t="inlineStr">
         <is>
           <t>AMS</t>
         </is>
       </c>
-      <c r="N9" s="6" t="inlineStr">
+      <c r="N9" s="8" t="inlineStr">
         <is>
           <t>LP</t>
         </is>
       </c>
-      <c r="O9" s="6" t="n"/>
-      <c r="P9" s="6" t="inlineStr">
-        <is>
-          <t>NO</t>
-        </is>
-      </c>
-      <c r="Q9" s="6" t="n"/>
-      <c r="R9" s="6" t="n"/>
-      <c r="S9" s="6" t="n"/>
-      <c r="T9" s="6" t="n"/>
-      <c r="U9" s="6" t="n"/>
-      <c r="V9" s="6" t="n"/>
-      <c r="W9" s="6" t="n"/>
+      <c r="O9" s="8" t="n"/>
+      <c r="P9" s="8" t="inlineStr">
+        <is>
+          <t>NO</t>
+        </is>
+      </c>
+      <c r="Q9" s="8" t="n"/>
+      <c r="R9" s="8" t="n"/>
+      <c r="S9" s="8" t="n"/>
+      <c r="T9" s="8" t="n"/>
+      <c r="U9" s="8" t="n"/>
+      <c r="V9" s="8" t="n"/>
+      <c r="W9" s="8" t="n"/>
     </row>
     <row r="10" ht="19.5" customHeight="1">
-      <c r="A10" s="6" t="n"/>
-      <c r="B10" s="6" t="n"/>
-      <c r="C10" s="6" t="n"/>
-      <c r="D10" s="6" t="n"/>
-      <c r="E10" s="6" t="n"/>
-      <c r="F10" s="6" t="n"/>
-      <c r="G10" s="6" t="n"/>
-      <c r="H10" s="6" t="n"/>
-      <c r="I10" s="7" t="n"/>
+      <c r="A10" s="8" t="n"/>
+      <c r="B10" s="8" t="n"/>
+      <c r="C10" s="8" t="n"/>
+      <c r="D10" s="8" t="n"/>
+      <c r="E10" s="8" t="n"/>
+      <c r="F10" s="8" t="n"/>
+      <c r="G10" s="8" t="n"/>
+      <c r="H10" s="8" t="n"/>
+      <c r="I10" s="5" t="n"/>
       <c r="J10" s="4" t="n"/>
       <c r="K10" s="4" t="n"/>
-      <c r="L10" s="6" t="n"/>
-      <c r="M10" s="6" t="n"/>
-      <c r="N10" s="6" t="n"/>
-      <c r="O10" s="6" t="n"/>
-      <c r="P10" s="6" t="n"/>
-      <c r="Q10" s="6" t="n"/>
-      <c r="R10" s="6" t="n"/>
-      <c r="S10" s="6" t="n"/>
-      <c r="T10" s="6" t="n"/>
-      <c r="U10" s="6" t="n"/>
-      <c r="V10" s="6" t="n"/>
-      <c r="W10" s="6" t="n"/>
+      <c r="L10" s="8" t="n"/>
+      <c r="M10" s="8" t="n"/>
+      <c r="N10" s="8" t="n"/>
+      <c r="O10" s="8" t="n"/>
+      <c r="P10" s="8" t="n"/>
+      <c r="Q10" s="8" t="n"/>
+      <c r="R10" s="8" t="n"/>
+      <c r="S10" s="8" t="n"/>
+      <c r="T10" s="8" t="n"/>
+      <c r="U10" s="8" t="n"/>
+      <c r="V10" s="8" t="n"/>
+      <c r="W10" s="8" t="n"/>
     </row>
     <row r="11" ht="19.5" customHeight="1">
-      <c r="A11" s="6" t="inlineStr">
+      <c r="A11" s="8" t="inlineStr">
         <is>
           <t>03/06/2024</t>
         </is>
       </c>
-      <c r="B11" s="6" t="inlineStr">
+      <c r="B11" s="8" t="inlineStr">
         <is>
           <t>SO240306001</t>
         </is>
       </c>
-      <c r="C11" s="6" t="inlineStr">
+      <c r="C11" s="8" t="inlineStr">
         <is>
           <t>YES</t>
         </is>
       </c>
-      <c r="D11" s="6" t="inlineStr">
+      <c r="D11" s="8" t="inlineStr">
         <is>
           <t>Ashley Baker</t>
         </is>
       </c>
-      <c r="E11" s="6" t="inlineStr">
+      <c r="E11" s="8" t="inlineStr">
         <is>
           <t>(272)727-2000</t>
         </is>
       </c>
-      <c r="F11" s="6" t="n"/>
-      <c r="G11" s="6" t="n"/>
-      <c r="H11" s="6" t="inlineStr">
+      <c r="F11" s="8" t="n"/>
+      <c r="G11" s="8" t="n"/>
+      <c r="H11" s="8" t="inlineStr">
         <is>
           <t>Artist</t>
         </is>
       </c>
-      <c r="I11" s="7" t="inlineStr">
+      <c r="I11" s="3" t="inlineStr">
         <is>
           <t>Title</t>
         </is>
@@ -1120,77 +1129,73 @@
       <c r="K11" s="4" t="n">
         <v>199</v>
       </c>
-      <c r="L11" s="6" t="n"/>
-      <c r="M11" s="6" t="inlineStr">
+      <c r="L11" s="8" t="n"/>
+      <c r="M11" s="8" t="inlineStr">
         <is>
           <t>AMA</t>
         </is>
       </c>
-      <c r="N11" s="6" t="inlineStr">
+      <c r="N11" s="8" t="inlineStr">
         <is>
           <t>LP</t>
         </is>
       </c>
-      <c r="O11" s="6" t="inlineStr">
+      <c r="O11" s="8" t="inlineStr">
         <is>
           <t>Ashley</t>
         </is>
       </c>
-      <c r="P11" s="6" t="inlineStr">
-        <is>
-          <t>NO</t>
-        </is>
-      </c>
-      <c r="Q11" s="6" t="n"/>
-      <c r="R11" s="6" t="n"/>
-      <c r="S11" s="6" t="n"/>
-      <c r="T11" s="6" t="n"/>
-      <c r="U11" s="6" t="n"/>
-      <c r="V11" s="6" t="n"/>
-      <c r="W11" s="6" t="n"/>
+      <c r="P11" s="8" t="inlineStr">
+        <is>
+          <t>NO</t>
+        </is>
+      </c>
+      <c r="Q11" s="8" t="n"/>
+      <c r="R11" s="8" t="n"/>
+      <c r="S11" s="8" t="n"/>
+      <c r="T11" s="8" t="n"/>
+      <c r="U11" s="8" t="n"/>
+      <c r="V11" s="8" t="n"/>
+      <c r="W11" s="8" t="n"/>
     </row>
     <row r="12" ht="19.5" customHeight="1">
-      <c r="A12" s="6" t="inlineStr">
+      <c r="A12" s="8" t="inlineStr">
         <is>
           <t>03/06/2024</t>
         </is>
       </c>
-      <c r="B12" s="6" t="inlineStr">
+      <c r="B12" s="8" t="inlineStr">
         <is>
           <t>SO240306002</t>
         </is>
       </c>
-      <c r="C12" s="6" t="inlineStr">
-        <is>
-          <t>NO</t>
-        </is>
-      </c>
-      <c r="D12" s="6" t="inlineStr">
+      <c r="C12" s="8" t="inlineStr"/>
+      <c r="D12" s="8" t="inlineStr">
         <is>
           <t>Ashley</t>
         </is>
       </c>
-      <c r="E12" s="6" t="inlineStr">
+      <c r="E12" s="8" t="inlineStr">
         <is>
           <t>(987)456-3210</t>
         </is>
       </c>
-      <c r="F12" s="6" t="inlineStr">
-        <is>
-          <t>NO</t>
-        </is>
-      </c>
-      <c r="G12" s="6" t="inlineStr">
+      <c r="F12" s="8" t="inlineStr">
         <is>
           <t>YES</t>
         </is>
       </c>
-      <c r="H12" s="6" t="inlineStr">
+      <c r="G12" s="8" t="inlineStr">
+        <is>
+          <t>YES</t>
+        </is>
+      </c>
+      <c r="H12" s="8" t="inlineStr">
         <is>
           <t>artist</t>
         </is>
       </c>
-      <c r="I12" s="7" t="inlineStr">
+      <c r="I12" s="3" t="inlineStr">
         <is>
           <t>title</t>
         </is>
@@ -1201,191 +1206,385 @@
       <c r="K12" s="4" t="n">
         <v>15</v>
       </c>
-      <c r="L12" s="6" t="inlineStr">
+      <c r="L12" s="8" t="inlineStr">
         <is>
           <t> </t>
         </is>
       </c>
-      <c r="M12" s="6" t="inlineStr">
+      <c r="M12" s="8" t="inlineStr">
         <is>
           <t>AMA</t>
         </is>
       </c>
-      <c r="N12" s="6" t="inlineStr">
+      <c r="N12" s="8" t="inlineStr">
         <is>
           <t>CD</t>
         </is>
       </c>
-      <c r="O12" s="6" t="inlineStr">
+      <c r="O12" s="8" t="inlineStr">
         <is>
           <t>Ashley</t>
         </is>
       </c>
-      <c r="P12" s="6" t="inlineStr">
-        <is>
-          <t>NO</t>
-        </is>
-      </c>
-      <c r="Q12" s="6" t="n"/>
-      <c r="R12" s="6" t="n"/>
-      <c r="S12" s="6" t="n"/>
-      <c r="T12" s="6" t="n"/>
-      <c r="U12" s="6" t="n"/>
-      <c r="V12" s="6" t="n"/>
-      <c r="W12" s="6" t="n"/>
-    </row>
-    <row r="13"/>
-    <row r="14">
-      <c r="A14" t="inlineStr">
+      <c r="P12" s="8" t="inlineStr">
+        <is>
+          <t>NO</t>
+        </is>
+      </c>
+      <c r="Q12" s="8" t="inlineStr"/>
+      <c r="R12" s="8" t="inlineStr"/>
+      <c r="S12" s="8" t="inlineStr"/>
+      <c r="T12" s="8" t="inlineStr"/>
+      <c r="U12" s="8" t="inlineStr"/>
+      <c r="V12" s="8" t="inlineStr"/>
+      <c r="W12" s="8" t="inlineStr"/>
+    </row>
+    <row r="13" ht="18.75" customHeight="1">
+      <c r="A13" s="8" t="n"/>
+      <c r="B13" s="8" t="n"/>
+      <c r="C13" s="8" t="n"/>
+      <c r="D13" s="8" t="n"/>
+      <c r="E13" s="8" t="n"/>
+      <c r="F13" s="8" t="n"/>
+      <c r="G13" s="8" t="n"/>
+      <c r="H13" s="8" t="n"/>
+      <c r="I13" s="8" t="n"/>
+      <c r="J13" s="9" t="n"/>
+      <c r="K13" s="9" t="n"/>
+      <c r="L13" s="8" t="n"/>
+      <c r="M13" s="8" t="n"/>
+      <c r="N13" s="8" t="n"/>
+      <c r="O13" s="8" t="n"/>
+      <c r="P13" s="8" t="n"/>
+      <c r="Q13" s="8" t="n"/>
+      <c r="R13" s="8" t="n"/>
+      <c r="S13" s="8" t="n"/>
+      <c r="T13" s="8" t="n"/>
+      <c r="U13" s="8" t="n"/>
+      <c r="V13" s="8" t="n"/>
+      <c r="W13" s="8" t="n"/>
+    </row>
+    <row r="14" ht="18.75" customHeight="1">
+      <c r="A14" s="8" t="inlineStr">
         <is>
           <t>03/07/2024</t>
         </is>
       </c>
-      <c r="B14" t="inlineStr">
+      <c r="B14" s="8" t="inlineStr">
         <is>
           <t>SO240307001</t>
         </is>
       </c>
-      <c r="C14" t="inlineStr">
-        <is>
-          <t>NO</t>
-        </is>
-      </c>
-      <c r="D14" t="inlineStr">
+      <c r="C14" s="8" t="inlineStr">
+        <is>
+          <t>NO</t>
+        </is>
+      </c>
+      <c r="D14" s="8" t="inlineStr">
         <is>
           <t>ab</t>
         </is>
       </c>
-      <c r="E14" t="inlineStr">
+      <c r="E14" s="8" t="inlineStr">
         <is>
           <t>(789)789-7878</t>
         </is>
       </c>
-      <c r="F14" t="inlineStr">
-        <is>
-          <t>NO</t>
-        </is>
-      </c>
-      <c r="G14" t="inlineStr">
+      <c r="F14" s="8" t="inlineStr">
+        <is>
+          <t>NO</t>
+        </is>
+      </c>
+      <c r="G14" s="8" t="inlineStr">
         <is>
           <t>YES</t>
         </is>
       </c>
-      <c r="H14" t="inlineStr">
+      <c r="H14" s="8" t="inlineStr">
         <is>
           <t>artist</t>
         </is>
       </c>
-      <c r="I14" t="inlineStr">
+      <c r="I14" s="8" t="inlineStr">
         <is>
           <t>title</t>
         </is>
       </c>
-      <c r="J14" t="n">
+      <c r="J14" s="5" t="n">
         <v>5</v>
       </c>
-      <c r="K14" t="n">
+      <c r="K14" s="5" t="n">
         <v>20</v>
       </c>
-      <c r="L14" t="inlineStr">
+      <c r="L14" s="8" t="inlineStr">
         <is>
           <t> </t>
         </is>
       </c>
-      <c r="M14" t="inlineStr">
+      <c r="M14" s="8" t="inlineStr">
         <is>
           <t>AMS</t>
         </is>
       </c>
-      <c r="N14" t="inlineStr">
+      <c r="N14" s="8" t="inlineStr">
         <is>
           <t>CD</t>
         </is>
       </c>
-      <c r="O14" t="inlineStr">
+      <c r="O14" s="8" t="inlineStr">
         <is>
           <t>abake</t>
         </is>
       </c>
-      <c r="P14" t="inlineStr">
+      <c r="P14" s="8" t="inlineStr">
         <is>
           <t>PICKUP</t>
         </is>
       </c>
-    </row>
-    <row r="15">
-      <c r="A15" t="inlineStr">
+      <c r="Q14" s="8" t="n"/>
+      <c r="R14" s="8" t="n"/>
+      <c r="S14" s="8" t="n"/>
+      <c r="T14" s="8" t="n"/>
+      <c r="U14" s="8" t="n"/>
+      <c r="V14" s="8" t="n"/>
+      <c r="W14" s="8" t="n"/>
+    </row>
+    <row r="15" ht="18.75" customHeight="1">
+      <c r="A15" s="8" t="inlineStr">
         <is>
           <t>03/07/2024</t>
         </is>
       </c>
-      <c r="B15" t="inlineStr">
+      <c r="B15" s="8" t="inlineStr">
         <is>
           <t>SO240307002</t>
         </is>
       </c>
-      <c r="C15" t="inlineStr">
-        <is>
-          <t>NO</t>
-        </is>
-      </c>
-      <c r="D15" t="inlineStr">
+      <c r="C15" s="8" t="inlineStr">
+        <is>
+          <t>NO</t>
+        </is>
+      </c>
+      <c r="D15" s="8" t="inlineStr">
         <is>
           <t>ab</t>
         </is>
       </c>
-      <c r="E15" t="inlineStr">
+      <c r="E15" s="8" t="inlineStr">
         <is>
           <t>(787)978-9777</t>
         </is>
       </c>
-      <c r="F15" t="inlineStr">
-        <is>
-          <t>NO</t>
-        </is>
-      </c>
-      <c r="G15" t="inlineStr">
-        <is>
-          <t>NO</t>
-        </is>
-      </c>
-      <c r="H15" t="inlineStr">
+      <c r="F15" s="8" t="inlineStr">
+        <is>
+          <t>NO</t>
+        </is>
+      </c>
+      <c r="G15" s="8" t="inlineStr">
+        <is>
+          <t>NO</t>
+        </is>
+      </c>
+      <c r="H15" s="8" t="inlineStr">
         <is>
           <t>artist</t>
         </is>
       </c>
-      <c r="I15" t="inlineStr">
+      <c r="I15" s="8" t="inlineStr">
         <is>
           <t>title</t>
         </is>
       </c>
-      <c r="J15" t="n">
+      <c r="J15" s="5" t="n">
         <v>5</v>
       </c>
-      <c r="K15" t="n">
+      <c r="K15" s="5" t="n">
         <v>87</v>
       </c>
-      <c r="L15" t="inlineStr">
+      <c r="L15" s="8" t="inlineStr">
         <is>
           <t> </t>
         </is>
       </c>
-      <c r="M15" t="inlineStr">
+      <c r="M15" s="8" t="inlineStr">
         <is>
           <t>AMA</t>
         </is>
       </c>
-      <c r="N15" t="inlineStr">
+      <c r="N15" s="8" t="inlineStr">
         <is>
           <t>CD</t>
         </is>
       </c>
-      <c r="O15" t="inlineStr">
+      <c r="O15" s="8" t="inlineStr">
         <is>
           <t>abake</t>
         </is>
       </c>
-      <c r="P15" t="inlineStr">
+      <c r="P15" s="8" t="inlineStr">
+        <is>
+          <t>PICKUP</t>
+        </is>
+      </c>
+      <c r="Q15" s="8" t="n"/>
+      <c r="R15" s="8" t="n"/>
+      <c r="S15" s="8" t="n"/>
+      <c r="T15" s="8" t="n"/>
+      <c r="U15" s="8" t="n"/>
+      <c r="V15" s="8" t="n"/>
+      <c r="W15" s="8" t="n"/>
+    </row>
+    <row r="16">
+      <c r="A16" t="inlineStr">
+        <is>
+          <t>03/07/2024</t>
+        </is>
+      </c>
+      <c r="B16" t="inlineStr">
+        <is>
+          <t>SO240307003</t>
+        </is>
+      </c>
+      <c r="C16" t="inlineStr">
+        <is>
+          <t>NO</t>
+        </is>
+      </c>
+      <c r="D16" t="inlineStr">
+        <is>
+          <t>ab</t>
+        </is>
+      </c>
+      <c r="E16" t="inlineStr">
+        <is>
+          <t>(885)858-5858</t>
+        </is>
+      </c>
+      <c r="F16" t="inlineStr">
+        <is>
+          <t>NO</t>
+        </is>
+      </c>
+      <c r="G16" t="inlineStr">
+        <is>
+          <t>YES</t>
+        </is>
+      </c>
+      <c r="H16" t="inlineStr">
+        <is>
+          <t>artist</t>
+        </is>
+      </c>
+      <c r="I16" t="inlineStr">
+        <is>
+          <t>title</t>
+        </is>
+      </c>
+      <c r="J16" t="n">
+        <v>10</v>
+      </c>
+      <c r="K16" t="n">
+        <v>89.98999999999999</v>
+      </c>
+      <c r="L16" t="inlineStr">
+        <is>
+          <t> </t>
+        </is>
+      </c>
+      <c r="M16" t="inlineStr">
+        <is>
+          <t>AMA</t>
+        </is>
+      </c>
+      <c r="N16" t="inlineStr">
+        <is>
+          <t>DVD</t>
+        </is>
+      </c>
+      <c r="O16" t="inlineStr">
+        <is>
+          <t>abake</t>
+        </is>
+      </c>
+      <c r="P16" t="inlineStr">
+        <is>
+          <t>PICKUP</t>
+        </is>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" t="inlineStr">
+        <is>
+          <t>03/07/2024</t>
+        </is>
+      </c>
+      <c r="B17" t="inlineStr">
+        <is>
+          <t>SO240307004</t>
+        </is>
+      </c>
+      <c r="C17" t="inlineStr">
+        <is>
+          <t>NO</t>
+        </is>
+      </c>
+      <c r="D17" t="inlineStr">
+        <is>
+          <t>ab</t>
+        </is>
+      </c>
+      <c r="E17" t="inlineStr">
+        <is>
+          <t>(789)789-7897</t>
+        </is>
+      </c>
+      <c r="F17" t="inlineStr">
+        <is>
+          <t>YES</t>
+        </is>
+      </c>
+      <c r="G17" t="inlineStr">
+        <is>
+          <t>NO</t>
+        </is>
+      </c>
+      <c r="H17" t="inlineStr">
+        <is>
+          <t>artist</t>
+        </is>
+      </c>
+      <c r="I17" t="inlineStr">
+        <is>
+          <t>title</t>
+        </is>
+      </c>
+      <c r="J17" t="n">
+        <v>5</v>
+      </c>
+      <c r="K17" t="n">
+        <v>150</v>
+      </c>
+      <c r="L17" t="inlineStr">
+        <is>
+          <t> </t>
+        </is>
+      </c>
+      <c r="M17" t="inlineStr">
+        <is>
+          <t>AMA</t>
+        </is>
+      </c>
+      <c r="N17" t="inlineStr">
+        <is>
+          <t>CD</t>
+        </is>
+      </c>
+      <c r="O17" t="inlineStr">
+        <is>
+          <t>abake</t>
+        </is>
+      </c>
+      <c r="P17" t="inlineStr">
         <is>
           <t>PICKUP</t>
         </is>

</xml_diff>

<commit_message>
modified main, xlfile, and generators -main     - data passed to xlfile is now dictionary     - fixed the behavior of submitting Special     orders to where the user can make other orders     after the other -xlfile     - Added a new function to insert an empty row     before the first Special Order entry of the day     - Added a new function to insert data into xl     from dictionary -generators     - Removed the function that indicates if the     entry is the first entry of the day and adds     an empty row
</commit_message>
<xml_diff>
--- a/SO_Test.xlsx
+++ b/SO_Test.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="245" uniqueCount="91">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="224" uniqueCount="87">
   <si>
     <t>DATE</t>
   </si>
@@ -275,18 +275,6 @@
   </si>
   <si>
     <t>(789)789-7897</t>
-  </si>
-  <si>
-    <t>03/10/2024</t>
-  </si>
-  <si>
-    <t>SO240310001</t>
-  </si>
-  <si>
-    <t>(789)456-1230</t>
-  </si>
-  <si>
-    <t>N/A</t>
   </si>
 </sst>
 </file>
@@ -691,7 +679,7 @@
   <sheetPr>
     <outlinePr summaryBelow="0"/>
   </sheetPr>
-  <dimension ref="A1:AD19"/>
+  <dimension ref="A1:AD17"/>
   <sheetViews>
     <sheetView workbookViewId="0" tabSelected="1"/>
   </sheetViews>
@@ -1767,116 +1755,6 @@
       <c r="AC17" s="3"/>
       <c r="AD17" s="3"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="18" customHeight="1" ht="18.75">
-      <c r="A18" s="3"/>
-      <c r="B18" s="3"/>
-      <c r="C18" s="3"/>
-      <c r="D18" s="3"/>
-      <c r="E18" s="3"/>
-      <c r="F18" s="3"/>
-      <c r="G18" s="3"/>
-      <c r="H18" s="3"/>
-      <c r="I18" s="3"/>
-      <c r="J18" s="3"/>
-      <c r="K18" s="6"/>
-      <c r="L18" s="6"/>
-      <c r="M18" s="3"/>
-      <c r="N18" s="3"/>
-      <c r="O18" s="3"/>
-      <c r="P18" s="3"/>
-      <c r="Q18" s="3"/>
-      <c r="R18" s="5"/>
-      <c r="S18" s="3"/>
-      <c r="T18" s="3"/>
-      <c r="U18" s="3"/>
-      <c r="V18" s="3"/>
-      <c r="W18" s="3"/>
-      <c r="X18" s="3"/>
-      <c r="Y18" s="3"/>
-      <c r="Z18" s="3"/>
-      <c r="AA18" s="3"/>
-      <c r="AB18" s="3"/>
-      <c r="AC18" s="3"/>
-      <c r="AD18" s="3"/>
-    </row>
-    <row x14ac:dyDescent="0.25" r="19" customHeight="1" ht="18.75">
-      <c r="A19" s="3" t="s">
-        <v>87</v>
-      </c>
-      <c r="B19" s="3" t="s">
-        <v>88</v>
-      </c>
-      <c r="C19" s="3" t="s">
-        <v>32</v>
-      </c>
-      <c r="D19" s="3" t="s">
-        <v>33</v>
-      </c>
-      <c r="E19" s="3" t="s">
-        <v>34</v>
-      </c>
-      <c r="F19" s="3" t="s">
-        <v>89</v>
-      </c>
-      <c r="G19" s="3" t="s">
-        <v>36</v>
-      </c>
-      <c r="H19" s="3" t="s">
-        <v>36</v>
-      </c>
-      <c r="I19" s="3" t="s">
-        <v>62</v>
-      </c>
-      <c r="J19" s="3" t="s">
-        <v>63</v>
-      </c>
-      <c r="K19" s="4">
-        <v>5</v>
-      </c>
-      <c r="L19" s="4">
-        <v>35</v>
-      </c>
-      <c r="M19" s="3"/>
-      <c r="N19" s="3" t="s">
-        <v>49</v>
-      </c>
-      <c r="O19" s="3" t="s">
-        <v>43</v>
-      </c>
-      <c r="P19" s="3" t="s">
-        <v>79</v>
-      </c>
-      <c r="Q19" s="3" t="s">
-        <v>80</v>
-      </c>
-      <c r="R19" s="5" t="s">
-        <v>90</v>
-      </c>
-      <c r="S19" s="3" t="s">
-        <v>90</v>
-      </c>
-      <c r="T19" s="3" t="s">
-        <v>90</v>
-      </c>
-      <c r="U19" s="3" t="s">
-        <v>90</v>
-      </c>
-      <c r="V19" s="3" t="s">
-        <v>32</v>
-      </c>
-      <c r="W19" s="3"/>
-      <c r="X19" s="3"/>
-      <c r="Y19" s="3" t="s">
-        <v>32</v>
-      </c>
-      <c r="Z19" s="3"/>
-      <c r="AA19" s="3"/>
-      <c r="AB19" s="3" t="s">
-        <v>32</v>
-      </c>
-      <c r="AC19" s="3"/>
-      <c r="AD19" s="3"/>
-    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
modified main - fixed the issue with the SO Ref Num repeating the same value
</commit_message>
<xml_diff>
--- a/SO_Test.xlsx
+++ b/SO_Test.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:AD21"/>
+  <dimension ref="A1:AD23"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1814,59 +1814,63 @@
     <row r="17">
       <c r="A17" t="inlineStr">
         <is>
-          <t>03/07/2024</t>
+          <t> </t>
         </is>
       </c>
       <c r="B17" t="inlineStr">
         <is>
-          <t>SO240307004</t>
+          <t> </t>
         </is>
       </c>
       <c r="C17" t="inlineStr">
         <is>
-          <t>NO</t>
+          <t> </t>
         </is>
       </c>
       <c r="D17" t="inlineStr">
         <is>
-          <t>ab</t>
+          <t> </t>
         </is>
       </c>
       <c r="E17" t="inlineStr">
         <is>
-          <t>abc@abc.com</t>
+          <t> </t>
         </is>
       </c>
       <c r="F17" t="inlineStr">
         <is>
-          <t>(789)789-7897</t>
+          <t> </t>
         </is>
       </c>
       <c r="G17" t="inlineStr">
         <is>
-          <t>YES</t>
+          <t> </t>
         </is>
       </c>
       <c r="H17" t="inlineStr">
         <is>
-          <t>NO</t>
+          <t> </t>
         </is>
       </c>
       <c r="I17" t="inlineStr">
         <is>
-          <t>artist</t>
+          <t> </t>
         </is>
       </c>
       <c r="J17" t="inlineStr">
         <is>
-          <t>title</t>
-        </is>
-      </c>
-      <c r="K17" t="n">
-        <v>5</v>
-      </c>
-      <c r="L17" t="n">
-        <v>150</v>
+          <t> </t>
+        </is>
+      </c>
+      <c r="K17" t="inlineStr">
+        <is>
+          <t> </t>
+        </is>
+      </c>
+      <c r="L17" t="inlineStr">
+        <is>
+          <t> </t>
+        </is>
       </c>
       <c r="M17" t="inlineStr">
         <is>
@@ -1875,110 +1879,146 @@
       </c>
       <c r="N17" t="inlineStr">
         <is>
-          <t>AMA</t>
+          <t> </t>
         </is>
       </c>
       <c r="O17" t="inlineStr">
         <is>
-          <t>CD</t>
+          <t> </t>
         </is>
       </c>
       <c r="P17" t="inlineStr">
         <is>
-          <t>abake</t>
+          <t> </t>
         </is>
       </c>
       <c r="Q17" t="inlineStr">
         <is>
-          <t>PICKUP</t>
-        </is>
-      </c>
-      <c r="R17" t="inlineStr"/>
-      <c r="S17" t="inlineStr"/>
-      <c r="T17" t="inlineStr"/>
-      <c r="U17" t="inlineStr"/>
+          <t> </t>
+        </is>
+      </c>
+      <c r="R17" t="inlineStr">
+        <is>
+          <t> </t>
+        </is>
+      </c>
+      <c r="S17" t="inlineStr">
+        <is>
+          <t> </t>
+        </is>
+      </c>
+      <c r="T17" t="inlineStr">
+        <is>
+          <t> </t>
+        </is>
+      </c>
+      <c r="U17" t="inlineStr">
+        <is>
+          <t> </t>
+        </is>
+      </c>
       <c r="V17" t="inlineStr">
         <is>
-          <t>NO</t>
-        </is>
-      </c>
-      <c r="W17" t="inlineStr"/>
-      <c r="X17" t="inlineStr"/>
+          <t> </t>
+        </is>
+      </c>
+      <c r="W17" t="inlineStr">
+        <is>
+          <t> </t>
+        </is>
+      </c>
+      <c r="X17" t="inlineStr">
+        <is>
+          <t> </t>
+        </is>
+      </c>
       <c r="Y17" t="inlineStr">
         <is>
-          <t>NO</t>
-        </is>
-      </c>
-      <c r="Z17" t="inlineStr"/>
-      <c r="AA17" t="inlineStr"/>
+          <t> </t>
+        </is>
+      </c>
+      <c r="Z17" t="inlineStr">
+        <is>
+          <t> </t>
+        </is>
+      </c>
+      <c r="AA17" t="inlineStr">
+        <is>
+          <t> </t>
+        </is>
+      </c>
       <c r="AB17" t="inlineStr">
         <is>
-          <t>NO</t>
-        </is>
-      </c>
-      <c r="AC17" t="inlineStr"/>
-      <c r="AD17" t="inlineStr"/>
+          <t> </t>
+        </is>
+      </c>
+      <c r="AC17" t="inlineStr">
+        <is>
+          <t> </t>
+        </is>
+      </c>
+      <c r="AD17" t="inlineStr">
+        <is>
+          <t> </t>
+        </is>
+      </c>
     </row>
     <row r="18">
       <c r="A18" t="inlineStr">
         <is>
-          <t> </t>
+          <t>03/11/2024</t>
         </is>
       </c>
       <c r="B18" t="inlineStr">
         <is>
-          <t> </t>
+          <t>SO240311001</t>
         </is>
       </c>
       <c r="C18" t="inlineStr">
         <is>
-          <t> </t>
+          <t>NO</t>
         </is>
       </c>
       <c r="D18" t="inlineStr">
         <is>
-          <t> </t>
+          <t>ab</t>
         </is>
       </c>
       <c r="E18" t="inlineStr">
         <is>
-          <t> </t>
+          <t>abc@abc.com</t>
         </is>
       </c>
       <c r="F18" t="inlineStr">
         <is>
-          <t> </t>
+          <t xml:space="preserve">(789)456-1230 </t>
         </is>
       </c>
       <c r="G18" t="inlineStr">
         <is>
-          <t> </t>
+          <t>YES</t>
         </is>
       </c>
       <c r="H18" t="inlineStr">
         <is>
-          <t> </t>
+          <t>YES</t>
         </is>
       </c>
       <c r="I18" t="inlineStr">
         <is>
-          <t> </t>
+          <t>artist</t>
         </is>
       </c>
       <c r="J18" t="inlineStr">
         <is>
-          <t> </t>
-        </is>
-      </c>
-      <c r="K18" t="inlineStr">
-        <is>
-          <t> </t>
-        </is>
-      </c>
-      <c r="L18" t="inlineStr">
-        <is>
-          <t> </t>
-        </is>
+          <t>title</t>
+        </is>
+      </c>
+      <c r="K18" t="n">
+        <v>5</v>
+      </c>
+      <c r="L18" t="n">
+        <v>15</v>
       </c>
       <c r="M18" t="inlineStr">
         <is>
@@ -1987,150 +2027,106 @@
       </c>
       <c r="N18" t="inlineStr">
         <is>
-          <t> </t>
+          <t>AMS</t>
         </is>
       </c>
       <c r="O18" t="inlineStr">
         <is>
-          <t> </t>
+          <t>LP</t>
         </is>
       </c>
       <c r="P18" t="inlineStr">
         <is>
-          <t> </t>
+          <t>abake</t>
         </is>
       </c>
       <c r="Q18" t="inlineStr">
         <is>
-          <t> </t>
-        </is>
-      </c>
-      <c r="R18" t="inlineStr">
-        <is>
-          <t> </t>
-        </is>
-      </c>
-      <c r="S18" t="inlineStr">
-        <is>
-          <t> </t>
-        </is>
-      </c>
-      <c r="T18" t="inlineStr">
-        <is>
-          <t> </t>
-        </is>
-      </c>
-      <c r="U18" t="inlineStr">
-        <is>
-          <t> </t>
-        </is>
-      </c>
+          <t>PICKUP</t>
+        </is>
+      </c>
+      <c r="R18" t="inlineStr"/>
+      <c r="S18" t="inlineStr"/>
+      <c r="T18" t="inlineStr"/>
+      <c r="U18" t="inlineStr"/>
       <c r="V18" t="inlineStr">
         <is>
-          <t> </t>
-        </is>
-      </c>
-      <c r="W18" t="inlineStr">
-        <is>
-          <t> </t>
-        </is>
-      </c>
-      <c r="X18" t="inlineStr">
-        <is>
-          <t> </t>
-        </is>
-      </c>
+          <t>NO</t>
+        </is>
+      </c>
+      <c r="W18" t="inlineStr"/>
+      <c r="X18" t="inlineStr"/>
       <c r="Y18" t="inlineStr">
         <is>
-          <t> </t>
-        </is>
-      </c>
-      <c r="Z18" t="inlineStr">
-        <is>
-          <t> </t>
-        </is>
-      </c>
-      <c r="AA18" t="inlineStr">
-        <is>
-          <t> </t>
-        </is>
-      </c>
+          <t>NO</t>
+        </is>
+      </c>
+      <c r="Z18" t="inlineStr"/>
+      <c r="AA18" t="inlineStr"/>
       <c r="AB18" t="inlineStr">
         <is>
-          <t> </t>
-        </is>
-      </c>
-      <c r="AC18" t="inlineStr">
-        <is>
-          <t> </t>
-        </is>
-      </c>
-      <c r="AD18" t="inlineStr">
-        <is>
-          <t> </t>
-        </is>
-      </c>
+          <t>NO</t>
+        </is>
+      </c>
+      <c r="AC18" t="inlineStr"/>
+      <c r="AD18" t="inlineStr"/>
     </row>
     <row r="19">
       <c r="A19" t="inlineStr">
         <is>
-          <t> </t>
+          <t>03/11/2024</t>
         </is>
       </c>
       <c r="B19" t="inlineStr">
         <is>
-          <t> </t>
+          <t>SO240311002</t>
         </is>
       </c>
       <c r="C19" t="inlineStr">
         <is>
-          <t> </t>
+          <t>NO</t>
         </is>
       </c>
       <c r="D19" t="inlineStr">
         <is>
-          <t> </t>
+          <t>ab</t>
         </is>
       </c>
       <c r="E19" t="inlineStr">
         <is>
-          <t> </t>
+          <t>asdsf</t>
         </is>
       </c>
       <c r="F19" t="inlineStr">
         <is>
-          <t> </t>
+          <t>(789)465-1230</t>
         </is>
       </c>
       <c r="G19" t="inlineStr">
         <is>
-          <t> </t>
+          <t>YES</t>
         </is>
       </c>
       <c r="H19" t="inlineStr">
         <is>
-          <t> </t>
+          <t>YES</t>
         </is>
       </c>
       <c r="I19" t="inlineStr">
         <is>
-          <t> </t>
+          <t>artist</t>
         </is>
       </c>
       <c r="J19" t="inlineStr">
         <is>
-          <t> </t>
-        </is>
-      </c>
-      <c r="K19" t="inlineStr">
-        <is>
-          <t> </t>
-        </is>
-      </c>
-      <c r="L19" t="inlineStr">
-        <is>
-          <t> </t>
-        </is>
+          <t>title</t>
+        </is>
+      </c>
+      <c r="K19" t="n">
+        <v>10</v>
+      </c>
+      <c r="L19" t="n">
+        <v>50.99</v>
       </c>
       <c r="M19" t="inlineStr">
         <is>
@@ -2139,99 +2135,75 @@
       </c>
       <c r="N19" t="inlineStr">
         <is>
-          <t> </t>
+          <t>AMS</t>
         </is>
       </c>
       <c r="O19" t="inlineStr">
         <is>
-          <t> </t>
+          <t>LP</t>
         </is>
       </c>
       <c r="P19" t="inlineStr">
         <is>
-          <t> </t>
+          <t>abake</t>
         </is>
       </c>
       <c r="Q19" t="inlineStr">
         <is>
-          <t> </t>
+          <t>SHIPPING</t>
         </is>
       </c>
       <c r="R19" t="inlineStr">
         <is>
-          <t> </t>
+          <t>2120 Septiembre dr</t>
         </is>
       </c>
       <c r="S19" t="inlineStr">
         <is>
-          <t> </t>
+          <t>ELPaso</t>
         </is>
       </c>
       <c r="T19" t="inlineStr">
         <is>
-          <t> </t>
+          <t>TX</t>
         </is>
       </c>
       <c r="U19" t="inlineStr">
         <is>
-          <t> </t>
+          <t>79935</t>
         </is>
       </c>
       <c r="V19" t="inlineStr">
         <is>
-          <t> </t>
-        </is>
-      </c>
-      <c r="W19" t="inlineStr">
-        <is>
-          <t> </t>
-        </is>
-      </c>
-      <c r="X19" t="inlineStr">
-        <is>
-          <t> </t>
-        </is>
-      </c>
+          <t>NO</t>
+        </is>
+      </c>
+      <c r="W19" t="inlineStr"/>
+      <c r="X19" t="inlineStr"/>
       <c r="Y19" t="inlineStr">
         <is>
-          <t> </t>
-        </is>
-      </c>
-      <c r="Z19" t="inlineStr">
-        <is>
-          <t> </t>
-        </is>
-      </c>
-      <c r="AA19" t="inlineStr">
-        <is>
-          <t> </t>
-        </is>
-      </c>
+          <t>NO</t>
+        </is>
+      </c>
+      <c r="Z19" t="inlineStr"/>
+      <c r="AA19" t="inlineStr"/>
       <c r="AB19" t="inlineStr">
         <is>
-          <t> </t>
-        </is>
-      </c>
-      <c r="AC19" t="inlineStr">
-        <is>
-          <t> </t>
-        </is>
-      </c>
-      <c r="AD19" t="inlineStr">
-        <is>
-          <t> </t>
-        </is>
-      </c>
+          <t>NO</t>
+        </is>
+      </c>
+      <c r="AC19" t="inlineStr"/>
+      <c r="AD19" t="inlineStr"/>
     </row>
     <row r="20">
       <c r="A20" t="inlineStr">
         <is>
-          <t>03/10/2024</t>
+          <t>03/11/2024</t>
         </is>
       </c>
       <c r="B20" t="inlineStr">
         <is>
-          <t>SO240310001</t>
+          <t>SO240311003</t>
         </is>
       </c>
       <c r="C20" t="inlineStr">
@@ -2246,12 +2218,12 @@
       </c>
       <c r="E20" t="inlineStr">
         <is>
-          <t>adsf</t>
+          <t>ab</t>
         </is>
       </c>
       <c r="F20" t="inlineStr">
         <is>
-          <t>(789)456-1233</t>
+          <t>(789)123-4567</t>
         </is>
       </c>
       <c r="G20" t="inlineStr">
@@ -2261,24 +2233,24 @@
       </c>
       <c r="H20" t="inlineStr">
         <is>
-          <t>NO</t>
+          <t>YES</t>
         </is>
       </c>
       <c r="I20" t="inlineStr">
         <is>
-          <t>ad</t>
+          <t>artist</t>
         </is>
       </c>
       <c r="J20" t="inlineStr">
         <is>
-          <t>fgd</t>
+          <t>title</t>
         </is>
       </c>
       <c r="K20" t="n">
         <v>5</v>
       </c>
       <c r="L20" t="n">
-        <v>30</v>
+        <v>90</v>
       </c>
       <c r="M20" t="inlineStr">
         <is>
@@ -2292,7 +2264,7 @@
       </c>
       <c r="O20" t="inlineStr">
         <is>
-          <t>CD</t>
+          <t>OTHER</t>
         </is>
       </c>
       <c r="P20" t="inlineStr">
@@ -2334,12 +2306,12 @@
     <row r="21">
       <c r="A21" t="inlineStr">
         <is>
-          <t>03/10/2024</t>
+          <t>03/11/2024</t>
         </is>
       </c>
       <c r="B21" t="inlineStr">
         <is>
-          <t>SO240310001</t>
+          <t>SO240311004</t>
         </is>
       </c>
       <c r="C21" t="inlineStr">
@@ -2349,17 +2321,17 @@
       </c>
       <c r="D21" t="inlineStr">
         <is>
+          <t>Ashley</t>
+        </is>
+      </c>
+      <c r="E21" t="inlineStr">
+        <is>
           <t>ab</t>
         </is>
       </c>
-      <c r="E21" t="inlineStr">
-        <is>
-          <t>ldifger</t>
-        </is>
-      </c>
       <c r="F21" t="inlineStr">
         <is>
-          <t>(789)456-1233</t>
+          <t>(159)753-2856</t>
         </is>
       </c>
       <c r="G21" t="inlineStr">
@@ -2374,19 +2346,19 @@
       </c>
       <c r="I21" t="inlineStr">
         <is>
-          <t>tres</t>
+          <t>artist</t>
         </is>
       </c>
       <c r="J21" t="inlineStr">
         <is>
-          <t>tres</t>
+          <t>title</t>
         </is>
       </c>
       <c r="K21" t="n">
-        <v>10</v>
+        <v>60</v>
       </c>
       <c r="L21" t="n">
-        <v>85</v>
+        <v>822</v>
       </c>
       <c r="M21" t="inlineStr">
         <is>
@@ -2395,7 +2367,7 @@
       </c>
       <c r="N21" t="inlineStr">
         <is>
-          <t>AMS</t>
+          <t>AEC</t>
         </is>
       </c>
       <c r="O21" t="inlineStr">
@@ -2413,26 +2385,10 @@
           <t>PICKUP</t>
         </is>
       </c>
-      <c r="R21" t="inlineStr">
-        <is>
-          <t>N/A</t>
-        </is>
-      </c>
-      <c r="S21" t="inlineStr">
-        <is>
-          <t>N/A</t>
-        </is>
-      </c>
-      <c r="T21" t="inlineStr">
-        <is>
-          <t>N/A</t>
-        </is>
-      </c>
-      <c r="U21" t="inlineStr">
-        <is>
-          <t>N/A</t>
-        </is>
-      </c>
+      <c r="R21" t="inlineStr"/>
+      <c r="S21" t="inlineStr"/>
+      <c r="T21" t="inlineStr"/>
+      <c r="U21" t="inlineStr"/>
       <c r="V21" t="inlineStr">
         <is>
           <t>NO</t>
@@ -2454,6 +2410,238 @@
       </c>
       <c r="AC21" t="inlineStr"/>
       <c r="AD21" t="inlineStr"/>
+    </row>
+    <row r="22">
+      <c r="A22" t="inlineStr">
+        <is>
+          <t>03/11/2024</t>
+        </is>
+      </c>
+      <c r="B22" t="inlineStr">
+        <is>
+          <t>SO240311005</t>
+        </is>
+      </c>
+      <c r="C22" t="inlineStr">
+        <is>
+          <t>NO</t>
+        </is>
+      </c>
+      <c r="D22" t="inlineStr">
+        <is>
+          <t>ab</t>
+        </is>
+      </c>
+      <c r="E22" t="inlineStr">
+        <is>
+          <t>ababa</t>
+        </is>
+      </c>
+      <c r="F22" t="inlineStr">
+        <is>
+          <t>(789)456-1230</t>
+        </is>
+      </c>
+      <c r="G22" t="inlineStr">
+        <is>
+          <t>YES</t>
+        </is>
+      </c>
+      <c r="H22" t="inlineStr">
+        <is>
+          <t>YES</t>
+        </is>
+      </c>
+      <c r="I22" t="inlineStr">
+        <is>
+          <t>artist</t>
+        </is>
+      </c>
+      <c r="J22" t="inlineStr">
+        <is>
+          <t>title`</t>
+        </is>
+      </c>
+      <c r="K22" t="n">
+        <v>9</v>
+      </c>
+      <c r="L22" t="n">
+        <v>55</v>
+      </c>
+      <c r="M22" t="inlineStr">
+        <is>
+          <t> </t>
+        </is>
+      </c>
+      <c r="N22" t="inlineStr">
+        <is>
+          <t>AEC</t>
+        </is>
+      </c>
+      <c r="O22" t="inlineStr">
+        <is>
+          <t>LP</t>
+        </is>
+      </c>
+      <c r="P22" t="inlineStr">
+        <is>
+          <t>abake</t>
+        </is>
+      </c>
+      <c r="Q22" t="inlineStr">
+        <is>
+          <t>PICKUP</t>
+        </is>
+      </c>
+      <c r="R22" t="inlineStr"/>
+      <c r="S22" t="inlineStr"/>
+      <c r="T22" t="inlineStr"/>
+      <c r="U22" t="inlineStr"/>
+      <c r="V22" t="inlineStr">
+        <is>
+          <t>NO</t>
+        </is>
+      </c>
+      <c r="W22" t="inlineStr"/>
+      <c r="X22" t="inlineStr"/>
+      <c r="Y22" t="inlineStr">
+        <is>
+          <t>NO</t>
+        </is>
+      </c>
+      <c r="Z22" t="inlineStr"/>
+      <c r="AA22" t="inlineStr"/>
+      <c r="AB22" t="inlineStr">
+        <is>
+          <t>NO</t>
+        </is>
+      </c>
+      <c r="AC22" t="inlineStr"/>
+      <c r="AD22" t="inlineStr"/>
+    </row>
+    <row r="23">
+      <c r="A23" t="inlineStr">
+        <is>
+          <t>03/11/2024</t>
+        </is>
+      </c>
+      <c r="B23" t="inlineStr">
+        <is>
+          <t>SO240311006</t>
+        </is>
+      </c>
+      <c r="C23" t="inlineStr">
+        <is>
+          <t>NO</t>
+        </is>
+      </c>
+      <c r="D23" t="inlineStr">
+        <is>
+          <t>ab</t>
+        </is>
+      </c>
+      <c r="E23" t="inlineStr">
+        <is>
+          <t>ababababa</t>
+        </is>
+      </c>
+      <c r="F23" t="inlineStr">
+        <is>
+          <t>(528)525-8225</t>
+        </is>
+      </c>
+      <c r="G23" t="inlineStr">
+        <is>
+          <t>YES</t>
+        </is>
+      </c>
+      <c r="H23" t="inlineStr">
+        <is>
+          <t>YES</t>
+        </is>
+      </c>
+      <c r="I23" t="inlineStr">
+        <is>
+          <t>art</t>
+        </is>
+      </c>
+      <c r="J23" t="inlineStr">
+        <is>
+          <t>title</t>
+        </is>
+      </c>
+      <c r="K23" t="n">
+        <v>16</v>
+      </c>
+      <c r="L23" t="n">
+        <v>98</v>
+      </c>
+      <c r="M23" t="inlineStr">
+        <is>
+          <t> </t>
+        </is>
+      </c>
+      <c r="N23" t="inlineStr">
+        <is>
+          <t>me</t>
+        </is>
+      </c>
+      <c r="O23" t="inlineStr">
+        <is>
+          <t>BLU-RAY</t>
+        </is>
+      </c>
+      <c r="P23" t="inlineStr">
+        <is>
+          <t>abake</t>
+        </is>
+      </c>
+      <c r="Q23" t="inlineStr">
+        <is>
+          <t>PICKUP</t>
+        </is>
+      </c>
+      <c r="R23" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="S23" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="T23" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="U23" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="V23" t="inlineStr">
+        <is>
+          <t>NO</t>
+        </is>
+      </c>
+      <c r="W23" t="inlineStr"/>
+      <c r="X23" t="inlineStr"/>
+      <c r="Y23" t="inlineStr">
+        <is>
+          <t>NO</t>
+        </is>
+      </c>
+      <c r="Z23" t="inlineStr"/>
+      <c r="AA23" t="inlineStr"/>
+      <c r="AB23" t="inlineStr">
+        <is>
+          <t>NO</t>
+        </is>
+      </c>
+      <c r="AC23" t="inlineStr"/>
+      <c r="AD23" t="inlineStr"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>

<commit_message>
Modified main.py - SO_Update_Frame() class     - now the selected order will display what options         are available for the selected order to complete         and will list the options that are already         completed by who and when underneath the         "Confirm" button     - Need to have it automatically clear the completed         options after the "Confirm" button is pressed         and ultimately remove the "Confirm" button         once all the options are completed and that moment
</commit_message>
<xml_diff>
--- a/SO_Test.xlsx
+++ b/SO_Test.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:AD23"/>
+  <dimension ref="A1:AD24"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -2843,6 +2843,138 @@
         </is>
       </c>
     </row>
+    <row r="24">
+      <c r="A24" t="inlineStr">
+        <is>
+          <t>03/11/2024</t>
+        </is>
+      </c>
+      <c r="B24" t="inlineStr">
+        <is>
+          <t>SO240311007</t>
+        </is>
+      </c>
+      <c r="C24" t="inlineStr">
+        <is>
+          <t>YES</t>
+        </is>
+      </c>
+      <c r="D24" t="inlineStr">
+        <is>
+          <t>ab</t>
+        </is>
+      </c>
+      <c r="E24" t="inlineStr">
+        <is>
+          <t>asdfjkhl</t>
+        </is>
+      </c>
+      <c r="F24" t="inlineStr">
+        <is>
+          <t>(789)456-1230</t>
+        </is>
+      </c>
+      <c r="G24" t="inlineStr">
+        <is>
+          <t>YES</t>
+        </is>
+      </c>
+      <c r="H24" t="inlineStr">
+        <is>
+          <t>YES</t>
+        </is>
+      </c>
+      <c r="I24" t="inlineStr">
+        <is>
+          <t>aszdg</t>
+        </is>
+      </c>
+      <c r="J24" t="inlineStr">
+        <is>
+          <t>adfsg</t>
+        </is>
+      </c>
+      <c r="K24" t="n">
+        <v>50</v>
+      </c>
+      <c r="L24" t="n">
+        <v>900</v>
+      </c>
+      <c r="M24" t="inlineStr">
+        <is>
+          <t> </t>
+        </is>
+      </c>
+      <c r="N24" t="inlineStr">
+        <is>
+          <t>ytouse</t>
+        </is>
+      </c>
+      <c r="O24" t="inlineStr">
+        <is>
+          <t>DVD</t>
+        </is>
+      </c>
+      <c r="P24" t="inlineStr">
+        <is>
+          <t>abake</t>
+        </is>
+      </c>
+      <c r="Q24" t="inlineStr">
+        <is>
+          <t>PICKUP</t>
+        </is>
+      </c>
+      <c r="R24" t="inlineStr"/>
+      <c r="S24" t="inlineStr"/>
+      <c r="T24" t="inlineStr"/>
+      <c r="U24" t="inlineStr"/>
+      <c r="V24" t="inlineStr">
+        <is>
+          <t>YES</t>
+        </is>
+      </c>
+      <c r="W24" t="inlineStr">
+        <is>
+          <t>03/11/2024</t>
+        </is>
+      </c>
+      <c r="X24" t="inlineStr">
+        <is>
+          <t>abake</t>
+        </is>
+      </c>
+      <c r="Y24" t="inlineStr">
+        <is>
+          <t>YES</t>
+        </is>
+      </c>
+      <c r="Z24" t="inlineStr">
+        <is>
+          <t>03/11/2024</t>
+        </is>
+      </c>
+      <c r="AA24" t="inlineStr">
+        <is>
+          <t>abake</t>
+        </is>
+      </c>
+      <c r="AB24" t="inlineStr">
+        <is>
+          <t>YES</t>
+        </is>
+      </c>
+      <c r="AC24" t="inlineStr">
+        <is>
+          <t>03/11/2024</t>
+        </is>
+      </c>
+      <c r="AD24" t="inlineStr">
+        <is>
+          <t>abake</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
modified main - added other comments for intended changes and additions
</commit_message>
<xml_diff>
--- a/SO_Test.xlsx
+++ b/SO_Test.xlsx
@@ -598,7 +598,7 @@
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>NO</t>
+          <t>YES</t>
         </is>
       </c>
       <c r="D2" t="inlineStr">
@@ -642,6 +642,7 @@
       <c r="L2" t="n">
         <v>24</v>
       </c>
+      <c r="M2" t="inlineStr"/>
       <c r="N2" t="inlineStr">
         <is>
           <t>Vendors</t>
@@ -662,21 +663,87 @@
           <t>NO</t>
         </is>
       </c>
+      <c r="R2" t="inlineStr"/>
+      <c r="S2" t="inlineStr"/>
+      <c r="T2" t="inlineStr"/>
+      <c r="U2" t="inlineStr"/>
       <c r="V2" t="inlineStr">
         <is>
-          <t>NO</t>
+          <t>YES</t>
+        </is>
+      </c>
+      <c r="W2" t="inlineStr">
+        <is>
+          <t>03/12/2024</t>
+        </is>
+      </c>
+      <c r="X2" t="inlineStr">
+        <is>
+          <t>abake</t>
         </is>
       </c>
       <c r="Y2" t="inlineStr">
         <is>
-          <t>NO</t>
+          <t>YES</t>
+        </is>
+      </c>
+      <c r="Z2" t="inlineStr">
+        <is>
+          <t>03/12/2024</t>
+        </is>
+      </c>
+      <c r="AA2" t="inlineStr">
+        <is>
+          <t>abake</t>
         </is>
       </c>
       <c r="AB2" t="inlineStr">
         <is>
-          <t>NO</t>
-        </is>
-      </c>
+          <t>YES</t>
+        </is>
+      </c>
+      <c r="AC2" t="inlineStr">
+        <is>
+          <t>03/12/2024</t>
+        </is>
+      </c>
+      <c r="AD2" t="inlineStr">
+        <is>
+          <t>abake</t>
+        </is>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="inlineStr"/>
+      <c r="B3" t="inlineStr"/>
+      <c r="C3" t="inlineStr"/>
+      <c r="D3" t="inlineStr"/>
+      <c r="E3" t="inlineStr"/>
+      <c r="F3" t="inlineStr"/>
+      <c r="G3" t="inlineStr"/>
+      <c r="H3" t="inlineStr"/>
+      <c r="I3" t="inlineStr"/>
+      <c r="J3" t="inlineStr"/>
+      <c r="K3" t="inlineStr"/>
+      <c r="L3" t="inlineStr"/>
+      <c r="M3" t="inlineStr"/>
+      <c r="N3" t="inlineStr"/>
+      <c r="O3" t="inlineStr"/>
+      <c r="P3" t="inlineStr"/>
+      <c r="Q3" t="inlineStr"/>
+      <c r="R3" t="inlineStr"/>
+      <c r="S3" t="inlineStr"/>
+      <c r="T3" t="inlineStr"/>
+      <c r="U3" t="inlineStr"/>
+      <c r="V3" t="inlineStr"/>
+      <c r="W3" t="inlineStr"/>
+      <c r="X3" t="inlineStr"/>
+      <c r="Y3" t="inlineStr"/>
+      <c r="Z3" t="inlineStr"/>
+      <c r="AA3" t="inlineStr"/>
+      <c r="AB3" t="inlineStr"/>
+      <c r="AC3" t="inlineStr"/>
+      <c r="AD3" t="inlineStr"/>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
@@ -691,7 +758,7 @@
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>NO</t>
+          <t>YES</t>
         </is>
       </c>
       <c r="D4" t="inlineStr">
@@ -735,6 +802,7 @@
       <c r="L4" t="n">
         <v>34</v>
       </c>
+      <c r="M4" t="inlineStr"/>
       <c r="N4" t="inlineStr">
         <is>
           <t>AMA</t>
@@ -755,6 +823,10 @@
           <t>NO</t>
         </is>
       </c>
+      <c r="R4" t="inlineStr"/>
+      <c r="S4" t="inlineStr"/>
+      <c r="T4" t="inlineStr"/>
+      <c r="U4" t="inlineStr"/>
       <c r="V4" t="inlineStr">
         <is>
           <t>YES</t>
@@ -787,7 +859,17 @@
       </c>
       <c r="AB4" t="inlineStr">
         <is>
-          <t>NO</t>
+          <t>YES</t>
+        </is>
+      </c>
+      <c r="AC4" t="inlineStr">
+        <is>
+          <t>03/12/2024</t>
+        </is>
+      </c>
+      <c r="AD4" t="inlineStr">
+        <is>
+          <t>abake</t>
         </is>
       </c>
     </row>
@@ -848,6 +930,7 @@
       <c r="L5" t="n">
         <v>49.99</v>
       </c>
+      <c r="M5" t="inlineStr"/>
       <c r="N5" t="inlineStr">
         <is>
           <t>AMS</t>
@@ -891,16 +974,54 @@
           <t>NO</t>
         </is>
       </c>
+      <c r="W5" t="inlineStr"/>
+      <c r="X5" t="inlineStr"/>
       <c r="Y5" t="inlineStr">
         <is>
           <t>NO</t>
         </is>
       </c>
+      <c r="Z5" t="inlineStr"/>
+      <c r="AA5" t="inlineStr"/>
       <c r="AB5" t="inlineStr">
         <is>
           <t>NO</t>
         </is>
       </c>
+      <c r="AC5" t="inlineStr"/>
+      <c r="AD5" t="inlineStr"/>
+    </row>
+    <row r="6">
+      <c r="A6" t="inlineStr"/>
+      <c r="B6" t="inlineStr"/>
+      <c r="C6" t="inlineStr"/>
+      <c r="D6" t="inlineStr"/>
+      <c r="E6" t="inlineStr"/>
+      <c r="F6" t="inlineStr"/>
+      <c r="G6" t="inlineStr"/>
+      <c r="H6" t="inlineStr"/>
+      <c r="I6" t="inlineStr"/>
+      <c r="J6" t="inlineStr"/>
+      <c r="K6" t="inlineStr"/>
+      <c r="L6" t="inlineStr"/>
+      <c r="M6" t="inlineStr"/>
+      <c r="N6" t="inlineStr"/>
+      <c r="O6" t="inlineStr"/>
+      <c r="P6" t="inlineStr"/>
+      <c r="Q6" t="inlineStr"/>
+      <c r="R6" t="inlineStr"/>
+      <c r="S6" t="inlineStr"/>
+      <c r="T6" t="inlineStr"/>
+      <c r="U6" t="inlineStr"/>
+      <c r="V6" t="inlineStr"/>
+      <c r="W6" t="inlineStr"/>
+      <c r="X6" t="inlineStr"/>
+      <c r="Y6" t="inlineStr"/>
+      <c r="Z6" t="inlineStr"/>
+      <c r="AA6" t="inlineStr"/>
+      <c r="AB6" t="inlineStr"/>
+      <c r="AC6" t="inlineStr"/>
+      <c r="AD6" t="inlineStr"/>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
@@ -915,7 +1036,7 @@
       </c>
       <c r="C7" t="inlineStr">
         <is>
-          <t>NO</t>
+          <t>YES</t>
         </is>
       </c>
       <c r="D7" t="inlineStr">
@@ -959,6 +1080,7 @@
       <c r="L7" t="n">
         <v>50.2</v>
       </c>
+      <c r="M7" t="inlineStr"/>
       <c r="N7" t="inlineStr">
         <is>
           <t>AMS</t>
@@ -979,6 +1101,10 @@
           <t>NO</t>
         </is>
       </c>
+      <c r="R7" t="inlineStr"/>
+      <c r="S7" t="inlineStr"/>
+      <c r="T7" t="inlineStr"/>
+      <c r="U7" t="inlineStr"/>
       <c r="V7" t="inlineStr">
         <is>
           <t>YES</t>
@@ -1011,9 +1137,51 @@
       </c>
       <c r="AB7" t="inlineStr">
         <is>
-          <t>NO</t>
-        </is>
-      </c>
+          <t>YES</t>
+        </is>
+      </c>
+      <c r="AC7" t="inlineStr">
+        <is>
+          <t>03/12/2024</t>
+        </is>
+      </c>
+      <c r="AD7" t="inlineStr">
+        <is>
+          <t>abake</t>
+        </is>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="inlineStr"/>
+      <c r="B8" t="inlineStr"/>
+      <c r="C8" t="inlineStr"/>
+      <c r="D8" t="inlineStr"/>
+      <c r="E8" t="inlineStr"/>
+      <c r="F8" t="inlineStr"/>
+      <c r="G8" t="inlineStr"/>
+      <c r="H8" t="inlineStr"/>
+      <c r="I8" t="inlineStr"/>
+      <c r="J8" t="inlineStr"/>
+      <c r="K8" t="inlineStr"/>
+      <c r="L8" t="inlineStr"/>
+      <c r="M8" t="inlineStr"/>
+      <c r="N8" t="inlineStr"/>
+      <c r="O8" t="inlineStr"/>
+      <c r="P8" t="inlineStr"/>
+      <c r="Q8" t="inlineStr"/>
+      <c r="R8" t="inlineStr"/>
+      <c r="S8" t="inlineStr"/>
+      <c r="T8" t="inlineStr"/>
+      <c r="U8" t="inlineStr"/>
+      <c r="V8" t="inlineStr"/>
+      <c r="W8" t="inlineStr"/>
+      <c r="X8" t="inlineStr"/>
+      <c r="Y8" t="inlineStr"/>
+      <c r="Z8" t="inlineStr"/>
+      <c r="AA8" t="inlineStr"/>
+      <c r="AB8" t="inlineStr"/>
+      <c r="AC8" t="inlineStr"/>
+      <c r="AD8" t="inlineStr"/>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
@@ -1072,6 +1240,7 @@
       <c r="L9" t="n">
         <v>58.63</v>
       </c>
+      <c r="M9" t="inlineStr"/>
       <c r="N9" t="inlineStr">
         <is>
           <t>AMS</t>
@@ -1082,26 +1251,69 @@
           <t>LP</t>
         </is>
       </c>
+      <c r="P9" t="inlineStr"/>
       <c r="Q9" t="inlineStr">
         <is>
           <t>NO</t>
         </is>
       </c>
+      <c r="R9" t="inlineStr"/>
+      <c r="S9" t="inlineStr"/>
+      <c r="T9" t="inlineStr"/>
+      <c r="U9" t="inlineStr"/>
       <c r="V9" t="inlineStr">
         <is>
           <t>NO</t>
         </is>
       </c>
+      <c r="W9" t="inlineStr"/>
+      <c r="X9" t="inlineStr"/>
       <c r="Y9" t="inlineStr">
         <is>
           <t>NO</t>
         </is>
       </c>
+      <c r="Z9" t="inlineStr"/>
+      <c r="AA9" t="inlineStr"/>
       <c r="AB9" t="inlineStr">
         <is>
           <t>NO</t>
         </is>
       </c>
+      <c r="AC9" t="inlineStr"/>
+      <c r="AD9" t="inlineStr"/>
+    </row>
+    <row r="10">
+      <c r="A10" t="inlineStr"/>
+      <c r="B10" t="inlineStr"/>
+      <c r="C10" t="inlineStr"/>
+      <c r="D10" t="inlineStr"/>
+      <c r="E10" t="inlineStr"/>
+      <c r="F10" t="inlineStr"/>
+      <c r="G10" t="inlineStr"/>
+      <c r="H10" t="inlineStr"/>
+      <c r="I10" t="inlineStr"/>
+      <c r="J10" t="inlineStr"/>
+      <c r="K10" t="inlineStr"/>
+      <c r="L10" t="inlineStr"/>
+      <c r="M10" t="inlineStr"/>
+      <c r="N10" t="inlineStr"/>
+      <c r="O10" t="inlineStr"/>
+      <c r="P10" t="inlineStr"/>
+      <c r="Q10" t="inlineStr"/>
+      <c r="R10" t="inlineStr"/>
+      <c r="S10" t="inlineStr"/>
+      <c r="T10" t="inlineStr"/>
+      <c r="U10" t="inlineStr"/>
+      <c r="V10" t="inlineStr"/>
+      <c r="W10" t="inlineStr"/>
+      <c r="X10" t="inlineStr"/>
+      <c r="Y10" t="inlineStr"/>
+      <c r="Z10" t="inlineStr"/>
+      <c r="AA10" t="inlineStr"/>
+      <c r="AB10" t="inlineStr"/>
+      <c r="AC10" t="inlineStr"/>
+      <c r="AD10" t="inlineStr"/>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr">
@@ -1160,6 +1372,7 @@
       <c r="L11" t="n">
         <v>199</v>
       </c>
+      <c r="M11" t="inlineStr"/>
       <c r="N11" t="inlineStr">
         <is>
           <t>AMA</t>
@@ -1180,21 +1393,31 @@
           <t>NO</t>
         </is>
       </c>
+      <c r="R11" t="inlineStr"/>
+      <c r="S11" t="inlineStr"/>
+      <c r="T11" t="inlineStr"/>
+      <c r="U11" t="inlineStr"/>
       <c r="V11" t="inlineStr">
         <is>
           <t>NO</t>
         </is>
       </c>
+      <c r="W11" t="inlineStr"/>
+      <c r="X11" t="inlineStr"/>
       <c r="Y11" t="inlineStr">
         <is>
           <t>NO</t>
         </is>
       </c>
+      <c r="Z11" t="inlineStr"/>
+      <c r="AA11" t="inlineStr"/>
       <c r="AB11" t="inlineStr">
         <is>
           <t>NO</t>
         </is>
       </c>
+      <c r="AC11" t="inlineStr"/>
+      <c r="AD11" t="inlineStr"/>
     </row>
     <row r="12">
       <c r="A12" t="inlineStr">
@@ -1253,11 +1476,7 @@
       <c r="L12" t="n">
         <v>15</v>
       </c>
-      <c r="M12" t="inlineStr">
-        <is>
-          <t> </t>
-        </is>
-      </c>
+      <c r="M12" t="inlineStr"/>
       <c r="N12" t="inlineStr">
         <is>
           <t>AMA</t>
@@ -1278,9 +1497,23 @@
           <t>NO</t>
         </is>
       </c>
+      <c r="R12" t="inlineStr"/>
+      <c r="S12" t="inlineStr"/>
+      <c r="T12" t="inlineStr"/>
+      <c r="U12" t="inlineStr"/>
       <c r="V12" t="inlineStr">
         <is>
-          <t>NO</t>
+          <t>YES</t>
+        </is>
+      </c>
+      <c r="W12" t="inlineStr">
+        <is>
+          <t>03/12/2024</t>
+        </is>
+      </c>
+      <c r="X12" t="inlineStr">
+        <is>
+          <t>abake</t>
         </is>
       </c>
       <c r="Y12" t="inlineStr">
@@ -1288,11 +1521,47 @@
           <t>NO</t>
         </is>
       </c>
+      <c r="Z12" t="inlineStr"/>
+      <c r="AA12" t="inlineStr"/>
       <c r="AB12" t="inlineStr">
         <is>
           <t>NO</t>
         </is>
       </c>
+      <c r="AC12" t="inlineStr"/>
+      <c r="AD12" t="inlineStr"/>
+    </row>
+    <row r="13">
+      <c r="A13" t="inlineStr"/>
+      <c r="B13" t="inlineStr"/>
+      <c r="C13" t="inlineStr"/>
+      <c r="D13" t="inlineStr"/>
+      <c r="E13" t="inlineStr"/>
+      <c r="F13" t="inlineStr"/>
+      <c r="G13" t="inlineStr"/>
+      <c r="H13" t="inlineStr"/>
+      <c r="I13" t="inlineStr"/>
+      <c r="J13" t="inlineStr"/>
+      <c r="K13" t="inlineStr"/>
+      <c r="L13" t="inlineStr"/>
+      <c r="M13" t="inlineStr"/>
+      <c r="N13" t="inlineStr"/>
+      <c r="O13" t="inlineStr"/>
+      <c r="P13" t="inlineStr"/>
+      <c r="Q13" t="inlineStr"/>
+      <c r="R13" t="inlineStr"/>
+      <c r="S13" t="inlineStr"/>
+      <c r="T13" t="inlineStr"/>
+      <c r="U13" t="inlineStr"/>
+      <c r="V13" t="inlineStr"/>
+      <c r="W13" t="inlineStr"/>
+      <c r="X13" t="inlineStr"/>
+      <c r="Y13" t="inlineStr"/>
+      <c r="Z13" t="inlineStr"/>
+      <c r="AA13" t="inlineStr"/>
+      <c r="AB13" t="inlineStr"/>
+      <c r="AC13" t="inlineStr"/>
+      <c r="AD13" t="inlineStr"/>
     </row>
     <row r="14">
       <c r="A14" t="inlineStr">
@@ -1351,11 +1620,7 @@
       <c r="L14" t="n">
         <v>20</v>
       </c>
-      <c r="M14" t="inlineStr">
-        <is>
-          <t> </t>
-        </is>
-      </c>
+      <c r="M14" t="inlineStr"/>
       <c r="N14" t="inlineStr">
         <is>
           <t>AMS</t>
@@ -1376,6 +1641,10 @@
           <t>PICKUP</t>
         </is>
       </c>
+      <c r="R14" t="inlineStr"/>
+      <c r="S14" t="inlineStr"/>
+      <c r="T14" t="inlineStr"/>
+      <c r="U14" t="inlineStr"/>
       <c r="V14" t="inlineStr">
         <is>
           <t>YES</t>
@@ -1411,6 +1680,8 @@
           <t>NO</t>
         </is>
       </c>
+      <c r="AC14" t="inlineStr"/>
+      <c r="AD14" t="inlineStr"/>
     </row>
     <row r="15">
       <c r="A15" t="inlineStr">
@@ -1469,11 +1740,7 @@
       <c r="L15" t="n">
         <v>87</v>
       </c>
-      <c r="M15" t="inlineStr">
-        <is>
-          <t> </t>
-        </is>
-      </c>
+      <c r="M15" t="inlineStr"/>
       <c r="N15" t="inlineStr">
         <is>
           <t>AMA</t>
@@ -1494,6 +1761,10 @@
           <t>PICKUP</t>
         </is>
       </c>
+      <c r="R15" t="inlineStr"/>
+      <c r="S15" t="inlineStr"/>
+      <c r="T15" t="inlineStr"/>
+      <c r="U15" t="inlineStr"/>
       <c r="V15" t="inlineStr">
         <is>
           <t>YES</t>
@@ -1597,11 +1868,7 @@
       <c r="L16" t="n">
         <v>89.98999999999999</v>
       </c>
-      <c r="M16" t="inlineStr">
-        <is>
-          <t> </t>
-        </is>
-      </c>
+      <c r="M16" t="inlineStr"/>
       <c r="N16" t="inlineStr">
         <is>
           <t>AMA</t>
@@ -1622,6 +1889,10 @@
           <t>PICKUP</t>
         </is>
       </c>
+      <c r="R16" t="inlineStr"/>
+      <c r="S16" t="inlineStr"/>
+      <c r="T16" t="inlineStr"/>
+      <c r="U16" t="inlineStr"/>
       <c r="V16" t="inlineStr">
         <is>
           <t>YES</t>
@@ -1669,156 +1940,36 @@
       </c>
     </row>
     <row r="17">
-      <c r="A17" t="inlineStr">
-        <is>
-          <t> </t>
-        </is>
-      </c>
-      <c r="B17" t="inlineStr">
-        <is>
-          <t> </t>
-        </is>
-      </c>
-      <c r="C17" t="inlineStr">
-        <is>
-          <t> </t>
-        </is>
-      </c>
-      <c r="D17" t="inlineStr">
-        <is>
-          <t> </t>
-        </is>
-      </c>
-      <c r="E17" t="inlineStr">
-        <is>
-          <t> </t>
-        </is>
-      </c>
-      <c r="F17" t="inlineStr">
-        <is>
-          <t> </t>
-        </is>
-      </c>
-      <c r="G17" t="inlineStr">
-        <is>
-          <t> </t>
-        </is>
-      </c>
-      <c r="H17" t="inlineStr">
-        <is>
-          <t> </t>
-        </is>
-      </c>
-      <c r="I17" t="inlineStr">
-        <is>
-          <t> </t>
-        </is>
-      </c>
-      <c r="J17" t="inlineStr">
-        <is>
-          <t> </t>
-        </is>
-      </c>
-      <c r="K17" t="inlineStr">
-        <is>
-          <t> </t>
-        </is>
-      </c>
-      <c r="L17" t="inlineStr">
-        <is>
-          <t> </t>
-        </is>
-      </c>
-      <c r="M17" t="inlineStr">
-        <is>
-          <t> </t>
-        </is>
-      </c>
-      <c r="N17" t="inlineStr">
-        <is>
-          <t> </t>
-        </is>
-      </c>
-      <c r="O17" t="inlineStr">
-        <is>
-          <t> </t>
-        </is>
-      </c>
-      <c r="P17" t="inlineStr">
-        <is>
-          <t> </t>
-        </is>
-      </c>
-      <c r="Q17" t="inlineStr">
-        <is>
-          <t> </t>
-        </is>
-      </c>
-      <c r="R17" t="inlineStr">
-        <is>
-          <t> </t>
-        </is>
-      </c>
-      <c r="S17" t="inlineStr">
-        <is>
-          <t> </t>
-        </is>
-      </c>
-      <c r="T17" t="inlineStr">
-        <is>
-          <t> </t>
-        </is>
-      </c>
-      <c r="U17" t="inlineStr">
-        <is>
-          <t> </t>
-        </is>
-      </c>
-      <c r="V17" t="inlineStr">
-        <is>
-          <t> </t>
-        </is>
-      </c>
-      <c r="W17" t="inlineStr">
-        <is>
-          <t> </t>
-        </is>
-      </c>
-      <c r="X17" t="inlineStr">
-        <is>
-          <t> </t>
-        </is>
-      </c>
-      <c r="Y17" t="inlineStr">
-        <is>
-          <t> </t>
-        </is>
-      </c>
-      <c r="Z17" t="inlineStr">
-        <is>
-          <t> </t>
-        </is>
-      </c>
-      <c r="AA17" t="inlineStr">
-        <is>
-          <t> </t>
-        </is>
-      </c>
-      <c r="AB17" t="inlineStr">
-        <is>
-          <t> </t>
-        </is>
-      </c>
-      <c r="AC17" t="inlineStr">
-        <is>
-          <t> </t>
-        </is>
-      </c>
-      <c r="AD17" t="inlineStr">
-        <is>
-          <t> </t>
-        </is>
-      </c>
+      <c r="A17" t="inlineStr"/>
+      <c r="B17" t="inlineStr"/>
+      <c r="C17" t="inlineStr"/>
+      <c r="D17" t="inlineStr"/>
+      <c r="E17" t="inlineStr"/>
+      <c r="F17" t="inlineStr"/>
+      <c r="G17" t="inlineStr"/>
+      <c r="H17" t="inlineStr"/>
+      <c r="I17" t="inlineStr"/>
+      <c r="J17" t="inlineStr"/>
+      <c r="K17" t="inlineStr"/>
+      <c r="L17" t="inlineStr"/>
+      <c r="M17" t="inlineStr"/>
+      <c r="N17" t="inlineStr"/>
+      <c r="O17" t="inlineStr"/>
+      <c r="P17" t="inlineStr"/>
+      <c r="Q17" t="inlineStr"/>
+      <c r="R17" t="inlineStr"/>
+      <c r="S17" t="inlineStr"/>
+      <c r="T17" t="inlineStr"/>
+      <c r="U17" t="inlineStr"/>
+      <c r="V17" t="inlineStr"/>
+      <c r="W17" t="inlineStr"/>
+      <c r="X17" t="inlineStr"/>
+      <c r="Y17" t="inlineStr"/>
+      <c r="Z17" t="inlineStr"/>
+      <c r="AA17" t="inlineStr"/>
+      <c r="AB17" t="inlineStr"/>
+      <c r="AC17" t="inlineStr"/>
+      <c r="AD17" t="inlineStr"/>
     </row>
     <row r="18">
       <c r="A18" t="inlineStr">
@@ -1877,11 +2028,7 @@
       <c r="L18" t="n">
         <v>15</v>
       </c>
-      <c r="M18" t="inlineStr">
-        <is>
-          <t> </t>
-        </is>
-      </c>
+      <c r="M18" t="inlineStr"/>
       <c r="N18" t="inlineStr">
         <is>
           <t>AMS</t>
@@ -1902,6 +2049,10 @@
           <t>PICKUP</t>
         </is>
       </c>
+      <c r="R18" t="inlineStr"/>
+      <c r="S18" t="inlineStr"/>
+      <c r="T18" t="inlineStr"/>
+      <c r="U18" t="inlineStr"/>
       <c r="V18" t="inlineStr">
         <is>
           <t>YES</t>
@@ -2005,11 +2156,7 @@
       <c r="L19" t="n">
         <v>50.99</v>
       </c>
-      <c r="M19" t="inlineStr">
-        <is>
-          <t> </t>
-        </is>
-      </c>
+      <c r="M19" t="inlineStr"/>
       <c r="N19" t="inlineStr">
         <is>
           <t>AMS</t>
@@ -2153,11 +2300,7 @@
       <c r="L20" t="n">
         <v>90</v>
       </c>
-      <c r="M20" t="inlineStr">
-        <is>
-          <t> </t>
-        </is>
-      </c>
+      <c r="M20" t="inlineStr"/>
       <c r="N20" t="inlineStr">
         <is>
           <t>AMS</t>
@@ -2178,6 +2321,10 @@
           <t>PICKUP</t>
         </is>
       </c>
+      <c r="R20" t="inlineStr"/>
+      <c r="S20" t="inlineStr"/>
+      <c r="T20" t="inlineStr"/>
+      <c r="U20" t="inlineStr"/>
       <c r="V20" t="inlineStr">
         <is>
           <t>YES</t>
@@ -2281,11 +2428,7 @@
       <c r="L21" t="n">
         <v>822</v>
       </c>
-      <c r="M21" t="inlineStr">
-        <is>
-          <t> </t>
-        </is>
-      </c>
+      <c r="M21" t="inlineStr"/>
       <c r="N21" t="inlineStr">
         <is>
           <t>AEC</t>
@@ -2306,21 +2449,31 @@
           <t>PICKUP</t>
         </is>
       </c>
+      <c r="R21" t="inlineStr"/>
+      <c r="S21" t="inlineStr"/>
+      <c r="T21" t="inlineStr"/>
+      <c r="U21" t="inlineStr"/>
       <c r="V21" t="inlineStr">
         <is>
           <t>NO</t>
         </is>
       </c>
+      <c r="W21" t="inlineStr"/>
+      <c r="X21" t="inlineStr"/>
       <c r="Y21" t="inlineStr">
         <is>
           <t>NO</t>
         </is>
       </c>
+      <c r="Z21" t="inlineStr"/>
+      <c r="AA21" t="inlineStr"/>
       <c r="AB21" t="inlineStr">
         <is>
           <t>NO</t>
         </is>
       </c>
+      <c r="AC21" t="inlineStr"/>
+      <c r="AD21" t="inlineStr"/>
     </row>
     <row r="22">
       <c r="A22" t="inlineStr">
@@ -2379,11 +2532,7 @@
       <c r="L22" t="n">
         <v>55</v>
       </c>
-      <c r="M22" t="inlineStr">
-        <is>
-          <t> </t>
-        </is>
-      </c>
+      <c r="M22" t="inlineStr"/>
       <c r="N22" t="inlineStr">
         <is>
           <t>AEC</t>
@@ -2404,6 +2553,10 @@
           <t>PICKUP</t>
         </is>
       </c>
+      <c r="R22" t="inlineStr"/>
+      <c r="S22" t="inlineStr"/>
+      <c r="T22" t="inlineStr"/>
+      <c r="U22" t="inlineStr"/>
       <c r="V22" t="inlineStr">
         <is>
           <t>YES</t>
@@ -2507,11 +2660,7 @@
       <c r="L23" t="n">
         <v>98</v>
       </c>
-      <c r="M23" t="inlineStr">
-        <is>
-          <t> </t>
-        </is>
-      </c>
+      <c r="M23" t="inlineStr"/>
       <c r="N23" t="inlineStr">
         <is>
           <t>me</t>
@@ -2532,6 +2681,10 @@
           <t>PICKUP</t>
         </is>
       </c>
+      <c r="R23" t="inlineStr"/>
+      <c r="S23" t="inlineStr"/>
+      <c r="T23" t="inlineStr"/>
+      <c r="U23" t="inlineStr"/>
       <c r="V23" t="inlineStr">
         <is>
           <t>YES</t>

</xml_diff>

<commit_message>
changes made from testing
</commit_message>
<xml_diff>
--- a/SO_Test.xlsx
+++ b/SO_Test.xlsx
@@ -642,7 +642,6 @@
       <c r="L2" t="n">
         <v>24</v>
       </c>
-      <c r="M2" t="inlineStr"/>
       <c r="N2" t="inlineStr">
         <is>
           <t>Vendors</t>
@@ -663,10 +662,6 @@
           <t>NO</t>
         </is>
       </c>
-      <c r="R2" t="inlineStr"/>
-      <c r="S2" t="inlineStr"/>
-      <c r="T2" t="inlineStr"/>
-      <c r="U2" t="inlineStr"/>
       <c r="V2" t="inlineStr">
         <is>
           <t>YES</t>
@@ -713,38 +708,7 @@
         </is>
       </c>
     </row>
-    <row r="3">
-      <c r="A3" t="inlineStr"/>
-      <c r="B3" t="inlineStr"/>
-      <c r="C3" t="inlineStr"/>
-      <c r="D3" t="inlineStr"/>
-      <c r="E3" t="inlineStr"/>
-      <c r="F3" t="inlineStr"/>
-      <c r="G3" t="inlineStr"/>
-      <c r="H3" t="inlineStr"/>
-      <c r="I3" t="inlineStr"/>
-      <c r="J3" t="inlineStr"/>
-      <c r="K3" t="inlineStr"/>
-      <c r="L3" t="inlineStr"/>
-      <c r="M3" t="inlineStr"/>
-      <c r="N3" t="inlineStr"/>
-      <c r="O3" t="inlineStr"/>
-      <c r="P3" t="inlineStr"/>
-      <c r="Q3" t="inlineStr"/>
-      <c r="R3" t="inlineStr"/>
-      <c r="S3" t="inlineStr"/>
-      <c r="T3" t="inlineStr"/>
-      <c r="U3" t="inlineStr"/>
-      <c r="V3" t="inlineStr"/>
-      <c r="W3" t="inlineStr"/>
-      <c r="X3" t="inlineStr"/>
-      <c r="Y3" t="inlineStr"/>
-      <c r="Z3" t="inlineStr"/>
-      <c r="AA3" t="inlineStr"/>
-      <c r="AB3" t="inlineStr"/>
-      <c r="AC3" t="inlineStr"/>
-      <c r="AD3" t="inlineStr"/>
-    </row>
+    <row r="3"/>
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
@@ -802,7 +766,6 @@
       <c r="L4" t="n">
         <v>34</v>
       </c>
-      <c r="M4" t="inlineStr"/>
       <c r="N4" t="inlineStr">
         <is>
           <t>AMA</t>
@@ -823,10 +786,6 @@
           <t>NO</t>
         </is>
       </c>
-      <c r="R4" t="inlineStr"/>
-      <c r="S4" t="inlineStr"/>
-      <c r="T4" t="inlineStr"/>
-      <c r="U4" t="inlineStr"/>
       <c r="V4" t="inlineStr">
         <is>
           <t>YES</t>
@@ -930,7 +889,6 @@
       <c r="L5" t="n">
         <v>49.99</v>
       </c>
-      <c r="M5" t="inlineStr"/>
       <c r="N5" t="inlineStr">
         <is>
           <t>AMS</t>
@@ -974,55 +932,18 @@
           <t>NO</t>
         </is>
       </c>
-      <c r="W5" t="inlineStr"/>
-      <c r="X5" t="inlineStr"/>
       <c r="Y5" t="inlineStr">
         <is>
           <t>NO</t>
         </is>
       </c>
-      <c r="Z5" t="inlineStr"/>
-      <c r="AA5" t="inlineStr"/>
       <c r="AB5" t="inlineStr">
         <is>
           <t>NO</t>
         </is>
       </c>
-      <c r="AC5" t="inlineStr"/>
-      <c r="AD5" t="inlineStr"/>
     </row>
-    <row r="6">
-      <c r="A6" t="inlineStr"/>
-      <c r="B6" t="inlineStr"/>
-      <c r="C6" t="inlineStr"/>
-      <c r="D6" t="inlineStr"/>
-      <c r="E6" t="inlineStr"/>
-      <c r="F6" t="inlineStr"/>
-      <c r="G6" t="inlineStr"/>
-      <c r="H6" t="inlineStr"/>
-      <c r="I6" t="inlineStr"/>
-      <c r="J6" t="inlineStr"/>
-      <c r="K6" t="inlineStr"/>
-      <c r="L6" t="inlineStr"/>
-      <c r="M6" t="inlineStr"/>
-      <c r="N6" t="inlineStr"/>
-      <c r="O6" t="inlineStr"/>
-      <c r="P6" t="inlineStr"/>
-      <c r="Q6" t="inlineStr"/>
-      <c r="R6" t="inlineStr"/>
-      <c r="S6" t="inlineStr"/>
-      <c r="T6" t="inlineStr"/>
-      <c r="U6" t="inlineStr"/>
-      <c r="V6" t="inlineStr"/>
-      <c r="W6" t="inlineStr"/>
-      <c r="X6" t="inlineStr"/>
-      <c r="Y6" t="inlineStr"/>
-      <c r="Z6" t="inlineStr"/>
-      <c r="AA6" t="inlineStr"/>
-      <c r="AB6" t="inlineStr"/>
-      <c r="AC6" t="inlineStr"/>
-      <c r="AD6" t="inlineStr"/>
-    </row>
+    <row r="6"/>
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
@@ -1080,7 +1001,6 @@
       <c r="L7" t="n">
         <v>50.2</v>
       </c>
-      <c r="M7" t="inlineStr"/>
       <c r="N7" t="inlineStr">
         <is>
           <t>AMS</t>
@@ -1101,10 +1021,6 @@
           <t>NO</t>
         </is>
       </c>
-      <c r="R7" t="inlineStr"/>
-      <c r="S7" t="inlineStr"/>
-      <c r="T7" t="inlineStr"/>
-      <c r="U7" t="inlineStr"/>
       <c r="V7" t="inlineStr">
         <is>
           <t>YES</t>
@@ -1151,38 +1067,7 @@
         </is>
       </c>
     </row>
-    <row r="8">
-      <c r="A8" t="inlineStr"/>
-      <c r="B8" t="inlineStr"/>
-      <c r="C8" t="inlineStr"/>
-      <c r="D8" t="inlineStr"/>
-      <c r="E8" t="inlineStr"/>
-      <c r="F8" t="inlineStr"/>
-      <c r="G8" t="inlineStr"/>
-      <c r="H8" t="inlineStr"/>
-      <c r="I8" t="inlineStr"/>
-      <c r="J8" t="inlineStr"/>
-      <c r="K8" t="inlineStr"/>
-      <c r="L8" t="inlineStr"/>
-      <c r="M8" t="inlineStr"/>
-      <c r="N8" t="inlineStr"/>
-      <c r="O8" t="inlineStr"/>
-      <c r="P8" t="inlineStr"/>
-      <c r="Q8" t="inlineStr"/>
-      <c r="R8" t="inlineStr"/>
-      <c r="S8" t="inlineStr"/>
-      <c r="T8" t="inlineStr"/>
-      <c r="U8" t="inlineStr"/>
-      <c r="V8" t="inlineStr"/>
-      <c r="W8" t="inlineStr"/>
-      <c r="X8" t="inlineStr"/>
-      <c r="Y8" t="inlineStr"/>
-      <c r="Z8" t="inlineStr"/>
-      <c r="AA8" t="inlineStr"/>
-      <c r="AB8" t="inlineStr"/>
-      <c r="AC8" t="inlineStr"/>
-      <c r="AD8" t="inlineStr"/>
-    </row>
+    <row r="8"/>
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
@@ -1240,7 +1125,6 @@
       <c r="L9" t="n">
         <v>58.63</v>
       </c>
-      <c r="M9" t="inlineStr"/>
       <c r="N9" t="inlineStr">
         <is>
           <t>AMS</t>
@@ -1251,70 +1135,28 @@
           <t>LP</t>
         </is>
       </c>
-      <c r="P9" t="inlineStr"/>
       <c r="Q9" t="inlineStr">
         <is>
           <t>NO</t>
         </is>
       </c>
-      <c r="R9" t="inlineStr"/>
-      <c r="S9" t="inlineStr"/>
-      <c r="T9" t="inlineStr"/>
-      <c r="U9" t="inlineStr"/>
       <c r="V9" t="inlineStr">
         <is>
           <t>NO</t>
         </is>
       </c>
-      <c r="W9" t="inlineStr"/>
-      <c r="X9" t="inlineStr"/>
       <c r="Y9" t="inlineStr">
         <is>
           <t>NO</t>
         </is>
       </c>
-      <c r="Z9" t="inlineStr"/>
-      <c r="AA9" t="inlineStr"/>
       <c r="AB9" t="inlineStr">
         <is>
           <t>NO</t>
         </is>
       </c>
-      <c r="AC9" t="inlineStr"/>
-      <c r="AD9" t="inlineStr"/>
     </row>
-    <row r="10">
-      <c r="A10" t="inlineStr"/>
-      <c r="B10" t="inlineStr"/>
-      <c r="C10" t="inlineStr"/>
-      <c r="D10" t="inlineStr"/>
-      <c r="E10" t="inlineStr"/>
-      <c r="F10" t="inlineStr"/>
-      <c r="G10" t="inlineStr"/>
-      <c r="H10" t="inlineStr"/>
-      <c r="I10" t="inlineStr"/>
-      <c r="J10" t="inlineStr"/>
-      <c r="K10" t="inlineStr"/>
-      <c r="L10" t="inlineStr"/>
-      <c r="M10" t="inlineStr"/>
-      <c r="N10" t="inlineStr"/>
-      <c r="O10" t="inlineStr"/>
-      <c r="P10" t="inlineStr"/>
-      <c r="Q10" t="inlineStr"/>
-      <c r="R10" t="inlineStr"/>
-      <c r="S10" t="inlineStr"/>
-      <c r="T10" t="inlineStr"/>
-      <c r="U10" t="inlineStr"/>
-      <c r="V10" t="inlineStr"/>
-      <c r="W10" t="inlineStr"/>
-      <c r="X10" t="inlineStr"/>
-      <c r="Y10" t="inlineStr"/>
-      <c r="Z10" t="inlineStr"/>
-      <c r="AA10" t="inlineStr"/>
-      <c r="AB10" t="inlineStr"/>
-      <c r="AC10" t="inlineStr"/>
-      <c r="AD10" t="inlineStr"/>
-    </row>
+    <row r="10"/>
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
@@ -1372,7 +1214,6 @@
       <c r="L11" t="n">
         <v>199</v>
       </c>
-      <c r="M11" t="inlineStr"/>
       <c r="N11" t="inlineStr">
         <is>
           <t>AMA</t>
@@ -1393,31 +1234,21 @@
           <t>NO</t>
         </is>
       </c>
-      <c r="R11" t="inlineStr"/>
-      <c r="S11" t="inlineStr"/>
-      <c r="T11" t="inlineStr"/>
-      <c r="U11" t="inlineStr"/>
       <c r="V11" t="inlineStr">
         <is>
           <t>NO</t>
         </is>
       </c>
-      <c r="W11" t="inlineStr"/>
-      <c r="X11" t="inlineStr"/>
       <c r="Y11" t="inlineStr">
         <is>
           <t>NO</t>
         </is>
       </c>
-      <c r="Z11" t="inlineStr"/>
-      <c r="AA11" t="inlineStr"/>
       <c r="AB11" t="inlineStr">
         <is>
           <t>NO</t>
         </is>
       </c>
-      <c r="AC11" t="inlineStr"/>
-      <c r="AD11" t="inlineStr"/>
     </row>
     <row r="12">
       <c r="A12" t="inlineStr">
@@ -1476,7 +1307,6 @@
       <c r="L12" t="n">
         <v>15</v>
       </c>
-      <c r="M12" t="inlineStr"/>
       <c r="N12" t="inlineStr">
         <is>
           <t>AMA</t>
@@ -1497,10 +1327,6 @@
           <t>NO</t>
         </is>
       </c>
-      <c r="R12" t="inlineStr"/>
-      <c r="S12" t="inlineStr"/>
-      <c r="T12" t="inlineStr"/>
-      <c r="U12" t="inlineStr"/>
       <c r="V12" t="inlineStr">
         <is>
           <t>YES</t>
@@ -1521,48 +1347,13 @@
           <t>NO</t>
         </is>
       </c>
-      <c r="Z12" t="inlineStr"/>
-      <c r="AA12" t="inlineStr"/>
       <c r="AB12" t="inlineStr">
         <is>
           <t>NO</t>
         </is>
       </c>
-      <c r="AC12" t="inlineStr"/>
-      <c r="AD12" t="inlineStr"/>
     </row>
-    <row r="13">
-      <c r="A13" t="inlineStr"/>
-      <c r="B13" t="inlineStr"/>
-      <c r="C13" t="inlineStr"/>
-      <c r="D13" t="inlineStr"/>
-      <c r="E13" t="inlineStr"/>
-      <c r="F13" t="inlineStr"/>
-      <c r="G13" t="inlineStr"/>
-      <c r="H13" t="inlineStr"/>
-      <c r="I13" t="inlineStr"/>
-      <c r="J13" t="inlineStr"/>
-      <c r="K13" t="inlineStr"/>
-      <c r="L13" t="inlineStr"/>
-      <c r="M13" t="inlineStr"/>
-      <c r="N13" t="inlineStr"/>
-      <c r="O13" t="inlineStr"/>
-      <c r="P13" t="inlineStr"/>
-      <c r="Q13" t="inlineStr"/>
-      <c r="R13" t="inlineStr"/>
-      <c r="S13" t="inlineStr"/>
-      <c r="T13" t="inlineStr"/>
-      <c r="U13" t="inlineStr"/>
-      <c r="V13" t="inlineStr"/>
-      <c r="W13" t="inlineStr"/>
-      <c r="X13" t="inlineStr"/>
-      <c r="Y13" t="inlineStr"/>
-      <c r="Z13" t="inlineStr"/>
-      <c r="AA13" t="inlineStr"/>
-      <c r="AB13" t="inlineStr"/>
-      <c r="AC13" t="inlineStr"/>
-      <c r="AD13" t="inlineStr"/>
-    </row>
+    <row r="13"/>
     <row r="14">
       <c r="A14" t="inlineStr">
         <is>
@@ -1620,7 +1411,6 @@
       <c r="L14" t="n">
         <v>20</v>
       </c>
-      <c r="M14" t="inlineStr"/>
       <c r="N14" t="inlineStr">
         <is>
           <t>AMS</t>
@@ -1641,10 +1431,6 @@
           <t>PICKUP</t>
         </is>
       </c>
-      <c r="R14" t="inlineStr"/>
-      <c r="S14" t="inlineStr"/>
-      <c r="T14" t="inlineStr"/>
-      <c r="U14" t="inlineStr"/>
       <c r="V14" t="inlineStr">
         <is>
           <t>YES</t>
@@ -1680,8 +1466,6 @@
           <t>NO</t>
         </is>
       </c>
-      <c r="AC14" t="inlineStr"/>
-      <c r="AD14" t="inlineStr"/>
     </row>
     <row r="15">
       <c r="A15" t="inlineStr">
@@ -1740,7 +1524,6 @@
       <c r="L15" t="n">
         <v>87</v>
       </c>
-      <c r="M15" t="inlineStr"/>
       <c r="N15" t="inlineStr">
         <is>
           <t>AMA</t>
@@ -1761,10 +1544,6 @@
           <t>PICKUP</t>
         </is>
       </c>
-      <c r="R15" t="inlineStr"/>
-      <c r="S15" t="inlineStr"/>
-      <c r="T15" t="inlineStr"/>
-      <c r="U15" t="inlineStr"/>
       <c r="V15" t="inlineStr">
         <is>
           <t>YES</t>
@@ -1868,7 +1647,6 @@
       <c r="L16" t="n">
         <v>89.98999999999999</v>
       </c>
-      <c r="M16" t="inlineStr"/>
       <c r="N16" t="inlineStr">
         <is>
           <t>AMA</t>
@@ -1889,10 +1667,6 @@
           <t>PICKUP</t>
         </is>
       </c>
-      <c r="R16" t="inlineStr"/>
-      <c r="S16" t="inlineStr"/>
-      <c r="T16" t="inlineStr"/>
-      <c r="U16" t="inlineStr"/>
       <c r="V16" t="inlineStr">
         <is>
           <t>YES</t>
@@ -1939,38 +1713,7 @@
         </is>
       </c>
     </row>
-    <row r="17">
-      <c r="A17" t="inlineStr"/>
-      <c r="B17" t="inlineStr"/>
-      <c r="C17" t="inlineStr"/>
-      <c r="D17" t="inlineStr"/>
-      <c r="E17" t="inlineStr"/>
-      <c r="F17" t="inlineStr"/>
-      <c r="G17" t="inlineStr"/>
-      <c r="H17" t="inlineStr"/>
-      <c r="I17" t="inlineStr"/>
-      <c r="J17" t="inlineStr"/>
-      <c r="K17" t="inlineStr"/>
-      <c r="L17" t="inlineStr"/>
-      <c r="M17" t="inlineStr"/>
-      <c r="N17" t="inlineStr"/>
-      <c r="O17" t="inlineStr"/>
-      <c r="P17" t="inlineStr"/>
-      <c r="Q17" t="inlineStr"/>
-      <c r="R17" t="inlineStr"/>
-      <c r="S17" t="inlineStr"/>
-      <c r="T17" t="inlineStr"/>
-      <c r="U17" t="inlineStr"/>
-      <c r="V17" t="inlineStr"/>
-      <c r="W17" t="inlineStr"/>
-      <c r="X17" t="inlineStr"/>
-      <c r="Y17" t="inlineStr"/>
-      <c r="Z17" t="inlineStr"/>
-      <c r="AA17" t="inlineStr"/>
-      <c r="AB17" t="inlineStr"/>
-      <c r="AC17" t="inlineStr"/>
-      <c r="AD17" t="inlineStr"/>
-    </row>
+    <row r="17"/>
     <row r="18">
       <c r="A18" t="inlineStr">
         <is>
@@ -2028,7 +1771,6 @@
       <c r="L18" t="n">
         <v>15</v>
       </c>
-      <c r="M18" t="inlineStr"/>
       <c r="N18" t="inlineStr">
         <is>
           <t>AMS</t>
@@ -2049,10 +1791,6 @@
           <t>PICKUP</t>
         </is>
       </c>
-      <c r="R18" t="inlineStr"/>
-      <c r="S18" t="inlineStr"/>
-      <c r="T18" t="inlineStr"/>
-      <c r="U18" t="inlineStr"/>
       <c r="V18" t="inlineStr">
         <is>
           <t>YES</t>
@@ -2156,7 +1894,6 @@
       <c r="L19" t="n">
         <v>50.99</v>
       </c>
-      <c r="M19" t="inlineStr"/>
       <c r="N19" t="inlineStr">
         <is>
           <t>AMS</t>
@@ -2300,7 +2037,6 @@
       <c r="L20" t="n">
         <v>90</v>
       </c>
-      <c r="M20" t="inlineStr"/>
       <c r="N20" t="inlineStr">
         <is>
           <t>AMS</t>
@@ -2321,10 +2057,6 @@
           <t>PICKUP</t>
         </is>
       </c>
-      <c r="R20" t="inlineStr"/>
-      <c r="S20" t="inlineStr"/>
-      <c r="T20" t="inlineStr"/>
-      <c r="U20" t="inlineStr"/>
       <c r="V20" t="inlineStr">
         <is>
           <t>YES</t>
@@ -2428,7 +2160,6 @@
       <c r="L21" t="n">
         <v>822</v>
       </c>
-      <c r="M21" t="inlineStr"/>
       <c r="N21" t="inlineStr">
         <is>
           <t>AEC</t>
@@ -2449,31 +2180,21 @@
           <t>PICKUP</t>
         </is>
       </c>
-      <c r="R21" t="inlineStr"/>
-      <c r="S21" t="inlineStr"/>
-      <c r="T21" t="inlineStr"/>
-      <c r="U21" t="inlineStr"/>
       <c r="V21" t="inlineStr">
         <is>
           <t>NO</t>
         </is>
       </c>
-      <c r="W21" t="inlineStr"/>
-      <c r="X21" t="inlineStr"/>
       <c r="Y21" t="inlineStr">
         <is>
           <t>NO</t>
         </is>
       </c>
-      <c r="Z21" t="inlineStr"/>
-      <c r="AA21" t="inlineStr"/>
       <c r="AB21" t="inlineStr">
         <is>
           <t>NO</t>
         </is>
       </c>
-      <c r="AC21" t="inlineStr"/>
-      <c r="AD21" t="inlineStr"/>
     </row>
     <row r="22">
       <c r="A22" t="inlineStr">
@@ -2532,7 +2253,6 @@
       <c r="L22" t="n">
         <v>55</v>
       </c>
-      <c r="M22" t="inlineStr"/>
       <c r="N22" t="inlineStr">
         <is>
           <t>AEC</t>
@@ -2553,10 +2273,6 @@
           <t>PICKUP</t>
         </is>
       </c>
-      <c r="R22" t="inlineStr"/>
-      <c r="S22" t="inlineStr"/>
-      <c r="T22" t="inlineStr"/>
-      <c r="U22" t="inlineStr"/>
       <c r="V22" t="inlineStr">
         <is>
           <t>YES</t>
@@ -2660,7 +2376,6 @@
       <c r="L23" t="n">
         <v>98</v>
       </c>
-      <c r="M23" t="inlineStr"/>
       <c r="N23" t="inlineStr">
         <is>
           <t>me</t>
@@ -2681,10 +2396,6 @@
           <t>PICKUP</t>
         </is>
       </c>
-      <c r="R23" t="inlineStr"/>
-      <c r="S23" t="inlineStr"/>
-      <c r="T23" t="inlineStr"/>
-      <c r="U23" t="inlineStr"/>
       <c r="V23" t="inlineStr">
         <is>
           <t>YES</t>

</xml_diff>

<commit_message>
modified main.py - added a label in update SO to display when the prder was placed - made the results frame refresh once an oder is marked as completed
</commit_message>
<xml_diff>
--- a/SO_Test.xlsx
+++ b/SO_Test.xlsx
@@ -1330,24 +1330,52 @@
       <c r="T9" t="inlineStr"/>
       <c r="U9" t="inlineStr">
         <is>
-          <t>NO</t>
-        </is>
-      </c>
-      <c r="V9" t="inlineStr"/>
-      <c r="W9" t="inlineStr"/>
+          <t>YES</t>
+        </is>
+      </c>
+      <c r="V9" t="inlineStr">
+        <is>
+          <t>03/14/2024</t>
+        </is>
+      </c>
+      <c r="W9" t="inlineStr">
+        <is>
+          <t>abake</t>
+        </is>
+      </c>
       <c r="X9" t="inlineStr">
         <is>
-          <t>NO</t>
-        </is>
-      </c>
-      <c r="Y9" t="inlineStr"/>
-      <c r="Z9" t="inlineStr"/>
+          <t>YES</t>
+        </is>
+      </c>
+      <c r="Y9" t="inlineStr">
+        <is>
+          <t>03/14/2024</t>
+        </is>
+      </c>
+      <c r="Z9" t="inlineStr">
+        <is>
+          <t>abake</t>
+        </is>
+      </c>
       <c r="AA9" t="n">
-        <v>0</v>
-      </c>
-      <c r="AB9" t="inlineStr"/>
-      <c r="AC9" t="inlineStr"/>
-      <c r="AD9" t="inlineStr"/>
+        <v>1</v>
+      </c>
+      <c r="AB9" t="inlineStr">
+        <is>
+          <t>03/14/2024</t>
+        </is>
+      </c>
+      <c r="AC9" t="inlineStr">
+        <is>
+          <t>abake</t>
+        </is>
+      </c>
+      <c r="AD9" t="inlineStr">
+        <is>
+          <t>picked up</t>
+        </is>
+      </c>
       <c r="AE9" t="inlineStr"/>
       <c r="AF9" t="inlineStr"/>
       <c r="AG9" t="inlineStr"/>
@@ -1576,11 +1604,19 @@
       <c r="T12" t="inlineStr"/>
       <c r="U12" t="inlineStr">
         <is>
-          <t>NO</t>
-        </is>
-      </c>
-      <c r="V12" t="inlineStr"/>
-      <c r="W12" t="inlineStr"/>
+          <t>YES</t>
+        </is>
+      </c>
+      <c r="V12" t="inlineStr">
+        <is>
+          <t>03/14/2024</t>
+        </is>
+      </c>
+      <c r="W12" t="inlineStr">
+        <is>
+          <t>abake</t>
+        </is>
+      </c>
       <c r="X12" t="inlineStr">
         <is>
           <t>YES</t>
@@ -1990,11 +2026,19 @@
       <c r="T16" t="inlineStr"/>
       <c r="U16" t="inlineStr">
         <is>
-          <t>NO</t>
-        </is>
-      </c>
-      <c r="V16" t="inlineStr"/>
-      <c r="W16" t="inlineStr"/>
+          <t>YES</t>
+        </is>
+      </c>
+      <c r="V16" t="inlineStr">
+        <is>
+          <t>03/14/2024</t>
+        </is>
+      </c>
+      <c r="W16" t="inlineStr">
+        <is>
+          <t>abake</t>
+        </is>
+      </c>
       <c r="X16" t="inlineStr">
         <is>
           <t>YES</t>
@@ -2584,11 +2628,19 @@
       <c r="T21" t="inlineStr"/>
       <c r="U21" t="inlineStr">
         <is>
-          <t>NO</t>
-        </is>
-      </c>
-      <c r="V21" t="inlineStr"/>
-      <c r="W21" t="inlineStr"/>
+          <t>YES</t>
+        </is>
+      </c>
+      <c r="V21" t="inlineStr">
+        <is>
+          <t>03/14/2024</t>
+        </is>
+      </c>
+      <c r="W21" t="inlineStr">
+        <is>
+          <t>abake</t>
+        </is>
+      </c>
       <c r="X21" t="inlineStr">
         <is>
           <t>NO</t>
@@ -3506,54 +3558,58 @@
     <row r="28">
       <c r="A28" t="inlineStr">
         <is>
-          <t>03/13/2024</t>
+          <t> </t>
         </is>
       </c>
       <c r="B28" t="inlineStr">
         <is>
-          <t>SO240313006</t>
+          <t> </t>
         </is>
       </c>
       <c r="C28" t="inlineStr">
         <is>
-          <t>ab</t>
+          <t> </t>
         </is>
       </c>
       <c r="D28" t="inlineStr">
         <is>
-          <t>54654123</t>
+          <t> </t>
         </is>
       </c>
       <c r="E28" t="inlineStr">
         <is>
-          <t>(456)789-4562</t>
+          <t> </t>
         </is>
       </c>
       <c r="F28" t="inlineStr">
         <is>
-          <t>YES</t>
+          <t> </t>
         </is>
       </c>
       <c r="G28" t="inlineStr">
         <is>
-          <t>YES</t>
+          <t> </t>
         </is>
       </c>
       <c r="H28" t="inlineStr">
         <is>
-          <t>ar</t>
+          <t> </t>
         </is>
       </c>
       <c r="I28" t="inlineStr">
         <is>
-          <t>ti</t>
-        </is>
-      </c>
-      <c r="J28" t="n">
-        <v>5</v>
-      </c>
-      <c r="K28" t="n">
-        <v>50</v>
+          <t> </t>
+        </is>
+      </c>
+      <c r="J28" t="inlineStr">
+        <is>
+          <t> </t>
+        </is>
+      </c>
+      <c r="K28" t="inlineStr">
+        <is>
+          <t> </t>
+        </is>
       </c>
       <c r="L28" t="inlineStr">
         <is>
@@ -3562,94 +3618,124 @@
       </c>
       <c r="M28" t="inlineStr">
         <is>
-          <t>other</t>
+          <t> </t>
         </is>
       </c>
       <c r="N28" t="inlineStr">
         <is>
-          <t>other</t>
+          <t> </t>
         </is>
       </c>
       <c r="O28" t="inlineStr">
         <is>
-          <t>abake</t>
+          <t> </t>
         </is>
       </c>
       <c r="P28" t="inlineStr">
         <is>
-          <t>PICKUP</t>
-        </is>
-      </c>
-      <c r="Q28" t="inlineStr"/>
-      <c r="R28" t="inlineStr"/>
-      <c r="S28" t="inlineStr"/>
-      <c r="T28" t="inlineStr"/>
+          <t> </t>
+        </is>
+      </c>
+      <c r="Q28" t="inlineStr">
+        <is>
+          <t> </t>
+        </is>
+      </c>
+      <c r="R28" t="inlineStr">
+        <is>
+          <t> </t>
+        </is>
+      </c>
+      <c r="S28" t="inlineStr">
+        <is>
+          <t> </t>
+        </is>
+      </c>
+      <c r="T28" t="inlineStr">
+        <is>
+          <t> </t>
+        </is>
+      </c>
       <c r="U28" t="inlineStr">
         <is>
-          <t>YES</t>
+          <t> </t>
         </is>
       </c>
       <c r="V28" t="inlineStr">
         <is>
-          <t>03/13/2024</t>
+          <t> </t>
         </is>
       </c>
       <c r="W28" t="inlineStr">
         <is>
-          <t>abake</t>
+          <t> </t>
         </is>
       </c>
       <c r="X28" t="inlineStr">
         <is>
-          <t>YES</t>
+          <t> </t>
         </is>
       </c>
       <c r="Y28" t="inlineStr">
         <is>
-          <t>03/13/2024</t>
+          <t> </t>
         </is>
       </c>
       <c r="Z28" t="inlineStr">
         <is>
-          <t>abake</t>
-        </is>
-      </c>
-      <c r="AA28" t="n">
-        <v>2</v>
+          <t> </t>
+        </is>
+      </c>
+      <c r="AA28" t="inlineStr">
+        <is>
+          <t> </t>
+        </is>
       </c>
       <c r="AB28" t="inlineStr">
         <is>
-          <t>03/13/2024</t>
+          <t> </t>
         </is>
       </c>
       <c r="AC28" t="inlineStr">
         <is>
-          <t>abake</t>
+          <t> </t>
         </is>
       </c>
       <c r="AD28" t="inlineStr">
         <is>
-          <t>Left VM</t>
+          <t> </t>
         </is>
       </c>
       <c r="AE28" t="inlineStr">
         <is>
-          <t>PICKED UP</t>
+          <t> </t>
         </is>
       </c>
       <c r="AF28" t="inlineStr">
         <is>
-          <t>03/13/2024</t>
+          <t> </t>
         </is>
       </c>
       <c r="AG28" t="inlineStr">
         <is>
-          <t>abake</t>
-        </is>
-      </c>
-      <c r="AH28" t="inlineStr"/>
-      <c r="AI28" t="inlineStr"/>
-      <c r="AJ28" t="inlineStr"/>
+          <t> </t>
+        </is>
+      </c>
+      <c r="AH28" t="inlineStr">
+        <is>
+          <t> </t>
+        </is>
+      </c>
+      <c r="AI28" t="inlineStr">
+        <is>
+          <t> </t>
+        </is>
+      </c>
+      <c r="AJ28" t="inlineStr">
+        <is>
+          <t> </t>
+        </is>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>

<commit_message>
SO_FRAME > Vendors Need to work on vendors section
</commit_message>
<xml_diff>
--- a/SO_Test.xlsx
+++ b/SO_Test.xlsx
@@ -1857,7 +1857,17 @@
       </c>
       <c r="U18" t="inlineStr">
         <is>
-          <t>NO</t>
+          <t>YES</t>
+        </is>
+      </c>
+      <c r="V18" t="inlineStr">
+        <is>
+          <t>03/14/2024</t>
+        </is>
+      </c>
+      <c r="W18" t="inlineStr">
+        <is>
+          <t>abake</t>
         </is>
       </c>
       <c r="X18" t="inlineStr">
@@ -1876,7 +1886,7 @@
         </is>
       </c>
       <c r="AA18" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="AB18" t="inlineStr">
         <is>
@@ -1891,6 +1901,21 @@
       <c r="AD18" t="inlineStr">
         <is>
           <t>VM</t>
+        </is>
+      </c>
+      <c r="AE18" t="inlineStr">
+        <is>
+          <t>lkadrfga</t>
+        </is>
+      </c>
+      <c r="AF18" t="inlineStr">
+        <is>
+          <t>03/14/2024</t>
+        </is>
+      </c>
+      <c r="AG18" t="inlineStr">
+        <is>
+          <t>abake</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
modified vendors' label and switch
</commit_message>
<xml_diff>
--- a/SO_Test.xlsx
+++ b/SO_Test.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:AM28"/>
+  <dimension ref="A1:AM29"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -682,6 +682,7 @@
       <c r="K2" t="n">
         <v>24</v>
       </c>
+      <c r="L2" t="inlineStr"/>
       <c r="M2" t="inlineStr">
         <is>
           <t>Vendors</t>
@@ -702,6 +703,10 @@
           <t>NO</t>
         </is>
       </c>
+      <c r="Q2" t="inlineStr"/>
+      <c r="R2" t="inlineStr"/>
+      <c r="S2" t="inlineStr"/>
+      <c r="T2" t="inlineStr"/>
       <c r="U2" t="inlineStr">
         <is>
           <t>YES</t>
@@ -765,6 +770,53 @@
           <t>abake</t>
         </is>
       </c>
+      <c r="AH2" t="inlineStr"/>
+      <c r="AI2" t="inlineStr"/>
+      <c r="AJ2" t="inlineStr"/>
+      <c r="AK2" t="inlineStr"/>
+      <c r="AL2" t="inlineStr"/>
+      <c r="AM2" t="inlineStr"/>
+    </row>
+    <row r="3">
+      <c r="A3" t="inlineStr"/>
+      <c r="B3" t="inlineStr"/>
+      <c r="C3" t="inlineStr"/>
+      <c r="D3" t="inlineStr"/>
+      <c r="E3" t="inlineStr"/>
+      <c r="F3" t="inlineStr"/>
+      <c r="G3" t="inlineStr"/>
+      <c r="H3" t="inlineStr"/>
+      <c r="I3" t="inlineStr"/>
+      <c r="J3" t="inlineStr"/>
+      <c r="K3" t="inlineStr"/>
+      <c r="L3" t="inlineStr"/>
+      <c r="M3" t="inlineStr"/>
+      <c r="N3" t="inlineStr"/>
+      <c r="O3" t="inlineStr"/>
+      <c r="P3" t="inlineStr"/>
+      <c r="Q3" t="inlineStr"/>
+      <c r="R3" t="inlineStr"/>
+      <c r="S3" t="inlineStr"/>
+      <c r="T3" t="inlineStr"/>
+      <c r="U3" t="inlineStr"/>
+      <c r="V3" t="inlineStr"/>
+      <c r="W3" t="inlineStr"/>
+      <c r="X3" t="inlineStr"/>
+      <c r="Y3" t="inlineStr"/>
+      <c r="Z3" t="inlineStr"/>
+      <c r="AA3" t="inlineStr"/>
+      <c r="AB3" t="inlineStr"/>
+      <c r="AC3" t="inlineStr"/>
+      <c r="AD3" t="inlineStr"/>
+      <c r="AE3" t="inlineStr"/>
+      <c r="AF3" t="inlineStr"/>
+      <c r="AG3" t="inlineStr"/>
+      <c r="AH3" t="inlineStr"/>
+      <c r="AI3" t="inlineStr"/>
+      <c r="AJ3" t="inlineStr"/>
+      <c r="AK3" t="inlineStr"/>
+      <c r="AL3" t="inlineStr"/>
+      <c r="AM3" t="inlineStr"/>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
@@ -818,6 +870,7 @@
       <c r="K4" t="n">
         <v>34</v>
       </c>
+      <c r="L4" t="inlineStr"/>
       <c r="M4" t="inlineStr">
         <is>
           <t>AMA</t>
@@ -838,6 +891,10 @@
           <t>NO</t>
         </is>
       </c>
+      <c r="Q4" t="inlineStr"/>
+      <c r="R4" t="inlineStr"/>
+      <c r="S4" t="inlineStr"/>
+      <c r="T4" t="inlineStr"/>
       <c r="U4" t="inlineStr">
         <is>
           <t>YES</t>
@@ -886,6 +943,15 @@
           <t>PICKED UP</t>
         </is>
       </c>
+      <c r="AE4" t="inlineStr"/>
+      <c r="AF4" t="inlineStr"/>
+      <c r="AG4" t="inlineStr"/>
+      <c r="AH4" t="inlineStr"/>
+      <c r="AI4" t="inlineStr"/>
+      <c r="AJ4" t="inlineStr"/>
+      <c r="AK4" t="inlineStr"/>
+      <c r="AL4" t="inlineStr"/>
+      <c r="AM4" t="inlineStr"/>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
@@ -939,6 +1005,7 @@
       <c r="K5" t="n">
         <v>49.99</v>
       </c>
+      <c r="L5" t="inlineStr"/>
       <c r="M5" t="inlineStr">
         <is>
           <t>AMS</t>
@@ -982,14 +1049,71 @@
           <t>NO</t>
         </is>
       </c>
+      <c r="V5" t="inlineStr"/>
+      <c r="W5" t="inlineStr"/>
       <c r="X5" t="inlineStr">
         <is>
           <t>NO</t>
         </is>
       </c>
+      <c r="Y5" t="inlineStr"/>
+      <c r="Z5" t="inlineStr"/>
       <c r="AA5" t="n">
         <v>0</v>
       </c>
+      <c r="AB5" t="inlineStr"/>
+      <c r="AC5" t="inlineStr"/>
+      <c r="AD5" t="inlineStr"/>
+      <c r="AE5" t="inlineStr"/>
+      <c r="AF5" t="inlineStr"/>
+      <c r="AG5" t="inlineStr"/>
+      <c r="AH5" t="inlineStr"/>
+      <c r="AI5" t="inlineStr"/>
+      <c r="AJ5" t="inlineStr"/>
+      <c r="AK5" t="inlineStr"/>
+      <c r="AL5" t="inlineStr"/>
+      <c r="AM5" t="inlineStr"/>
+    </row>
+    <row r="6">
+      <c r="A6" t="inlineStr"/>
+      <c r="B6" t="inlineStr"/>
+      <c r="C6" t="inlineStr"/>
+      <c r="D6" t="inlineStr"/>
+      <c r="E6" t="inlineStr"/>
+      <c r="F6" t="inlineStr"/>
+      <c r="G6" t="inlineStr"/>
+      <c r="H6" t="inlineStr"/>
+      <c r="I6" t="inlineStr"/>
+      <c r="J6" t="inlineStr"/>
+      <c r="K6" t="inlineStr"/>
+      <c r="L6" t="inlineStr"/>
+      <c r="M6" t="inlineStr"/>
+      <c r="N6" t="inlineStr"/>
+      <c r="O6" t="inlineStr"/>
+      <c r="P6" t="inlineStr"/>
+      <c r="Q6" t="inlineStr"/>
+      <c r="R6" t="inlineStr"/>
+      <c r="S6" t="inlineStr"/>
+      <c r="T6" t="inlineStr"/>
+      <c r="U6" t="inlineStr"/>
+      <c r="V6" t="inlineStr"/>
+      <c r="W6" t="inlineStr"/>
+      <c r="X6" t="inlineStr"/>
+      <c r="Y6" t="inlineStr"/>
+      <c r="Z6" t="inlineStr"/>
+      <c r="AA6" t="inlineStr"/>
+      <c r="AB6" t="inlineStr"/>
+      <c r="AC6" t="inlineStr"/>
+      <c r="AD6" t="inlineStr"/>
+      <c r="AE6" t="inlineStr"/>
+      <c r="AF6" t="inlineStr"/>
+      <c r="AG6" t="inlineStr"/>
+      <c r="AH6" t="inlineStr"/>
+      <c r="AI6" t="inlineStr"/>
+      <c r="AJ6" t="inlineStr"/>
+      <c r="AK6" t="inlineStr"/>
+      <c r="AL6" t="inlineStr"/>
+      <c r="AM6" t="inlineStr"/>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
@@ -1043,6 +1167,7 @@
       <c r="K7" t="n">
         <v>50.2</v>
       </c>
+      <c r="L7" t="inlineStr"/>
       <c r="M7" t="inlineStr">
         <is>
           <t>AMS</t>
@@ -1063,6 +1188,10 @@
           <t>NO</t>
         </is>
       </c>
+      <c r="Q7" t="inlineStr"/>
+      <c r="R7" t="inlineStr"/>
+      <c r="S7" t="inlineStr"/>
+      <c r="T7" t="inlineStr"/>
       <c r="U7" t="inlineStr">
         <is>
           <t>YES</t>
@@ -1111,6 +1240,56 @@
           <t>VM</t>
         </is>
       </c>
+      <c r="AE7" t="inlineStr"/>
+      <c r="AF7" t="inlineStr"/>
+      <c r="AG7" t="inlineStr"/>
+      <c r="AH7" t="inlineStr"/>
+      <c r="AI7" t="inlineStr"/>
+      <c r="AJ7" t="inlineStr"/>
+      <c r="AK7" t="inlineStr"/>
+      <c r="AL7" t="inlineStr"/>
+      <c r="AM7" t="inlineStr"/>
+    </row>
+    <row r="8">
+      <c r="A8" t="inlineStr"/>
+      <c r="B8" t="inlineStr"/>
+      <c r="C8" t="inlineStr"/>
+      <c r="D8" t="inlineStr"/>
+      <c r="E8" t="inlineStr"/>
+      <c r="F8" t="inlineStr"/>
+      <c r="G8" t="inlineStr"/>
+      <c r="H8" t="inlineStr"/>
+      <c r="I8" t="inlineStr"/>
+      <c r="J8" t="inlineStr"/>
+      <c r="K8" t="inlineStr"/>
+      <c r="L8" t="inlineStr"/>
+      <c r="M8" t="inlineStr"/>
+      <c r="N8" t="inlineStr"/>
+      <c r="O8" t="inlineStr"/>
+      <c r="P8" t="inlineStr"/>
+      <c r="Q8" t="inlineStr"/>
+      <c r="R8" t="inlineStr"/>
+      <c r="S8" t="inlineStr"/>
+      <c r="T8" t="inlineStr"/>
+      <c r="U8" t="inlineStr"/>
+      <c r="V8" t="inlineStr"/>
+      <c r="W8" t="inlineStr"/>
+      <c r="X8" t="inlineStr"/>
+      <c r="Y8" t="inlineStr"/>
+      <c r="Z8" t="inlineStr"/>
+      <c r="AA8" t="inlineStr"/>
+      <c r="AB8" t="inlineStr"/>
+      <c r="AC8" t="inlineStr"/>
+      <c r="AD8" t="inlineStr"/>
+      <c r="AE8" t="inlineStr"/>
+      <c r="AF8" t="inlineStr"/>
+      <c r="AG8" t="inlineStr"/>
+      <c r="AH8" t="inlineStr"/>
+      <c r="AI8" t="inlineStr"/>
+      <c r="AJ8" t="inlineStr"/>
+      <c r="AK8" t="inlineStr"/>
+      <c r="AL8" t="inlineStr"/>
+      <c r="AM8" t="inlineStr"/>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
@@ -1164,6 +1343,7 @@
       <c r="K9" t="n">
         <v>58.63</v>
       </c>
+      <c r="L9" t="inlineStr"/>
       <c r="M9" t="inlineStr">
         <is>
           <t>AMS</t>
@@ -1174,11 +1354,16 @@
           <t>LP</t>
         </is>
       </c>
+      <c r="O9" t="inlineStr"/>
       <c r="P9" t="inlineStr">
         <is>
           <t>NO</t>
         </is>
       </c>
+      <c r="Q9" t="inlineStr"/>
+      <c r="R9" t="inlineStr"/>
+      <c r="S9" t="inlineStr"/>
+      <c r="T9" t="inlineStr"/>
       <c r="U9" t="inlineStr">
         <is>
           <t>YES</t>
@@ -1227,6 +1412,56 @@
           <t>picked up</t>
         </is>
       </c>
+      <c r="AE9" t="inlineStr"/>
+      <c r="AF9" t="inlineStr"/>
+      <c r="AG9" t="inlineStr"/>
+      <c r="AH9" t="inlineStr"/>
+      <c r="AI9" t="inlineStr"/>
+      <c r="AJ9" t="inlineStr"/>
+      <c r="AK9" t="inlineStr"/>
+      <c r="AL9" t="inlineStr"/>
+      <c r="AM9" t="inlineStr"/>
+    </row>
+    <row r="10">
+      <c r="A10" t="inlineStr"/>
+      <c r="B10" t="inlineStr"/>
+      <c r="C10" t="inlineStr"/>
+      <c r="D10" t="inlineStr"/>
+      <c r="E10" t="inlineStr"/>
+      <c r="F10" t="inlineStr"/>
+      <c r="G10" t="inlineStr"/>
+      <c r="H10" t="inlineStr"/>
+      <c r="I10" t="inlineStr"/>
+      <c r="J10" t="inlineStr"/>
+      <c r="K10" t="inlineStr"/>
+      <c r="L10" t="inlineStr"/>
+      <c r="M10" t="inlineStr"/>
+      <c r="N10" t="inlineStr"/>
+      <c r="O10" t="inlineStr"/>
+      <c r="P10" t="inlineStr"/>
+      <c r="Q10" t="inlineStr"/>
+      <c r="R10" t="inlineStr"/>
+      <c r="S10" t="inlineStr"/>
+      <c r="T10" t="inlineStr"/>
+      <c r="U10" t="inlineStr"/>
+      <c r="V10" t="inlineStr"/>
+      <c r="W10" t="inlineStr"/>
+      <c r="X10" t="inlineStr"/>
+      <c r="Y10" t="inlineStr"/>
+      <c r="Z10" t="inlineStr"/>
+      <c r="AA10" t="inlineStr"/>
+      <c r="AB10" t="inlineStr"/>
+      <c r="AC10" t="inlineStr"/>
+      <c r="AD10" t="inlineStr"/>
+      <c r="AE10" t="inlineStr"/>
+      <c r="AF10" t="inlineStr"/>
+      <c r="AG10" t="inlineStr"/>
+      <c r="AH10" t="inlineStr"/>
+      <c r="AI10" t="inlineStr"/>
+      <c r="AJ10" t="inlineStr"/>
+      <c r="AK10" t="inlineStr"/>
+      <c r="AL10" t="inlineStr"/>
+      <c r="AM10" t="inlineStr"/>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr">
@@ -1280,6 +1515,7 @@
       <c r="K11" t="n">
         <v>199</v>
       </c>
+      <c r="L11" t="inlineStr"/>
       <c r="M11" t="inlineStr">
         <is>
           <t>AMA</t>
@@ -1300,19 +1536,39 @@
           <t>NO</t>
         </is>
       </c>
+      <c r="Q11" t="inlineStr"/>
+      <c r="R11" t="inlineStr"/>
+      <c r="S11" t="inlineStr"/>
+      <c r="T11" t="inlineStr"/>
       <c r="U11" t="inlineStr">
         <is>
           <t>NO</t>
         </is>
       </c>
+      <c r="V11" t="inlineStr"/>
+      <c r="W11" t="inlineStr"/>
       <c r="X11" t="inlineStr">
         <is>
           <t>NO</t>
         </is>
       </c>
+      <c r="Y11" t="inlineStr"/>
+      <c r="Z11" t="inlineStr"/>
       <c r="AA11" t="n">
         <v>0</v>
       </c>
+      <c r="AB11" t="inlineStr"/>
+      <c r="AC11" t="inlineStr"/>
+      <c r="AD11" t="inlineStr"/>
+      <c r="AE11" t="inlineStr"/>
+      <c r="AF11" t="inlineStr"/>
+      <c r="AG11" t="inlineStr"/>
+      <c r="AH11" t="inlineStr"/>
+      <c r="AI11" t="inlineStr"/>
+      <c r="AJ11" t="inlineStr"/>
+      <c r="AK11" t="inlineStr"/>
+      <c r="AL11" t="inlineStr"/>
+      <c r="AM11" t="inlineStr"/>
     </row>
     <row r="12">
       <c r="A12" t="inlineStr">
@@ -1366,6 +1622,7 @@
       <c r="K12" t="n">
         <v>15</v>
       </c>
+      <c r="L12" t="inlineStr"/>
       <c r="M12" t="inlineStr">
         <is>
           <t>AMA</t>
@@ -1386,6 +1643,10 @@
           <t>NO</t>
         </is>
       </c>
+      <c r="Q12" t="inlineStr"/>
+      <c r="R12" t="inlineStr"/>
+      <c r="S12" t="inlineStr"/>
+      <c r="T12" t="inlineStr"/>
       <c r="U12" t="inlineStr">
         <is>
           <t>YES</t>
@@ -1419,6 +1680,59 @@
       <c r="AA12" t="n">
         <v>0</v>
       </c>
+      <c r="AB12" t="inlineStr"/>
+      <c r="AC12" t="inlineStr"/>
+      <c r="AD12" t="inlineStr"/>
+      <c r="AE12" t="inlineStr"/>
+      <c r="AF12" t="inlineStr"/>
+      <c r="AG12" t="inlineStr"/>
+      <c r="AH12" t="inlineStr"/>
+      <c r="AI12" t="inlineStr"/>
+      <c r="AJ12" t="inlineStr"/>
+      <c r="AK12" t="inlineStr"/>
+      <c r="AL12" t="inlineStr"/>
+      <c r="AM12" t="inlineStr"/>
+    </row>
+    <row r="13">
+      <c r="A13" t="inlineStr"/>
+      <c r="B13" t="inlineStr"/>
+      <c r="C13" t="inlineStr"/>
+      <c r="D13" t="inlineStr"/>
+      <c r="E13" t="inlineStr"/>
+      <c r="F13" t="inlineStr"/>
+      <c r="G13" t="inlineStr"/>
+      <c r="H13" t="inlineStr"/>
+      <c r="I13" t="inlineStr"/>
+      <c r="J13" t="inlineStr"/>
+      <c r="K13" t="inlineStr"/>
+      <c r="L13" t="inlineStr"/>
+      <c r="M13" t="inlineStr"/>
+      <c r="N13" t="inlineStr"/>
+      <c r="O13" t="inlineStr"/>
+      <c r="P13" t="inlineStr"/>
+      <c r="Q13" t="inlineStr"/>
+      <c r="R13" t="inlineStr"/>
+      <c r="S13" t="inlineStr"/>
+      <c r="T13" t="inlineStr"/>
+      <c r="U13" t="inlineStr"/>
+      <c r="V13" t="inlineStr"/>
+      <c r="W13" t="inlineStr"/>
+      <c r="X13" t="inlineStr"/>
+      <c r="Y13" t="inlineStr"/>
+      <c r="Z13" t="inlineStr"/>
+      <c r="AA13" t="inlineStr"/>
+      <c r="AB13" t="inlineStr"/>
+      <c r="AC13" t="inlineStr"/>
+      <c r="AD13" t="inlineStr"/>
+      <c r="AE13" t="inlineStr"/>
+      <c r="AF13" t="inlineStr"/>
+      <c r="AG13" t="inlineStr"/>
+      <c r="AH13" t="inlineStr"/>
+      <c r="AI13" t="inlineStr"/>
+      <c r="AJ13" t="inlineStr"/>
+      <c r="AK13" t="inlineStr"/>
+      <c r="AL13" t="inlineStr"/>
+      <c r="AM13" t="inlineStr"/>
     </row>
     <row r="14">
       <c r="A14" t="inlineStr">
@@ -1472,6 +1786,7 @@
       <c r="K14" t="n">
         <v>20</v>
       </c>
+      <c r="L14" t="inlineStr"/>
       <c r="M14" t="inlineStr">
         <is>
           <t>AMS</t>
@@ -1492,6 +1807,10 @@
           <t>PICKUP</t>
         </is>
       </c>
+      <c r="Q14" t="inlineStr"/>
+      <c r="R14" t="inlineStr"/>
+      <c r="S14" t="inlineStr"/>
+      <c r="T14" t="inlineStr"/>
       <c r="U14" t="inlineStr">
         <is>
           <t>YES</t>
@@ -1540,6 +1859,15 @@
           <t>VM</t>
         </is>
       </c>
+      <c r="AE14" t="inlineStr"/>
+      <c r="AF14" t="inlineStr"/>
+      <c r="AG14" t="inlineStr"/>
+      <c r="AH14" t="inlineStr"/>
+      <c r="AI14" t="inlineStr"/>
+      <c r="AJ14" t="inlineStr"/>
+      <c r="AK14" t="inlineStr"/>
+      <c r="AL14" t="inlineStr"/>
+      <c r="AM14" t="inlineStr"/>
     </row>
     <row r="15">
       <c r="A15" t="inlineStr">
@@ -1593,6 +1921,7 @@
       <c r="K15" t="n">
         <v>87</v>
       </c>
+      <c r="L15" t="inlineStr"/>
       <c r="M15" t="inlineStr">
         <is>
           <t>AMA</t>
@@ -1613,6 +1942,10 @@
           <t>PICKUP</t>
         </is>
       </c>
+      <c r="Q15" t="inlineStr"/>
+      <c r="R15" t="inlineStr"/>
+      <c r="S15" t="inlineStr"/>
+      <c r="T15" t="inlineStr"/>
       <c r="U15" t="inlineStr">
         <is>
           <t>YES</t>
@@ -1661,6 +1994,15 @@
           <t>VM</t>
         </is>
       </c>
+      <c r="AE15" t="inlineStr"/>
+      <c r="AF15" t="inlineStr"/>
+      <c r="AG15" t="inlineStr"/>
+      <c r="AH15" t="inlineStr"/>
+      <c r="AI15" t="inlineStr"/>
+      <c r="AJ15" t="inlineStr"/>
+      <c r="AK15" t="inlineStr"/>
+      <c r="AL15" t="inlineStr"/>
+      <c r="AM15" t="inlineStr"/>
     </row>
     <row r="16">
       <c r="A16" t="inlineStr">
@@ -1714,6 +2056,7 @@
       <c r="K16" t="n">
         <v>89.98999999999999</v>
       </c>
+      <c r="L16" t="inlineStr"/>
       <c r="M16" t="inlineStr">
         <is>
           <t>AMA</t>
@@ -1734,6 +2077,10 @@
           <t>PICKUP</t>
         </is>
       </c>
+      <c r="Q16" t="inlineStr"/>
+      <c r="R16" t="inlineStr"/>
+      <c r="S16" t="inlineStr"/>
+      <c r="T16" t="inlineStr"/>
       <c r="U16" t="inlineStr">
         <is>
           <t>YES</t>
@@ -1782,6 +2129,56 @@
           <t>PICKED UP</t>
         </is>
       </c>
+      <c r="AE16" t="inlineStr"/>
+      <c r="AF16" t="inlineStr"/>
+      <c r="AG16" t="inlineStr"/>
+      <c r="AH16" t="inlineStr"/>
+      <c r="AI16" t="inlineStr"/>
+      <c r="AJ16" t="inlineStr"/>
+      <c r="AK16" t="inlineStr"/>
+      <c r="AL16" t="inlineStr"/>
+      <c r="AM16" t="inlineStr"/>
+    </row>
+    <row r="17">
+      <c r="A17" t="inlineStr"/>
+      <c r="B17" t="inlineStr"/>
+      <c r="C17" t="inlineStr"/>
+      <c r="D17" t="inlineStr"/>
+      <c r="E17" t="inlineStr"/>
+      <c r="F17" t="inlineStr"/>
+      <c r="G17" t="inlineStr"/>
+      <c r="H17" t="inlineStr"/>
+      <c r="I17" t="inlineStr"/>
+      <c r="J17" t="inlineStr"/>
+      <c r="K17" t="inlineStr"/>
+      <c r="L17" t="inlineStr"/>
+      <c r="M17" t="inlineStr"/>
+      <c r="N17" t="inlineStr"/>
+      <c r="O17" t="inlineStr"/>
+      <c r="P17" t="inlineStr"/>
+      <c r="Q17" t="inlineStr"/>
+      <c r="R17" t="inlineStr"/>
+      <c r="S17" t="inlineStr"/>
+      <c r="T17" t="inlineStr"/>
+      <c r="U17" t="inlineStr"/>
+      <c r="V17" t="inlineStr"/>
+      <c r="W17" t="inlineStr"/>
+      <c r="X17" t="inlineStr"/>
+      <c r="Y17" t="inlineStr"/>
+      <c r="Z17" t="inlineStr"/>
+      <c r="AA17" t="inlineStr"/>
+      <c r="AB17" t="inlineStr"/>
+      <c r="AC17" t="inlineStr"/>
+      <c r="AD17" t="inlineStr"/>
+      <c r="AE17" t="inlineStr"/>
+      <c r="AF17" t="inlineStr"/>
+      <c r="AG17" t="inlineStr"/>
+      <c r="AH17" t="inlineStr"/>
+      <c r="AI17" t="inlineStr"/>
+      <c r="AJ17" t="inlineStr"/>
+      <c r="AK17" t="inlineStr"/>
+      <c r="AL17" t="inlineStr"/>
+      <c r="AM17" t="inlineStr"/>
     </row>
     <row r="18">
       <c r="A18" t="inlineStr">
@@ -1835,6 +2232,7 @@
       <c r="K18" t="n">
         <v>15</v>
       </c>
+      <c r="L18" t="inlineStr"/>
       <c r="M18" t="inlineStr">
         <is>
           <t>AMS</t>
@@ -1855,6 +2253,10 @@
           <t>PICKUP</t>
         </is>
       </c>
+      <c r="Q18" t="inlineStr"/>
+      <c r="R18" t="inlineStr"/>
+      <c r="S18" t="inlineStr"/>
+      <c r="T18" t="inlineStr"/>
       <c r="U18" t="inlineStr">
         <is>
           <t>YES</t>
@@ -1918,6 +2320,12 @@
           <t>abake</t>
         </is>
       </c>
+      <c r="AH18" t="inlineStr"/>
+      <c r="AI18" t="inlineStr"/>
+      <c r="AJ18" t="inlineStr"/>
+      <c r="AK18" t="inlineStr"/>
+      <c r="AL18" t="inlineStr"/>
+      <c r="AM18" t="inlineStr"/>
     </row>
     <row r="19">
       <c r="A19" t="inlineStr">
@@ -1971,6 +2379,7 @@
       <c r="K19" t="n">
         <v>50.99</v>
       </c>
+      <c r="L19" t="inlineStr"/>
       <c r="M19" t="inlineStr">
         <is>
           <t>AMS</t>
@@ -2074,6 +2483,12 @@
           <t>abake</t>
         </is>
       </c>
+      <c r="AH19" t="inlineStr"/>
+      <c r="AI19" t="inlineStr"/>
+      <c r="AJ19" t="inlineStr"/>
+      <c r="AK19" t="inlineStr"/>
+      <c r="AL19" t="inlineStr"/>
+      <c r="AM19" t="inlineStr"/>
     </row>
     <row r="20">
       <c r="A20" t="inlineStr">
@@ -2127,6 +2542,7 @@
       <c r="K20" t="n">
         <v>90</v>
       </c>
+      <c r="L20" t="inlineStr"/>
       <c r="M20" t="inlineStr">
         <is>
           <t>AMS</t>
@@ -2147,6 +2563,10 @@
           <t>PICKUP</t>
         </is>
       </c>
+      <c r="Q20" t="inlineStr"/>
+      <c r="R20" t="inlineStr"/>
+      <c r="S20" t="inlineStr"/>
+      <c r="T20" t="inlineStr"/>
       <c r="U20" t="inlineStr">
         <is>
           <t>YES</t>
@@ -2293,6 +2713,7 @@
       <c r="K21" t="n">
         <v>822</v>
       </c>
+      <c r="L21" t="inlineStr"/>
       <c r="M21" t="inlineStr">
         <is>
           <t>AEC</t>
@@ -2313,6 +2734,10 @@
           <t>PICKUP</t>
         </is>
       </c>
+      <c r="Q21" t="inlineStr"/>
+      <c r="R21" t="inlineStr"/>
+      <c r="S21" t="inlineStr"/>
+      <c r="T21" t="inlineStr"/>
       <c r="U21" t="inlineStr">
         <is>
           <t>YES</t>
@@ -2333,9 +2758,23 @@
           <t>NO</t>
         </is>
       </c>
+      <c r="Y21" t="inlineStr"/>
+      <c r="Z21" t="inlineStr"/>
       <c r="AA21" t="n">
         <v>0</v>
       </c>
+      <c r="AB21" t="inlineStr"/>
+      <c r="AC21" t="inlineStr"/>
+      <c r="AD21" t="inlineStr"/>
+      <c r="AE21" t="inlineStr"/>
+      <c r="AF21" t="inlineStr"/>
+      <c r="AG21" t="inlineStr"/>
+      <c r="AH21" t="inlineStr"/>
+      <c r="AI21" t="inlineStr"/>
+      <c r="AJ21" t="inlineStr"/>
+      <c r="AK21" t="inlineStr"/>
+      <c r="AL21" t="inlineStr"/>
+      <c r="AM21" t="inlineStr"/>
     </row>
     <row r="22">
       <c r="A22" t="inlineStr">
@@ -2488,6 +2927,15 @@
           <t> </t>
         </is>
       </c>
+      <c r="AE22" t="inlineStr"/>
+      <c r="AF22" t="inlineStr"/>
+      <c r="AG22" t="inlineStr"/>
+      <c r="AH22" t="inlineStr"/>
+      <c r="AI22" t="inlineStr"/>
+      <c r="AJ22" t="inlineStr"/>
+      <c r="AK22" t="inlineStr"/>
+      <c r="AL22" t="inlineStr"/>
+      <c r="AM22" t="inlineStr"/>
     </row>
     <row r="23">
       <c r="A23" t="inlineStr">
@@ -2566,6 +3014,10 @@
           <t>PICKUP</t>
         </is>
       </c>
+      <c r="Q23" t="inlineStr"/>
+      <c r="R23" t="inlineStr"/>
+      <c r="S23" t="inlineStr"/>
+      <c r="T23" t="inlineStr"/>
       <c r="U23" t="inlineStr">
         <is>
           <t>YES</t>
@@ -2599,6 +3051,18 @@
       <c r="AA23" t="n">
         <v>0</v>
       </c>
+      <c r="AB23" t="inlineStr"/>
+      <c r="AC23" t="inlineStr"/>
+      <c r="AD23" t="inlineStr"/>
+      <c r="AE23" t="inlineStr"/>
+      <c r="AF23" t="inlineStr"/>
+      <c r="AG23" t="inlineStr"/>
+      <c r="AH23" t="inlineStr"/>
+      <c r="AI23" t="inlineStr"/>
+      <c r="AJ23" t="inlineStr"/>
+      <c r="AK23" t="inlineStr"/>
+      <c r="AL23" t="inlineStr"/>
+      <c r="AM23" t="inlineStr"/>
     </row>
     <row r="24">
       <c r="A24" t="inlineStr">
@@ -2677,6 +3141,10 @@
           <t>PICKUP</t>
         </is>
       </c>
+      <c r="Q24" t="inlineStr"/>
+      <c r="R24" t="inlineStr"/>
+      <c r="S24" t="inlineStr"/>
+      <c r="T24" t="inlineStr"/>
       <c r="U24" t="inlineStr">
         <is>
           <t>YES</t>
@@ -2755,6 +3223,9 @@
           <t>abake</t>
         </is>
       </c>
+      <c r="AK24" t="inlineStr"/>
+      <c r="AL24" t="inlineStr"/>
+      <c r="AM24" t="inlineStr"/>
     </row>
     <row r="25">
       <c r="A25" t="inlineStr">
@@ -2833,6 +3304,10 @@
           <t>PICKUP</t>
         </is>
       </c>
+      <c r="Q25" t="inlineStr"/>
+      <c r="R25" t="inlineStr"/>
+      <c r="S25" t="inlineStr"/>
+      <c r="T25" t="inlineStr"/>
       <c r="U25" t="inlineStr">
         <is>
           <t>YES</t>
@@ -2911,6 +3386,9 @@
           <t>abake</t>
         </is>
       </c>
+      <c r="AK25" t="inlineStr"/>
+      <c r="AL25" t="inlineStr"/>
+      <c r="AM25" t="inlineStr"/>
     </row>
     <row r="26">
       <c r="A26" t="inlineStr">
@@ -2989,6 +3467,10 @@
           <t>PICKUP</t>
         </is>
       </c>
+      <c r="Q26" t="inlineStr"/>
+      <c r="R26" t="inlineStr"/>
+      <c r="S26" t="inlineStr"/>
+      <c r="T26" t="inlineStr"/>
       <c r="U26" t="inlineStr">
         <is>
           <t>YES</t>
@@ -3052,6 +3534,12 @@
           <t>abake</t>
         </is>
       </c>
+      <c r="AH26" t="inlineStr"/>
+      <c r="AI26" t="inlineStr"/>
+      <c r="AJ26" t="inlineStr"/>
+      <c r="AK26" t="inlineStr"/>
+      <c r="AL26" t="inlineStr"/>
+      <c r="AM26" t="inlineStr"/>
     </row>
     <row r="27">
       <c r="A27" t="inlineStr">
@@ -3130,6 +3618,10 @@
           <t>PICKUP</t>
         </is>
       </c>
+      <c r="Q27" t="inlineStr"/>
+      <c r="R27" t="inlineStr"/>
+      <c r="S27" t="inlineStr"/>
+      <c r="T27" t="inlineStr"/>
       <c r="U27" t="inlineStr">
         <is>
           <t>YES</t>
@@ -3208,6 +3700,9 @@
           <t>abake</t>
         </is>
       </c>
+      <c r="AK27" t="inlineStr"/>
+      <c r="AL27" t="inlineStr"/>
+      <c r="AM27" t="inlineStr"/>
     </row>
     <row r="28">
       <c r="A28" t="inlineStr">
@@ -3405,6 +3900,133 @@
           <t> </t>
         </is>
       </c>
+    </row>
+    <row r="29">
+      <c r="A29" t="inlineStr">
+        <is>
+          <t>03/14/2024</t>
+        </is>
+      </c>
+      <c r="B29" t="inlineStr">
+        <is>
+          <t>SO240314001</t>
+        </is>
+      </c>
+      <c r="C29" t="inlineStr">
+        <is>
+          <t>ab</t>
+        </is>
+      </c>
+      <c r="D29" t="inlineStr">
+        <is>
+          <t>abs@abc.com</t>
+        </is>
+      </c>
+      <c r="E29" t="inlineStr">
+        <is>
+          <t>(789)456-1233</t>
+        </is>
+      </c>
+      <c r="F29" t="inlineStr">
+        <is>
+          <t>YES</t>
+        </is>
+      </c>
+      <c r="G29" t="inlineStr">
+        <is>
+          <t>YES</t>
+        </is>
+      </c>
+      <c r="H29" t="inlineStr">
+        <is>
+          <t>artist</t>
+        </is>
+      </c>
+      <c r="I29" t="inlineStr">
+        <is>
+          <t>title</t>
+        </is>
+      </c>
+      <c r="J29" t="n">
+        <v>10</v>
+      </c>
+      <c r="K29" t="n">
+        <v>85</v>
+      </c>
+      <c r="L29" t="inlineStr">
+        <is>
+          <t> </t>
+        </is>
+      </c>
+      <c r="M29" t="inlineStr">
+        <is>
+          <t>Ebay</t>
+        </is>
+      </c>
+      <c r="N29" t="inlineStr">
+        <is>
+          <t>LP</t>
+        </is>
+      </c>
+      <c r="O29" t="inlineStr">
+        <is>
+          <t>abake</t>
+        </is>
+      </c>
+      <c r="P29" t="inlineStr">
+        <is>
+          <t>PICKUP</t>
+        </is>
+      </c>
+      <c r="Q29" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="R29" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="S29" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="T29" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="U29" t="inlineStr">
+        <is>
+          <t>NO</t>
+        </is>
+      </c>
+      <c r="V29" t="inlineStr"/>
+      <c r="W29" t="inlineStr"/>
+      <c r="X29" t="inlineStr">
+        <is>
+          <t>NO</t>
+        </is>
+      </c>
+      <c r="Y29" t="inlineStr"/>
+      <c r="Z29" t="inlineStr"/>
+      <c r="AA29" t="n">
+        <v>0</v>
+      </c>
+      <c r="AB29" t="inlineStr"/>
+      <c r="AC29" t="inlineStr"/>
+      <c r="AD29" t="inlineStr"/>
+      <c r="AE29" t="inlineStr"/>
+      <c r="AF29" t="inlineStr"/>
+      <c r="AG29" t="inlineStr"/>
+      <c r="AH29" t="inlineStr"/>
+      <c r="AI29" t="inlineStr"/>
+      <c r="AJ29" t="inlineStr"/>
+      <c r="AK29" t="inlineStr"/>
+      <c r="AL29" t="inlineStr"/>
+      <c r="AM29" t="inlineStr"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>

<commit_message>
modifying main and adding comments
</commit_message>
<xml_diff>
--- a/SO_Test.xlsx
+++ b/SO_Test.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:AM29"/>
+  <dimension ref="A1:AM32"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -3904,129 +3904,548 @@
     <row r="29">
       <c r="A29" t="inlineStr">
         <is>
-          <t>03/14/2024</t>
+          <t> </t>
         </is>
       </c>
       <c r="B29" t="inlineStr">
         <is>
-          <t>SO240314001</t>
+          <t> </t>
         </is>
       </c>
       <c r="C29" t="inlineStr">
         <is>
+          <t> </t>
+        </is>
+      </c>
+      <c r="D29" t="inlineStr">
+        <is>
+          <t> </t>
+        </is>
+      </c>
+      <c r="E29" t="inlineStr">
+        <is>
+          <t> </t>
+        </is>
+      </c>
+      <c r="F29" t="inlineStr">
+        <is>
+          <t> </t>
+        </is>
+      </c>
+      <c r="G29" t="inlineStr">
+        <is>
+          <t> </t>
+        </is>
+      </c>
+      <c r="H29" t="inlineStr">
+        <is>
+          <t> </t>
+        </is>
+      </c>
+      <c r="I29" t="inlineStr">
+        <is>
+          <t> </t>
+        </is>
+      </c>
+      <c r="J29" t="inlineStr">
+        <is>
+          <t> </t>
+        </is>
+      </c>
+      <c r="K29" t="inlineStr">
+        <is>
+          <t> </t>
+        </is>
+      </c>
+      <c r="L29" t="inlineStr">
+        <is>
+          <t> </t>
+        </is>
+      </c>
+      <c r="M29" t="inlineStr">
+        <is>
+          <t> </t>
+        </is>
+      </c>
+      <c r="N29" t="inlineStr">
+        <is>
+          <t> </t>
+        </is>
+      </c>
+      <c r="O29" t="inlineStr">
+        <is>
+          <t> </t>
+        </is>
+      </c>
+      <c r="P29" t="inlineStr">
+        <is>
+          <t> </t>
+        </is>
+      </c>
+      <c r="Q29" t="inlineStr">
+        <is>
+          <t> </t>
+        </is>
+      </c>
+      <c r="R29" t="inlineStr">
+        <is>
+          <t> </t>
+        </is>
+      </c>
+      <c r="S29" t="inlineStr">
+        <is>
+          <t> </t>
+        </is>
+      </c>
+      <c r="T29" t="inlineStr">
+        <is>
+          <t> </t>
+        </is>
+      </c>
+      <c r="U29" t="inlineStr">
+        <is>
+          <t> </t>
+        </is>
+      </c>
+      <c r="V29" t="inlineStr">
+        <is>
+          <t> </t>
+        </is>
+      </c>
+      <c r="W29" t="inlineStr">
+        <is>
+          <t> </t>
+        </is>
+      </c>
+      <c r="X29" t="inlineStr">
+        <is>
+          <t> </t>
+        </is>
+      </c>
+      <c r="Y29" t="inlineStr">
+        <is>
+          <t> </t>
+        </is>
+      </c>
+      <c r="Z29" t="inlineStr">
+        <is>
+          <t> </t>
+        </is>
+      </c>
+      <c r="AA29" t="inlineStr">
+        <is>
+          <t> </t>
+        </is>
+      </c>
+      <c r="AB29" t="inlineStr">
+        <is>
+          <t> </t>
+        </is>
+      </c>
+      <c r="AC29" t="inlineStr">
+        <is>
+          <t> </t>
+        </is>
+      </c>
+      <c r="AD29" t="inlineStr">
+        <is>
+          <t> </t>
+        </is>
+      </c>
+      <c r="AE29" t="inlineStr">
+        <is>
+          <t> </t>
+        </is>
+      </c>
+      <c r="AF29" t="inlineStr">
+        <is>
+          <t> </t>
+        </is>
+      </c>
+      <c r="AG29" t="inlineStr">
+        <is>
+          <t> </t>
+        </is>
+      </c>
+      <c r="AH29" t="inlineStr">
+        <is>
+          <t> </t>
+        </is>
+      </c>
+      <c r="AI29" t="inlineStr">
+        <is>
+          <t> </t>
+        </is>
+      </c>
+      <c r="AJ29" t="inlineStr">
+        <is>
+          <t> </t>
+        </is>
+      </c>
+      <c r="AK29" t="inlineStr">
+        <is>
+          <t> </t>
+        </is>
+      </c>
+      <c r="AL29" t="inlineStr">
+        <is>
+          <t> </t>
+        </is>
+      </c>
+      <c r="AM29" t="inlineStr">
+        <is>
+          <t> </t>
+        </is>
+      </c>
+    </row>
+    <row r="30">
+      <c r="A30" t="inlineStr">
+        <is>
+          <t>03/15/2024</t>
+        </is>
+      </c>
+      <c r="B30" t="inlineStr">
+        <is>
+          <t>SO240315001</t>
+        </is>
+      </c>
+      <c r="C30" t="inlineStr">
+        <is>
           <t>ab</t>
         </is>
       </c>
-      <c r="D29" t="inlineStr">
-        <is>
-          <t>abs@abc.com</t>
-        </is>
-      </c>
-      <c r="E29" t="inlineStr">
-        <is>
-          <t>(789)456-1233</t>
-        </is>
-      </c>
-      <c r="F29" t="inlineStr">
-        <is>
-          <t>YES</t>
-        </is>
-      </c>
-      <c r="G29" t="inlineStr">
-        <is>
-          <t>YES</t>
-        </is>
-      </c>
-      <c r="H29" t="inlineStr">
+      <c r="D30" t="inlineStr">
+        <is>
+          <t>abaker3003@gmail.com</t>
+        </is>
+      </c>
+      <c r="E30" t="inlineStr">
+        <is>
+          <t>(915)799-4875</t>
+        </is>
+      </c>
+      <c r="F30" t="inlineStr">
+        <is>
+          <t>YES</t>
+        </is>
+      </c>
+      <c r="G30" t="inlineStr">
+        <is>
+          <t>YES</t>
+        </is>
+      </c>
+      <c r="H30" t="inlineStr">
+        <is>
+          <t>Tool</t>
+        </is>
+      </c>
+      <c r="I30" t="inlineStr">
+        <is>
+          <t>Aenima</t>
+        </is>
+      </c>
+      <c r="J30" t="n">
+        <v>50</v>
+      </c>
+      <c r="K30" t="n">
+        <v>150</v>
+      </c>
+      <c r="L30" t="inlineStr">
+        <is>
+          <t> </t>
+        </is>
+      </c>
+      <c r="M30" t="inlineStr">
+        <is>
+          <t>AEC</t>
+        </is>
+      </c>
+      <c r="N30" t="inlineStr">
+        <is>
+          <t>CD</t>
+        </is>
+      </c>
+      <c r="O30" t="inlineStr">
+        <is>
+          <t>abake</t>
+        </is>
+      </c>
+      <c r="P30" t="inlineStr">
+        <is>
+          <t>PICKUP</t>
+        </is>
+      </c>
+      <c r="Q30" t="inlineStr"/>
+      <c r="R30" t="inlineStr"/>
+      <c r="S30" t="inlineStr"/>
+      <c r="T30" t="inlineStr"/>
+      <c r="U30" t="inlineStr">
+        <is>
+          <t>NO</t>
+        </is>
+      </c>
+      <c r="V30" t="inlineStr"/>
+      <c r="W30" t="inlineStr"/>
+      <c r="X30" t="inlineStr">
+        <is>
+          <t>NO</t>
+        </is>
+      </c>
+      <c r="Y30" t="inlineStr"/>
+      <c r="Z30" t="inlineStr"/>
+      <c r="AA30" t="n">
+        <v>0</v>
+      </c>
+      <c r="AB30" t="inlineStr"/>
+      <c r="AC30" t="inlineStr"/>
+      <c r="AD30" t="inlineStr"/>
+      <c r="AE30" t="inlineStr"/>
+      <c r="AF30" t="inlineStr"/>
+      <c r="AG30" t="inlineStr"/>
+      <c r="AH30" t="inlineStr"/>
+      <c r="AI30" t="inlineStr"/>
+      <c r="AJ30" t="inlineStr"/>
+      <c r="AK30" t="inlineStr"/>
+      <c r="AL30" t="inlineStr"/>
+      <c r="AM30" t="inlineStr"/>
+    </row>
+    <row r="31">
+      <c r="A31" t="inlineStr">
+        <is>
+          <t>03/15/2024</t>
+        </is>
+      </c>
+      <c r="B31" t="inlineStr">
+        <is>
+          <t>SO240315002</t>
+        </is>
+      </c>
+      <c r="C31" t="inlineStr">
+        <is>
+          <t>ab</t>
+        </is>
+      </c>
+      <c r="D31" t="inlineStr">
+        <is>
+          <t>a.baker3003@gmailcom</t>
+        </is>
+      </c>
+      <c r="E31" t="inlineStr">
+        <is>
+          <t>(915)799-4875</t>
+        </is>
+      </c>
+      <c r="F31" t="inlineStr">
+        <is>
+          <t>YES</t>
+        </is>
+      </c>
+      <c r="G31" t="inlineStr">
+        <is>
+          <t>YES</t>
+        </is>
+      </c>
+      <c r="H31" t="inlineStr">
+        <is>
+          <t>TOOL</t>
+        </is>
+      </c>
+      <c r="I31" t="inlineStr">
+        <is>
+          <t>Lateralus</t>
+        </is>
+      </c>
+      <c r="J31" t="n">
+        <v>25</v>
+      </c>
+      <c r="K31" t="n">
+        <v>148</v>
+      </c>
+      <c r="L31" t="inlineStr">
+        <is>
+          <t> </t>
+        </is>
+      </c>
+      <c r="M31" t="inlineStr">
+        <is>
+          <t>AMS</t>
+        </is>
+      </c>
+      <c r="N31" t="inlineStr">
+        <is>
+          <t>LP</t>
+        </is>
+      </c>
+      <c r="O31" t="inlineStr">
+        <is>
+          <t>abake</t>
+        </is>
+      </c>
+      <c r="P31" t="inlineStr">
+        <is>
+          <t>PICKUP</t>
+        </is>
+      </c>
+      <c r="Q31" t="inlineStr"/>
+      <c r="R31" t="inlineStr"/>
+      <c r="S31" t="inlineStr"/>
+      <c r="T31" t="inlineStr"/>
+      <c r="U31" t="inlineStr">
+        <is>
+          <t>NO</t>
+        </is>
+      </c>
+      <c r="V31" t="inlineStr"/>
+      <c r="W31" t="inlineStr"/>
+      <c r="X31" t="inlineStr">
+        <is>
+          <t>NO</t>
+        </is>
+      </c>
+      <c r="Y31" t="inlineStr"/>
+      <c r="Z31" t="inlineStr"/>
+      <c r="AA31" t="n">
+        <v>0</v>
+      </c>
+      <c r="AB31" t="inlineStr"/>
+      <c r="AC31" t="inlineStr"/>
+      <c r="AD31" t="inlineStr"/>
+      <c r="AE31" t="inlineStr"/>
+      <c r="AF31" t="inlineStr"/>
+      <c r="AG31" t="inlineStr"/>
+      <c r="AH31" t="inlineStr"/>
+      <c r="AI31" t="inlineStr"/>
+      <c r="AJ31" t="inlineStr"/>
+      <c r="AK31" t="inlineStr"/>
+      <c r="AL31" t="inlineStr"/>
+      <c r="AM31" t="inlineStr"/>
+    </row>
+    <row r="32">
+      <c r="A32" t="inlineStr">
+        <is>
+          <t>03/15/2024</t>
+        </is>
+      </c>
+      <c r="B32" t="inlineStr">
+        <is>
+          <t>SO240315003</t>
+        </is>
+      </c>
+      <c r="C32" t="inlineStr">
+        <is>
+          <t>ab</t>
+        </is>
+      </c>
+      <c r="D32" t="inlineStr">
+        <is>
+          <t>somethingsimple6767@gmail.com</t>
+        </is>
+      </c>
+      <c r="E32" t="inlineStr">
+        <is>
+          <t>(915)799-4875</t>
+        </is>
+      </c>
+      <c r="F32" t="inlineStr">
+        <is>
+          <t>YES</t>
+        </is>
+      </c>
+      <c r="G32" t="inlineStr">
+        <is>
+          <t>YES</t>
+        </is>
+      </c>
+      <c r="H32" t="inlineStr">
         <is>
           <t>artist</t>
         </is>
       </c>
-      <c r="I29" t="inlineStr">
+      <c r="I32" t="inlineStr">
         <is>
           <t>title</t>
         </is>
       </c>
-      <c r="J29" t="n">
-        <v>10</v>
-      </c>
-      <c r="K29" t="n">
-        <v>85</v>
-      </c>
-      <c r="L29" t="inlineStr">
-        <is>
-          <t> </t>
-        </is>
-      </c>
-      <c r="M29" t="inlineStr">
-        <is>
-          <t>Ebay</t>
-        </is>
-      </c>
-      <c r="N29" t="inlineStr">
-        <is>
-          <t>LP</t>
-        </is>
-      </c>
-      <c r="O29" t="inlineStr">
-        <is>
-          <t>abake</t>
-        </is>
-      </c>
-      <c r="P29" t="inlineStr">
+      <c r="J32" t="n">
+        <v>5</v>
+      </c>
+      <c r="K32" t="n">
+        <v>65</v>
+      </c>
+      <c r="L32" t="inlineStr">
+        <is>
+          <t> </t>
+        </is>
+      </c>
+      <c r="M32" t="inlineStr">
+        <is>
+          <t>OTHER</t>
+        </is>
+      </c>
+      <c r="N32" t="inlineStr">
+        <is>
+          <t>OTHER</t>
+        </is>
+      </c>
+      <c r="O32" t="inlineStr">
+        <is>
+          <t>abake</t>
+        </is>
+      </c>
+      <c r="P32" t="inlineStr">
         <is>
           <t>PICKUP</t>
         </is>
       </c>
-      <c r="Q29" t="inlineStr">
+      <c r="Q32" t="inlineStr">
         <is>
           <t>N/A</t>
         </is>
       </c>
-      <c r="R29" t="inlineStr">
+      <c r="R32" t="inlineStr">
         <is>
           <t>N/A</t>
         </is>
       </c>
-      <c r="S29" t="inlineStr">
+      <c r="S32" t="inlineStr">
         <is>
           <t>N/A</t>
         </is>
       </c>
-      <c r="T29" t="inlineStr">
+      <c r="T32" t="inlineStr">
         <is>
           <t>N/A</t>
         </is>
       </c>
-      <c r="U29" t="inlineStr">
+      <c r="U32" t="inlineStr">
         <is>
           <t>NO</t>
         </is>
       </c>
-      <c r="V29" t="inlineStr"/>
-      <c r="W29" t="inlineStr"/>
-      <c r="X29" t="inlineStr">
+      <c r="V32" t="inlineStr"/>
+      <c r="W32" t="inlineStr"/>
+      <c r="X32" t="inlineStr">
         <is>
           <t>NO</t>
         </is>
       </c>
-      <c r="Y29" t="inlineStr"/>
-      <c r="Z29" t="inlineStr"/>
-      <c r="AA29" t="n">
+      <c r="Y32" t="inlineStr"/>
+      <c r="Z32" t="inlineStr"/>
+      <c r="AA32" t="n">
         <v>0</v>
       </c>
-      <c r="AB29" t="inlineStr"/>
-      <c r="AC29" t="inlineStr"/>
-      <c r="AD29" t="inlineStr"/>
-      <c r="AE29" t="inlineStr"/>
-      <c r="AF29" t="inlineStr"/>
-      <c r="AG29" t="inlineStr"/>
-      <c r="AH29" t="inlineStr"/>
-      <c r="AI29" t="inlineStr"/>
-      <c r="AJ29" t="inlineStr"/>
-      <c r="AK29" t="inlineStr"/>
-      <c r="AL29" t="inlineStr"/>
-      <c r="AM29" t="inlineStr"/>
+      <c r="AB32" t="inlineStr"/>
+      <c r="AC32" t="inlineStr"/>
+      <c r="AD32" t="inlineStr"/>
+      <c r="AE32" t="inlineStr"/>
+      <c r="AF32" t="inlineStr"/>
+      <c r="AG32" t="inlineStr"/>
+      <c r="AH32" t="inlineStr"/>
+      <c r="AI32" t="inlineStr"/>
+      <c r="AJ32" t="inlineStr"/>
+      <c r="AK32" t="inlineStr"/>
+      <c r="AL32" t="inlineStr"/>
+      <c r="AM32" t="inlineStr"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>

<commit_message>
Modified main.py and red.json - main.py > SO_Form     - added focusin/focusout events to the fg color     of the entry widgets     - changed the font size of the labels - main.py > SO_Update_Frame     - Fixed the grammical error - red.json     - updated the scrollableframe's scrollbar     hover color
</commit_message>
<xml_diff>
--- a/SO_Test.xlsx
+++ b/SO_Test.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:AM32"/>
+  <dimension ref="A1:AM33"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -4188,20 +4188,52 @@
       <c r="W30" t="inlineStr"/>
       <c r="X30" t="inlineStr">
         <is>
-          <t>NO</t>
-        </is>
-      </c>
-      <c r="Y30" t="inlineStr"/>
-      <c r="Z30" t="inlineStr"/>
+          <t>YES</t>
+        </is>
+      </c>
+      <c r="Y30" t="inlineStr">
+        <is>
+          <t>03/15/2024</t>
+        </is>
+      </c>
+      <c r="Z30" t="inlineStr">
+        <is>
+          <t>abake</t>
+        </is>
+      </c>
       <c r="AA30" t="n">
-        <v>0</v>
-      </c>
-      <c r="AB30" t="inlineStr"/>
-      <c r="AC30" t="inlineStr"/>
-      <c r="AD30" t="inlineStr"/>
-      <c r="AE30" t="inlineStr"/>
-      <c r="AF30" t="inlineStr"/>
-      <c r="AG30" t="inlineStr"/>
+        <v>2</v>
+      </c>
+      <c r="AB30" t="inlineStr">
+        <is>
+          <t>03/15/2024</t>
+        </is>
+      </c>
+      <c r="AC30" t="inlineStr">
+        <is>
+          <t>abake</t>
+        </is>
+      </c>
+      <c r="AD30" t="inlineStr">
+        <is>
+          <t>left vm</t>
+        </is>
+      </c>
+      <c r="AE30" t="inlineStr">
+        <is>
+          <t>picked up</t>
+        </is>
+      </c>
+      <c r="AF30" t="inlineStr">
+        <is>
+          <t>03/15/2024</t>
+        </is>
+      </c>
+      <c r="AG30" t="inlineStr">
+        <is>
+          <t>abake</t>
+        </is>
+      </c>
       <c r="AH30" t="inlineStr"/>
       <c r="AI30" t="inlineStr"/>
       <c r="AJ30" t="inlineStr"/>
@@ -4397,26 +4429,10 @@
           <t>PICKUP</t>
         </is>
       </c>
-      <c r="Q32" t="inlineStr">
-        <is>
-          <t>N/A</t>
-        </is>
-      </c>
-      <c r="R32" t="inlineStr">
-        <is>
-          <t>N/A</t>
-        </is>
-      </c>
-      <c r="S32" t="inlineStr">
-        <is>
-          <t>N/A</t>
-        </is>
-      </c>
-      <c r="T32" t="inlineStr">
-        <is>
-          <t>N/A</t>
-        </is>
-      </c>
+      <c r="Q32" t="inlineStr"/>
+      <c r="R32" t="inlineStr"/>
+      <c r="S32" t="inlineStr"/>
+      <c r="T32" t="inlineStr"/>
       <c r="U32" t="inlineStr">
         <is>
           <t>NO</t>
@@ -4447,6 +4463,117 @@
       <c r="AL32" t="inlineStr"/>
       <c r="AM32" t="inlineStr"/>
     </row>
+    <row r="33">
+      <c r="A33" t="inlineStr">
+        <is>
+          <t>03/15/2024</t>
+        </is>
+      </c>
+      <c r="B33" t="inlineStr">
+        <is>
+          <t>SO240315004</t>
+        </is>
+      </c>
+      <c r="C33" t="inlineStr">
+        <is>
+          <t>ab</t>
+        </is>
+      </c>
+      <c r="D33" t="inlineStr">
+        <is>
+          <t>somethingsimple6767@gmail.com</t>
+        </is>
+      </c>
+      <c r="E33" t="inlineStr">
+        <is>
+          <t>(915)799-4875</t>
+        </is>
+      </c>
+      <c r="F33" t="inlineStr">
+        <is>
+          <t>YES</t>
+        </is>
+      </c>
+      <c r="G33" t="inlineStr">
+        <is>
+          <t>YES</t>
+        </is>
+      </c>
+      <c r="H33" t="inlineStr">
+        <is>
+          <t>artist</t>
+        </is>
+      </c>
+      <c r="I33" t="inlineStr">
+        <is>
+          <t>title</t>
+        </is>
+      </c>
+      <c r="J33" t="n">
+        <v>8</v>
+      </c>
+      <c r="K33" t="n">
+        <v>15</v>
+      </c>
+      <c r="L33" t="inlineStr">
+        <is>
+          <t> </t>
+        </is>
+      </c>
+      <c r="M33" t="inlineStr">
+        <is>
+          <t>Discogs</t>
+        </is>
+      </c>
+      <c r="N33" t="inlineStr">
+        <is>
+          <t>DVD</t>
+        </is>
+      </c>
+      <c r="O33" t="inlineStr">
+        <is>
+          <t>abake</t>
+        </is>
+      </c>
+      <c r="P33" t="inlineStr">
+        <is>
+          <t>PICKUP</t>
+        </is>
+      </c>
+      <c r="Q33" t="inlineStr"/>
+      <c r="R33" t="inlineStr"/>
+      <c r="S33" t="inlineStr"/>
+      <c r="T33" t="inlineStr"/>
+      <c r="U33" t="inlineStr">
+        <is>
+          <t>NO</t>
+        </is>
+      </c>
+      <c r="V33" t="inlineStr"/>
+      <c r="W33" t="inlineStr"/>
+      <c r="X33" t="inlineStr">
+        <is>
+          <t>NO</t>
+        </is>
+      </c>
+      <c r="Y33" t="inlineStr"/>
+      <c r="Z33" t="inlineStr"/>
+      <c r="AA33" t="n">
+        <v>0</v>
+      </c>
+      <c r="AB33" t="inlineStr"/>
+      <c r="AC33" t="inlineStr"/>
+      <c r="AD33" t="inlineStr"/>
+      <c r="AE33" t="inlineStr"/>
+      <c r="AF33" t="inlineStr"/>
+      <c r="AG33" t="inlineStr"/>
+      <c r="AH33" t="inlineStr"/>
+      <c r="AI33" t="inlineStr"/>
+      <c r="AJ33" t="inlineStr"/>
+      <c r="AK33" t="inlineStr"/>
+      <c r="AL33" t="inlineStr"/>
+      <c r="AM33" t="inlineStr"/>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Modified main and json file - main     - adjusted the geomety and wdget positions     - configures a light/dark option - red.json     - configured the key-value pair for the light mode
</commit_message>
<xml_diff>
--- a/SO_Test.xlsx
+++ b/SO_Test.xlsx
@@ -682,7 +682,6 @@
       <c r="K2" t="n">
         <v>24</v>
       </c>
-      <c r="L2" t="inlineStr"/>
       <c r="M2" t="inlineStr">
         <is>
           <t>Vendors</t>
@@ -703,10 +702,6 @@
           <t>NO</t>
         </is>
       </c>
-      <c r="Q2" t="inlineStr"/>
-      <c r="R2" t="inlineStr"/>
-      <c r="S2" t="inlineStr"/>
-      <c r="T2" t="inlineStr"/>
       <c r="U2" t="inlineStr">
         <is>
           <t>YES</t>
@@ -770,53 +765,6 @@
           <t>abake</t>
         </is>
       </c>
-      <c r="AH2" t="inlineStr"/>
-      <c r="AI2" t="inlineStr"/>
-      <c r="AJ2" t="inlineStr"/>
-      <c r="AK2" t="inlineStr"/>
-      <c r="AL2" t="inlineStr"/>
-      <c r="AM2" t="inlineStr"/>
-    </row>
-    <row r="3">
-      <c r="A3" t="inlineStr"/>
-      <c r="B3" t="inlineStr"/>
-      <c r="C3" t="inlineStr"/>
-      <c r="D3" t="inlineStr"/>
-      <c r="E3" t="inlineStr"/>
-      <c r="F3" t="inlineStr"/>
-      <c r="G3" t="inlineStr"/>
-      <c r="H3" t="inlineStr"/>
-      <c r="I3" t="inlineStr"/>
-      <c r="J3" t="inlineStr"/>
-      <c r="K3" t="inlineStr"/>
-      <c r="L3" t="inlineStr"/>
-      <c r="M3" t="inlineStr"/>
-      <c r="N3" t="inlineStr"/>
-      <c r="O3" t="inlineStr"/>
-      <c r="P3" t="inlineStr"/>
-      <c r="Q3" t="inlineStr"/>
-      <c r="R3" t="inlineStr"/>
-      <c r="S3" t="inlineStr"/>
-      <c r="T3" t="inlineStr"/>
-      <c r="U3" t="inlineStr"/>
-      <c r="V3" t="inlineStr"/>
-      <c r="W3" t="inlineStr"/>
-      <c r="X3" t="inlineStr"/>
-      <c r="Y3" t="inlineStr"/>
-      <c r="Z3" t="inlineStr"/>
-      <c r="AA3" t="inlineStr"/>
-      <c r="AB3" t="inlineStr"/>
-      <c r="AC3" t="inlineStr"/>
-      <c r="AD3" t="inlineStr"/>
-      <c r="AE3" t="inlineStr"/>
-      <c r="AF3" t="inlineStr"/>
-      <c r="AG3" t="inlineStr"/>
-      <c r="AH3" t="inlineStr"/>
-      <c r="AI3" t="inlineStr"/>
-      <c r="AJ3" t="inlineStr"/>
-      <c r="AK3" t="inlineStr"/>
-      <c r="AL3" t="inlineStr"/>
-      <c r="AM3" t="inlineStr"/>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
@@ -870,7 +818,6 @@
       <c r="K4" t="n">
         <v>34</v>
       </c>
-      <c r="L4" t="inlineStr"/>
       <c r="M4" t="inlineStr">
         <is>
           <t>AMA</t>
@@ -891,10 +838,6 @@
           <t>NO</t>
         </is>
       </c>
-      <c r="Q4" t="inlineStr"/>
-      <c r="R4" t="inlineStr"/>
-      <c r="S4" t="inlineStr"/>
-      <c r="T4" t="inlineStr"/>
       <c r="U4" t="inlineStr">
         <is>
           <t>YES</t>
@@ -943,15 +886,6 @@
           <t>PICKED UP</t>
         </is>
       </c>
-      <c r="AE4" t="inlineStr"/>
-      <c r="AF4" t="inlineStr"/>
-      <c r="AG4" t="inlineStr"/>
-      <c r="AH4" t="inlineStr"/>
-      <c r="AI4" t="inlineStr"/>
-      <c r="AJ4" t="inlineStr"/>
-      <c r="AK4" t="inlineStr"/>
-      <c r="AL4" t="inlineStr"/>
-      <c r="AM4" t="inlineStr"/>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
@@ -1005,7 +939,6 @@
       <c r="K5" t="n">
         <v>49.99</v>
       </c>
-      <c r="L5" t="inlineStr"/>
       <c r="M5" t="inlineStr">
         <is>
           <t>AMS</t>
@@ -1049,71 +982,14 @@
           <t>NO</t>
         </is>
       </c>
-      <c r="V5" t="inlineStr"/>
-      <c r="W5" t="inlineStr"/>
       <c r="X5" t="inlineStr">
         <is>
           <t>NO</t>
         </is>
       </c>
-      <c r="Y5" t="inlineStr"/>
-      <c r="Z5" t="inlineStr"/>
       <c r="AA5" t="n">
         <v>0</v>
       </c>
-      <c r="AB5" t="inlineStr"/>
-      <c r="AC5" t="inlineStr"/>
-      <c r="AD5" t="inlineStr"/>
-      <c r="AE5" t="inlineStr"/>
-      <c r="AF5" t="inlineStr"/>
-      <c r="AG5" t="inlineStr"/>
-      <c r="AH5" t="inlineStr"/>
-      <c r="AI5" t="inlineStr"/>
-      <c r="AJ5" t="inlineStr"/>
-      <c r="AK5" t="inlineStr"/>
-      <c r="AL5" t="inlineStr"/>
-      <c r="AM5" t="inlineStr"/>
-    </row>
-    <row r="6">
-      <c r="A6" t="inlineStr"/>
-      <c r="B6" t="inlineStr"/>
-      <c r="C6" t="inlineStr"/>
-      <c r="D6" t="inlineStr"/>
-      <c r="E6" t="inlineStr"/>
-      <c r="F6" t="inlineStr"/>
-      <c r="G6" t="inlineStr"/>
-      <c r="H6" t="inlineStr"/>
-      <c r="I6" t="inlineStr"/>
-      <c r="J6" t="inlineStr"/>
-      <c r="K6" t="inlineStr"/>
-      <c r="L6" t="inlineStr"/>
-      <c r="M6" t="inlineStr"/>
-      <c r="N6" t="inlineStr"/>
-      <c r="O6" t="inlineStr"/>
-      <c r="P6" t="inlineStr"/>
-      <c r="Q6" t="inlineStr"/>
-      <c r="R6" t="inlineStr"/>
-      <c r="S6" t="inlineStr"/>
-      <c r="T6" t="inlineStr"/>
-      <c r="U6" t="inlineStr"/>
-      <c r="V6" t="inlineStr"/>
-      <c r="W6" t="inlineStr"/>
-      <c r="X6" t="inlineStr"/>
-      <c r="Y6" t="inlineStr"/>
-      <c r="Z6" t="inlineStr"/>
-      <c r="AA6" t="inlineStr"/>
-      <c r="AB6" t="inlineStr"/>
-      <c r="AC6" t="inlineStr"/>
-      <c r="AD6" t="inlineStr"/>
-      <c r="AE6" t="inlineStr"/>
-      <c r="AF6" t="inlineStr"/>
-      <c r="AG6" t="inlineStr"/>
-      <c r="AH6" t="inlineStr"/>
-      <c r="AI6" t="inlineStr"/>
-      <c r="AJ6" t="inlineStr"/>
-      <c r="AK6" t="inlineStr"/>
-      <c r="AL6" t="inlineStr"/>
-      <c r="AM6" t="inlineStr"/>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
@@ -1167,7 +1043,6 @@
       <c r="K7" t="n">
         <v>50.2</v>
       </c>
-      <c r="L7" t="inlineStr"/>
       <c r="M7" t="inlineStr">
         <is>
           <t>AMS</t>
@@ -1188,10 +1063,6 @@
           <t>NO</t>
         </is>
       </c>
-      <c r="Q7" t="inlineStr"/>
-      <c r="R7" t="inlineStr"/>
-      <c r="S7" t="inlineStr"/>
-      <c r="T7" t="inlineStr"/>
       <c r="U7" t="inlineStr">
         <is>
           <t>YES</t>
@@ -1240,56 +1111,6 @@
           <t>VM</t>
         </is>
       </c>
-      <c r="AE7" t="inlineStr"/>
-      <c r="AF7" t="inlineStr"/>
-      <c r="AG7" t="inlineStr"/>
-      <c r="AH7" t="inlineStr"/>
-      <c r="AI7" t="inlineStr"/>
-      <c r="AJ7" t="inlineStr"/>
-      <c r="AK7" t="inlineStr"/>
-      <c r="AL7" t="inlineStr"/>
-      <c r="AM7" t="inlineStr"/>
-    </row>
-    <row r="8">
-      <c r="A8" t="inlineStr"/>
-      <c r="B8" t="inlineStr"/>
-      <c r="C8" t="inlineStr"/>
-      <c r="D8" t="inlineStr"/>
-      <c r="E8" t="inlineStr"/>
-      <c r="F8" t="inlineStr"/>
-      <c r="G8" t="inlineStr"/>
-      <c r="H8" t="inlineStr"/>
-      <c r="I8" t="inlineStr"/>
-      <c r="J8" t="inlineStr"/>
-      <c r="K8" t="inlineStr"/>
-      <c r="L8" t="inlineStr"/>
-      <c r="M8" t="inlineStr"/>
-      <c r="N8" t="inlineStr"/>
-      <c r="O8" t="inlineStr"/>
-      <c r="P8" t="inlineStr"/>
-      <c r="Q8" t="inlineStr"/>
-      <c r="R8" t="inlineStr"/>
-      <c r="S8" t="inlineStr"/>
-      <c r="T8" t="inlineStr"/>
-      <c r="U8" t="inlineStr"/>
-      <c r="V8" t="inlineStr"/>
-      <c r="W8" t="inlineStr"/>
-      <c r="X8" t="inlineStr"/>
-      <c r="Y8" t="inlineStr"/>
-      <c r="Z8" t="inlineStr"/>
-      <c r="AA8" t="inlineStr"/>
-      <c r="AB8" t="inlineStr"/>
-      <c r="AC8" t="inlineStr"/>
-      <c r="AD8" t="inlineStr"/>
-      <c r="AE8" t="inlineStr"/>
-      <c r="AF8" t="inlineStr"/>
-      <c r="AG8" t="inlineStr"/>
-      <c r="AH8" t="inlineStr"/>
-      <c r="AI8" t="inlineStr"/>
-      <c r="AJ8" t="inlineStr"/>
-      <c r="AK8" t="inlineStr"/>
-      <c r="AL8" t="inlineStr"/>
-      <c r="AM8" t="inlineStr"/>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
@@ -1343,7 +1164,6 @@
       <c r="K9" t="n">
         <v>58.63</v>
       </c>
-      <c r="L9" t="inlineStr"/>
       <c r="M9" t="inlineStr">
         <is>
           <t>AMS</t>
@@ -1354,16 +1174,11 @@
           <t>LP</t>
         </is>
       </c>
-      <c r="O9" t="inlineStr"/>
       <c r="P9" t="inlineStr">
         <is>
           <t>NO</t>
         </is>
       </c>
-      <c r="Q9" t="inlineStr"/>
-      <c r="R9" t="inlineStr"/>
-      <c r="S9" t="inlineStr"/>
-      <c r="T9" t="inlineStr"/>
       <c r="U9" t="inlineStr">
         <is>
           <t>YES</t>
@@ -1412,56 +1227,6 @@
           <t>picked up</t>
         </is>
       </c>
-      <c r="AE9" t="inlineStr"/>
-      <c r="AF9" t="inlineStr"/>
-      <c r="AG9" t="inlineStr"/>
-      <c r="AH9" t="inlineStr"/>
-      <c r="AI9" t="inlineStr"/>
-      <c r="AJ9" t="inlineStr"/>
-      <c r="AK9" t="inlineStr"/>
-      <c r="AL9" t="inlineStr"/>
-      <c r="AM9" t="inlineStr"/>
-    </row>
-    <row r="10">
-      <c r="A10" t="inlineStr"/>
-      <c r="B10" t="inlineStr"/>
-      <c r="C10" t="inlineStr"/>
-      <c r="D10" t="inlineStr"/>
-      <c r="E10" t="inlineStr"/>
-      <c r="F10" t="inlineStr"/>
-      <c r="G10" t="inlineStr"/>
-      <c r="H10" t="inlineStr"/>
-      <c r="I10" t="inlineStr"/>
-      <c r="J10" t="inlineStr"/>
-      <c r="K10" t="inlineStr"/>
-      <c r="L10" t="inlineStr"/>
-      <c r="M10" t="inlineStr"/>
-      <c r="N10" t="inlineStr"/>
-      <c r="O10" t="inlineStr"/>
-      <c r="P10" t="inlineStr"/>
-      <c r="Q10" t="inlineStr"/>
-      <c r="R10" t="inlineStr"/>
-      <c r="S10" t="inlineStr"/>
-      <c r="T10" t="inlineStr"/>
-      <c r="U10" t="inlineStr"/>
-      <c r="V10" t="inlineStr"/>
-      <c r="W10" t="inlineStr"/>
-      <c r="X10" t="inlineStr"/>
-      <c r="Y10" t="inlineStr"/>
-      <c r="Z10" t="inlineStr"/>
-      <c r="AA10" t="inlineStr"/>
-      <c r="AB10" t="inlineStr"/>
-      <c r="AC10" t="inlineStr"/>
-      <c r="AD10" t="inlineStr"/>
-      <c r="AE10" t="inlineStr"/>
-      <c r="AF10" t="inlineStr"/>
-      <c r="AG10" t="inlineStr"/>
-      <c r="AH10" t="inlineStr"/>
-      <c r="AI10" t="inlineStr"/>
-      <c r="AJ10" t="inlineStr"/>
-      <c r="AK10" t="inlineStr"/>
-      <c r="AL10" t="inlineStr"/>
-      <c r="AM10" t="inlineStr"/>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr">
@@ -1515,7 +1280,6 @@
       <c r="K11" t="n">
         <v>199</v>
       </c>
-      <c r="L11" t="inlineStr"/>
       <c r="M11" t="inlineStr">
         <is>
           <t>AMA</t>
@@ -1536,39 +1300,19 @@
           <t>NO</t>
         </is>
       </c>
-      <c r="Q11" t="inlineStr"/>
-      <c r="R11" t="inlineStr"/>
-      <c r="S11" t="inlineStr"/>
-      <c r="T11" t="inlineStr"/>
       <c r="U11" t="inlineStr">
         <is>
           <t>NO</t>
         </is>
       </c>
-      <c r="V11" t="inlineStr"/>
-      <c r="W11" t="inlineStr"/>
       <c r="X11" t="inlineStr">
         <is>
           <t>NO</t>
         </is>
       </c>
-      <c r="Y11" t="inlineStr"/>
-      <c r="Z11" t="inlineStr"/>
       <c r="AA11" t="n">
         <v>0</v>
       </c>
-      <c r="AB11" t="inlineStr"/>
-      <c r="AC11" t="inlineStr"/>
-      <c r="AD11" t="inlineStr"/>
-      <c r="AE11" t="inlineStr"/>
-      <c r="AF11" t="inlineStr"/>
-      <c r="AG11" t="inlineStr"/>
-      <c r="AH11" t="inlineStr"/>
-      <c r="AI11" t="inlineStr"/>
-      <c r="AJ11" t="inlineStr"/>
-      <c r="AK11" t="inlineStr"/>
-      <c r="AL11" t="inlineStr"/>
-      <c r="AM11" t="inlineStr"/>
     </row>
     <row r="12">
       <c r="A12" t="inlineStr">
@@ -1622,7 +1366,6 @@
       <c r="K12" t="n">
         <v>15</v>
       </c>
-      <c r="L12" t="inlineStr"/>
       <c r="M12" t="inlineStr">
         <is>
           <t>AMA</t>
@@ -1643,10 +1386,6 @@
           <t>NO</t>
         </is>
       </c>
-      <c r="Q12" t="inlineStr"/>
-      <c r="R12" t="inlineStr"/>
-      <c r="S12" t="inlineStr"/>
-      <c r="T12" t="inlineStr"/>
       <c r="U12" t="inlineStr">
         <is>
           <t>YES</t>
@@ -1680,59 +1419,6 @@
       <c r="AA12" t="n">
         <v>0</v>
       </c>
-      <c r="AB12" t="inlineStr"/>
-      <c r="AC12" t="inlineStr"/>
-      <c r="AD12" t="inlineStr"/>
-      <c r="AE12" t="inlineStr"/>
-      <c r="AF12" t="inlineStr"/>
-      <c r="AG12" t="inlineStr"/>
-      <c r="AH12" t="inlineStr"/>
-      <c r="AI12" t="inlineStr"/>
-      <c r="AJ12" t="inlineStr"/>
-      <c r="AK12" t="inlineStr"/>
-      <c r="AL12" t="inlineStr"/>
-      <c r="AM12" t="inlineStr"/>
-    </row>
-    <row r="13">
-      <c r="A13" t="inlineStr"/>
-      <c r="B13" t="inlineStr"/>
-      <c r="C13" t="inlineStr"/>
-      <c r="D13" t="inlineStr"/>
-      <c r="E13" t="inlineStr"/>
-      <c r="F13" t="inlineStr"/>
-      <c r="G13" t="inlineStr"/>
-      <c r="H13" t="inlineStr"/>
-      <c r="I13" t="inlineStr"/>
-      <c r="J13" t="inlineStr"/>
-      <c r="K13" t="inlineStr"/>
-      <c r="L13" t="inlineStr"/>
-      <c r="M13" t="inlineStr"/>
-      <c r="N13" t="inlineStr"/>
-      <c r="O13" t="inlineStr"/>
-      <c r="P13" t="inlineStr"/>
-      <c r="Q13" t="inlineStr"/>
-      <c r="R13" t="inlineStr"/>
-      <c r="S13" t="inlineStr"/>
-      <c r="T13" t="inlineStr"/>
-      <c r="U13" t="inlineStr"/>
-      <c r="V13" t="inlineStr"/>
-      <c r="W13" t="inlineStr"/>
-      <c r="X13" t="inlineStr"/>
-      <c r="Y13" t="inlineStr"/>
-      <c r="Z13" t="inlineStr"/>
-      <c r="AA13" t="inlineStr"/>
-      <c r="AB13" t="inlineStr"/>
-      <c r="AC13" t="inlineStr"/>
-      <c r="AD13" t="inlineStr"/>
-      <c r="AE13" t="inlineStr"/>
-      <c r="AF13" t="inlineStr"/>
-      <c r="AG13" t="inlineStr"/>
-      <c r="AH13" t="inlineStr"/>
-      <c r="AI13" t="inlineStr"/>
-      <c r="AJ13" t="inlineStr"/>
-      <c r="AK13" t="inlineStr"/>
-      <c r="AL13" t="inlineStr"/>
-      <c r="AM13" t="inlineStr"/>
     </row>
     <row r="14">
       <c r="A14" t="inlineStr">
@@ -1786,7 +1472,6 @@
       <c r="K14" t="n">
         <v>20</v>
       </c>
-      <c r="L14" t="inlineStr"/>
       <c r="M14" t="inlineStr">
         <is>
           <t>AMS</t>
@@ -1807,10 +1492,6 @@
           <t>PICKUP</t>
         </is>
       </c>
-      <c r="Q14" t="inlineStr"/>
-      <c r="R14" t="inlineStr"/>
-      <c r="S14" t="inlineStr"/>
-      <c r="T14" t="inlineStr"/>
       <c r="U14" t="inlineStr">
         <is>
           <t>YES</t>
@@ -1859,15 +1540,6 @@
           <t>VM</t>
         </is>
       </c>
-      <c r="AE14" t="inlineStr"/>
-      <c r="AF14" t="inlineStr"/>
-      <c r="AG14" t="inlineStr"/>
-      <c r="AH14" t="inlineStr"/>
-      <c r="AI14" t="inlineStr"/>
-      <c r="AJ14" t="inlineStr"/>
-      <c r="AK14" t="inlineStr"/>
-      <c r="AL14" t="inlineStr"/>
-      <c r="AM14" t="inlineStr"/>
     </row>
     <row r="15">
       <c r="A15" t="inlineStr">
@@ -1921,7 +1593,6 @@
       <c r="K15" t="n">
         <v>87</v>
       </c>
-      <c r="L15" t="inlineStr"/>
       <c r="M15" t="inlineStr">
         <is>
           <t>AMA</t>
@@ -1942,10 +1613,6 @@
           <t>PICKUP</t>
         </is>
       </c>
-      <c r="Q15" t="inlineStr"/>
-      <c r="R15" t="inlineStr"/>
-      <c r="S15" t="inlineStr"/>
-      <c r="T15" t="inlineStr"/>
       <c r="U15" t="inlineStr">
         <is>
           <t>YES</t>
@@ -1994,15 +1661,6 @@
           <t>VM</t>
         </is>
       </c>
-      <c r="AE15" t="inlineStr"/>
-      <c r="AF15" t="inlineStr"/>
-      <c r="AG15" t="inlineStr"/>
-      <c r="AH15" t="inlineStr"/>
-      <c r="AI15" t="inlineStr"/>
-      <c r="AJ15" t="inlineStr"/>
-      <c r="AK15" t="inlineStr"/>
-      <c r="AL15" t="inlineStr"/>
-      <c r="AM15" t="inlineStr"/>
     </row>
     <row r="16">
       <c r="A16" t="inlineStr">
@@ -2056,7 +1714,6 @@
       <c r="K16" t="n">
         <v>89.98999999999999</v>
       </c>
-      <c r="L16" t="inlineStr"/>
       <c r="M16" t="inlineStr">
         <is>
           <t>AMA</t>
@@ -2077,10 +1734,6 @@
           <t>PICKUP</t>
         </is>
       </c>
-      <c r="Q16" t="inlineStr"/>
-      <c r="R16" t="inlineStr"/>
-      <c r="S16" t="inlineStr"/>
-      <c r="T16" t="inlineStr"/>
       <c r="U16" t="inlineStr">
         <is>
           <t>YES</t>
@@ -2129,56 +1782,6 @@
           <t>PICKED UP</t>
         </is>
       </c>
-      <c r="AE16" t="inlineStr"/>
-      <c r="AF16" t="inlineStr"/>
-      <c r="AG16" t="inlineStr"/>
-      <c r="AH16" t="inlineStr"/>
-      <c r="AI16" t="inlineStr"/>
-      <c r="AJ16" t="inlineStr"/>
-      <c r="AK16" t="inlineStr"/>
-      <c r="AL16" t="inlineStr"/>
-      <c r="AM16" t="inlineStr"/>
-    </row>
-    <row r="17">
-      <c r="A17" t="inlineStr"/>
-      <c r="B17" t="inlineStr"/>
-      <c r="C17" t="inlineStr"/>
-      <c r="D17" t="inlineStr"/>
-      <c r="E17" t="inlineStr"/>
-      <c r="F17" t="inlineStr"/>
-      <c r="G17" t="inlineStr"/>
-      <c r="H17" t="inlineStr"/>
-      <c r="I17" t="inlineStr"/>
-      <c r="J17" t="inlineStr"/>
-      <c r="K17" t="inlineStr"/>
-      <c r="L17" t="inlineStr"/>
-      <c r="M17" t="inlineStr"/>
-      <c r="N17" t="inlineStr"/>
-      <c r="O17" t="inlineStr"/>
-      <c r="P17" t="inlineStr"/>
-      <c r="Q17" t="inlineStr"/>
-      <c r="R17" t="inlineStr"/>
-      <c r="S17" t="inlineStr"/>
-      <c r="T17" t="inlineStr"/>
-      <c r="U17" t="inlineStr"/>
-      <c r="V17" t="inlineStr"/>
-      <c r="W17" t="inlineStr"/>
-      <c r="X17" t="inlineStr"/>
-      <c r="Y17" t="inlineStr"/>
-      <c r="Z17" t="inlineStr"/>
-      <c r="AA17" t="inlineStr"/>
-      <c r="AB17" t="inlineStr"/>
-      <c r="AC17" t="inlineStr"/>
-      <c r="AD17" t="inlineStr"/>
-      <c r="AE17" t="inlineStr"/>
-      <c r="AF17" t="inlineStr"/>
-      <c r="AG17" t="inlineStr"/>
-      <c r="AH17" t="inlineStr"/>
-      <c r="AI17" t="inlineStr"/>
-      <c r="AJ17" t="inlineStr"/>
-      <c r="AK17" t="inlineStr"/>
-      <c r="AL17" t="inlineStr"/>
-      <c r="AM17" t="inlineStr"/>
     </row>
     <row r="18">
       <c r="A18" t="inlineStr">
@@ -2232,7 +1835,6 @@
       <c r="K18" t="n">
         <v>15</v>
       </c>
-      <c r="L18" t="inlineStr"/>
       <c r="M18" t="inlineStr">
         <is>
           <t>AMS</t>
@@ -2253,10 +1855,6 @@
           <t>PICKUP</t>
         </is>
       </c>
-      <c r="Q18" t="inlineStr"/>
-      <c r="R18" t="inlineStr"/>
-      <c r="S18" t="inlineStr"/>
-      <c r="T18" t="inlineStr"/>
       <c r="U18" t="inlineStr">
         <is>
           <t>YES</t>
@@ -2320,12 +1918,6 @@
           <t>abake</t>
         </is>
       </c>
-      <c r="AH18" t="inlineStr"/>
-      <c r="AI18" t="inlineStr"/>
-      <c r="AJ18" t="inlineStr"/>
-      <c r="AK18" t="inlineStr"/>
-      <c r="AL18" t="inlineStr"/>
-      <c r="AM18" t="inlineStr"/>
     </row>
     <row r="19">
       <c r="A19" t="inlineStr">
@@ -2379,7 +1971,6 @@
       <c r="K19" t="n">
         <v>50.99</v>
       </c>
-      <c r="L19" t="inlineStr"/>
       <c r="M19" t="inlineStr">
         <is>
           <t>AMS</t>
@@ -2483,12 +2074,6 @@
           <t>abake</t>
         </is>
       </c>
-      <c r="AH19" t="inlineStr"/>
-      <c r="AI19" t="inlineStr"/>
-      <c r="AJ19" t="inlineStr"/>
-      <c r="AK19" t="inlineStr"/>
-      <c r="AL19" t="inlineStr"/>
-      <c r="AM19" t="inlineStr"/>
     </row>
     <row r="20">
       <c r="A20" t="inlineStr">
@@ -2542,7 +2127,6 @@
       <c r="K20" t="n">
         <v>90</v>
       </c>
-      <c r="L20" t="inlineStr"/>
       <c r="M20" t="inlineStr">
         <is>
           <t>AMS</t>
@@ -2563,10 +2147,6 @@
           <t>PICKUP</t>
         </is>
       </c>
-      <c r="Q20" t="inlineStr"/>
-      <c r="R20" t="inlineStr"/>
-      <c r="S20" t="inlineStr"/>
-      <c r="T20" t="inlineStr"/>
       <c r="U20" t="inlineStr">
         <is>
           <t>YES</t>
@@ -2713,7 +2293,6 @@
       <c r="K21" t="n">
         <v>822</v>
       </c>
-      <c r="L21" t="inlineStr"/>
       <c r="M21" t="inlineStr">
         <is>
           <t>AEC</t>
@@ -2734,10 +2313,6 @@
           <t>PICKUP</t>
         </is>
       </c>
-      <c r="Q21" t="inlineStr"/>
-      <c r="R21" t="inlineStr"/>
-      <c r="S21" t="inlineStr"/>
-      <c r="T21" t="inlineStr"/>
       <c r="U21" t="inlineStr">
         <is>
           <t>YES</t>
@@ -2758,23 +2333,9 @@
           <t>NO</t>
         </is>
       </c>
-      <c r="Y21" t="inlineStr"/>
-      <c r="Z21" t="inlineStr"/>
       <c r="AA21" t="n">
         <v>0</v>
       </c>
-      <c r="AB21" t="inlineStr"/>
-      <c r="AC21" t="inlineStr"/>
-      <c r="AD21" t="inlineStr"/>
-      <c r="AE21" t="inlineStr"/>
-      <c r="AF21" t="inlineStr"/>
-      <c r="AG21" t="inlineStr"/>
-      <c r="AH21" t="inlineStr"/>
-      <c r="AI21" t="inlineStr"/>
-      <c r="AJ21" t="inlineStr"/>
-      <c r="AK21" t="inlineStr"/>
-      <c r="AL21" t="inlineStr"/>
-      <c r="AM21" t="inlineStr"/>
     </row>
     <row r="22">
       <c r="A22" t="inlineStr">
@@ -2927,15 +2488,6 @@
           <t> </t>
         </is>
       </c>
-      <c r="AE22" t="inlineStr"/>
-      <c r="AF22" t="inlineStr"/>
-      <c r="AG22" t="inlineStr"/>
-      <c r="AH22" t="inlineStr"/>
-      <c r="AI22" t="inlineStr"/>
-      <c r="AJ22" t="inlineStr"/>
-      <c r="AK22" t="inlineStr"/>
-      <c r="AL22" t="inlineStr"/>
-      <c r="AM22" t="inlineStr"/>
     </row>
     <row r="23">
       <c r="A23" t="inlineStr">
@@ -3014,10 +2566,6 @@
           <t>PICKUP</t>
         </is>
       </c>
-      <c r="Q23" t="inlineStr"/>
-      <c r="R23" t="inlineStr"/>
-      <c r="S23" t="inlineStr"/>
-      <c r="T23" t="inlineStr"/>
       <c r="U23" t="inlineStr">
         <is>
           <t>YES</t>
@@ -3051,18 +2599,6 @@
       <c r="AA23" t="n">
         <v>0</v>
       </c>
-      <c r="AB23" t="inlineStr"/>
-      <c r="AC23" t="inlineStr"/>
-      <c r="AD23" t="inlineStr"/>
-      <c r="AE23" t="inlineStr"/>
-      <c r="AF23" t="inlineStr"/>
-      <c r="AG23" t="inlineStr"/>
-      <c r="AH23" t="inlineStr"/>
-      <c r="AI23" t="inlineStr"/>
-      <c r="AJ23" t="inlineStr"/>
-      <c r="AK23" t="inlineStr"/>
-      <c r="AL23" t="inlineStr"/>
-      <c r="AM23" t="inlineStr"/>
     </row>
     <row r="24">
       <c r="A24" t="inlineStr">
@@ -3141,10 +2677,6 @@
           <t>PICKUP</t>
         </is>
       </c>
-      <c r="Q24" t="inlineStr"/>
-      <c r="R24" t="inlineStr"/>
-      <c r="S24" t="inlineStr"/>
-      <c r="T24" t="inlineStr"/>
       <c r="U24" t="inlineStr">
         <is>
           <t>YES</t>
@@ -3223,9 +2755,6 @@
           <t>abake</t>
         </is>
       </c>
-      <c r="AK24" t="inlineStr"/>
-      <c r="AL24" t="inlineStr"/>
-      <c r="AM24" t="inlineStr"/>
     </row>
     <row r="25">
       <c r="A25" t="inlineStr">
@@ -3304,10 +2833,6 @@
           <t>PICKUP</t>
         </is>
       </c>
-      <c r="Q25" t="inlineStr"/>
-      <c r="R25" t="inlineStr"/>
-      <c r="S25" t="inlineStr"/>
-      <c r="T25" t="inlineStr"/>
       <c r="U25" t="inlineStr">
         <is>
           <t>YES</t>
@@ -3386,9 +2911,6 @@
           <t>abake</t>
         </is>
       </c>
-      <c r="AK25" t="inlineStr"/>
-      <c r="AL25" t="inlineStr"/>
-      <c r="AM25" t="inlineStr"/>
     </row>
     <row r="26">
       <c r="A26" t="inlineStr">
@@ -3467,10 +2989,6 @@
           <t>PICKUP</t>
         </is>
       </c>
-      <c r="Q26" t="inlineStr"/>
-      <c r="R26" t="inlineStr"/>
-      <c r="S26" t="inlineStr"/>
-      <c r="T26" t="inlineStr"/>
       <c r="U26" t="inlineStr">
         <is>
           <t>YES</t>
@@ -3534,12 +3052,6 @@
           <t>abake</t>
         </is>
       </c>
-      <c r="AH26" t="inlineStr"/>
-      <c r="AI26" t="inlineStr"/>
-      <c r="AJ26" t="inlineStr"/>
-      <c r="AK26" t="inlineStr"/>
-      <c r="AL26" t="inlineStr"/>
-      <c r="AM26" t="inlineStr"/>
     </row>
     <row r="27">
       <c r="A27" t="inlineStr">
@@ -3618,10 +3130,6 @@
           <t>PICKUP</t>
         </is>
       </c>
-      <c r="Q27" t="inlineStr"/>
-      <c r="R27" t="inlineStr"/>
-      <c r="S27" t="inlineStr"/>
-      <c r="T27" t="inlineStr"/>
       <c r="U27" t="inlineStr">
         <is>
           <t>YES</t>
@@ -3700,9 +3208,6 @@
           <t>abake</t>
         </is>
       </c>
-      <c r="AK27" t="inlineStr"/>
-      <c r="AL27" t="inlineStr"/>
-      <c r="AM27" t="inlineStr"/>
     </row>
     <row r="28">
       <c r="A28" t="inlineStr">
@@ -4175,17 +3680,11 @@
           <t>PICKUP</t>
         </is>
       </c>
-      <c r="Q30" t="inlineStr"/>
-      <c r="R30" t="inlineStr"/>
-      <c r="S30" t="inlineStr"/>
-      <c r="T30" t="inlineStr"/>
       <c r="U30" t="inlineStr">
         <is>
           <t>NO</t>
         </is>
       </c>
-      <c r="V30" t="inlineStr"/>
-      <c r="W30" t="inlineStr"/>
       <c r="X30" t="inlineStr">
         <is>
           <t>YES</t>
@@ -4234,12 +3733,6 @@
           <t>abake</t>
         </is>
       </c>
-      <c r="AH30" t="inlineStr"/>
-      <c r="AI30" t="inlineStr"/>
-      <c r="AJ30" t="inlineStr"/>
-      <c r="AK30" t="inlineStr"/>
-      <c r="AL30" t="inlineStr"/>
-      <c r="AM30" t="inlineStr"/>
     </row>
     <row r="31">
       <c r="A31" t="inlineStr">
@@ -4318,39 +3811,54 @@
           <t>PICKUP</t>
         </is>
       </c>
-      <c r="Q31" t="inlineStr"/>
-      <c r="R31" t="inlineStr"/>
-      <c r="S31" t="inlineStr"/>
-      <c r="T31" t="inlineStr"/>
       <c r="U31" t="inlineStr">
         <is>
-          <t>NO</t>
-        </is>
-      </c>
-      <c r="V31" t="inlineStr"/>
-      <c r="W31" t="inlineStr"/>
+          <t>YES</t>
+        </is>
+      </c>
+      <c r="V31" t="inlineStr">
+        <is>
+          <t>03/18/2024</t>
+        </is>
+      </c>
+      <c r="W31" t="inlineStr">
+        <is>
+          <t>abake</t>
+        </is>
+      </c>
       <c r="X31" t="inlineStr">
         <is>
-          <t>NO</t>
-        </is>
-      </c>
-      <c r="Y31" t="inlineStr"/>
-      <c r="Z31" t="inlineStr"/>
+          <t>YES</t>
+        </is>
+      </c>
+      <c r="Y31" t="inlineStr">
+        <is>
+          <t>03/18/2024</t>
+        </is>
+      </c>
+      <c r="Z31" t="inlineStr">
+        <is>
+          <t>abake</t>
+        </is>
+      </c>
       <c r="AA31" t="n">
-        <v>0</v>
-      </c>
-      <c r="AB31" t="inlineStr"/>
-      <c r="AC31" t="inlineStr"/>
-      <c r="AD31" t="inlineStr"/>
-      <c r="AE31" t="inlineStr"/>
-      <c r="AF31" t="inlineStr"/>
-      <c r="AG31" t="inlineStr"/>
-      <c r="AH31" t="inlineStr"/>
-      <c r="AI31" t="inlineStr"/>
-      <c r="AJ31" t="inlineStr"/>
-      <c r="AK31" t="inlineStr"/>
-      <c r="AL31" t="inlineStr"/>
-      <c r="AM31" t="inlineStr"/>
+        <v>1</v>
+      </c>
+      <c r="AB31" t="inlineStr">
+        <is>
+          <t>03/18/2024</t>
+        </is>
+      </c>
+      <c r="AC31" t="inlineStr">
+        <is>
+          <t>abake</t>
+        </is>
+      </c>
+      <c r="AD31" t="inlineStr">
+        <is>
+          <t>left vm</t>
+        </is>
+      </c>
     </row>
     <row r="32">
       <c r="A32" t="inlineStr">
@@ -4429,91 +3937,75 @@
           <t>PICKUP</t>
         </is>
       </c>
-      <c r="Q32" t="inlineStr"/>
-      <c r="R32" t="inlineStr"/>
-      <c r="S32" t="inlineStr"/>
-      <c r="T32" t="inlineStr"/>
       <c r="U32" t="inlineStr">
         <is>
           <t>NO</t>
         </is>
       </c>
-      <c r="V32" t="inlineStr"/>
-      <c r="W32" t="inlineStr"/>
       <c r="X32" t="inlineStr">
         <is>
           <t>NO</t>
         </is>
       </c>
-      <c r="Y32" t="inlineStr"/>
-      <c r="Z32" t="inlineStr"/>
       <c r="AA32" t="n">
         <v>0</v>
       </c>
-      <c r="AB32" t="inlineStr"/>
-      <c r="AC32" t="inlineStr"/>
-      <c r="AD32" t="inlineStr"/>
-      <c r="AE32" t="inlineStr"/>
-      <c r="AF32" t="inlineStr"/>
-      <c r="AG32" t="inlineStr"/>
-      <c r="AH32" t="inlineStr"/>
-      <c r="AI32" t="inlineStr"/>
-      <c r="AJ32" t="inlineStr"/>
-      <c r="AK32" t="inlineStr"/>
-      <c r="AL32" t="inlineStr"/>
-      <c r="AM32" t="inlineStr"/>
     </row>
     <row r="33">
       <c r="A33" t="inlineStr">
         <is>
-          <t>03/15/2024</t>
+          <t> </t>
         </is>
       </c>
       <c r="B33" t="inlineStr">
         <is>
-          <t>SO240315004</t>
+          <t> </t>
         </is>
       </c>
       <c r="C33" t="inlineStr">
         <is>
-          <t>ab</t>
+          <t> </t>
         </is>
       </c>
       <c r="D33" t="inlineStr">
         <is>
-          <t>somethingsimple6767@gmail.com</t>
+          <t> </t>
         </is>
       </c>
       <c r="E33" t="inlineStr">
         <is>
-          <t>(915)799-4875</t>
+          <t> </t>
         </is>
       </c>
       <c r="F33" t="inlineStr">
         <is>
-          <t>YES</t>
+          <t> </t>
         </is>
       </c>
       <c r="G33" t="inlineStr">
         <is>
-          <t>YES</t>
+          <t> </t>
         </is>
       </c>
       <c r="H33" t="inlineStr">
         <is>
-          <t>artist</t>
+          <t> </t>
         </is>
       </c>
       <c r="I33" t="inlineStr">
         <is>
-          <t>title</t>
-        </is>
-      </c>
-      <c r="J33" t="n">
-        <v>8</v>
-      </c>
-      <c r="K33" t="n">
-        <v>15</v>
+          <t> </t>
+        </is>
+      </c>
+      <c r="J33" t="inlineStr">
+        <is>
+          <t> </t>
+        </is>
+      </c>
+      <c r="K33" t="inlineStr">
+        <is>
+          <t> </t>
+        </is>
       </c>
       <c r="L33" t="inlineStr">
         <is>
@@ -4522,57 +4014,139 @@
       </c>
       <c r="M33" t="inlineStr">
         <is>
-          <t>Discogs</t>
+          <t> </t>
         </is>
       </c>
       <c r="N33" t="inlineStr">
         <is>
-          <t>DVD</t>
+          <t> </t>
         </is>
       </c>
       <c r="O33" t="inlineStr">
         <is>
-          <t>abake</t>
+          <t> </t>
         </is>
       </c>
       <c r="P33" t="inlineStr">
         <is>
-          <t>PICKUP</t>
-        </is>
-      </c>
-      <c r="Q33" t="inlineStr"/>
-      <c r="R33" t="inlineStr"/>
-      <c r="S33" t="inlineStr"/>
-      <c r="T33" t="inlineStr"/>
+          <t> </t>
+        </is>
+      </c>
+      <c r="Q33" t="inlineStr">
+        <is>
+          <t> </t>
+        </is>
+      </c>
+      <c r="R33" t="inlineStr">
+        <is>
+          <t> </t>
+        </is>
+      </c>
+      <c r="S33" t="inlineStr">
+        <is>
+          <t> </t>
+        </is>
+      </c>
+      <c r="T33" t="inlineStr">
+        <is>
+          <t> </t>
+        </is>
+      </c>
       <c r="U33" t="inlineStr">
         <is>
-          <t>NO</t>
-        </is>
-      </c>
-      <c r="V33" t="inlineStr"/>
-      <c r="W33" t="inlineStr"/>
+          <t> </t>
+        </is>
+      </c>
+      <c r="V33" t="inlineStr">
+        <is>
+          <t> </t>
+        </is>
+      </c>
+      <c r="W33" t="inlineStr">
+        <is>
+          <t> </t>
+        </is>
+      </c>
       <c r="X33" t="inlineStr">
         <is>
-          <t>NO</t>
-        </is>
-      </c>
-      <c r="Y33" t="inlineStr"/>
-      <c r="Z33" t="inlineStr"/>
-      <c r="AA33" t="n">
-        <v>0</v>
-      </c>
-      <c r="AB33" t="inlineStr"/>
-      <c r="AC33" t="inlineStr"/>
-      <c r="AD33" t="inlineStr"/>
-      <c r="AE33" t="inlineStr"/>
-      <c r="AF33" t="inlineStr"/>
-      <c r="AG33" t="inlineStr"/>
-      <c r="AH33" t="inlineStr"/>
-      <c r="AI33" t="inlineStr"/>
-      <c r="AJ33" t="inlineStr"/>
-      <c r="AK33" t="inlineStr"/>
-      <c r="AL33" t="inlineStr"/>
-      <c r="AM33" t="inlineStr"/>
+          <t> </t>
+        </is>
+      </c>
+      <c r="Y33" t="inlineStr">
+        <is>
+          <t> </t>
+        </is>
+      </c>
+      <c r="Z33" t="inlineStr">
+        <is>
+          <t> </t>
+        </is>
+      </c>
+      <c r="AA33" t="inlineStr">
+        <is>
+          <t> </t>
+        </is>
+      </c>
+      <c r="AB33" t="inlineStr">
+        <is>
+          <t> </t>
+        </is>
+      </c>
+      <c r="AC33" t="inlineStr">
+        <is>
+          <t> </t>
+        </is>
+      </c>
+      <c r="AD33" t="inlineStr">
+        <is>
+          <t> </t>
+        </is>
+      </c>
+      <c r="AE33" t="inlineStr">
+        <is>
+          <t> </t>
+        </is>
+      </c>
+      <c r="AF33" t="inlineStr">
+        <is>
+          <t> </t>
+        </is>
+      </c>
+      <c r="AG33" t="inlineStr">
+        <is>
+          <t> </t>
+        </is>
+      </c>
+      <c r="AH33" t="inlineStr">
+        <is>
+          <t> </t>
+        </is>
+      </c>
+      <c r="AI33" t="inlineStr">
+        <is>
+          <t> </t>
+        </is>
+      </c>
+      <c r="AJ33" t="inlineStr">
+        <is>
+          <t> </t>
+        </is>
+      </c>
+      <c r="AK33" t="inlineStr">
+        <is>
+          <t> </t>
+        </is>
+      </c>
+      <c r="AL33" t="inlineStr">
+        <is>
+          <t> </t>
+        </is>
+      </c>
+      <c r="AM33" t="inlineStr">
+        <is>
+          <t> </t>
+        </is>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>